<commit_message>
Gesamtinvestitionskosten Inputspalte B in JavaFx implementiert
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FBEC8A-291B-46EF-A125-BA15C3D06B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F85CF5-BEBE-4061-9492-E9527D04E7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" firstSheet="1" activeTab="1" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -435,12 +435,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -765,20 +765,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2300000</v>
+        <v>260</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -892,10 +892,10 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="19">
         <v>2000</v>
       </c>
       <c r="C12" t="s">
@@ -903,7 +903,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="19" t="s">
         <v>70</v>
       </c>
       <c r="C13" t="s">
@@ -923,14 +923,14 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
-    <col min="2" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.86328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="31.1328125" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -957,23 +957,23 @@
         <v>20</v>
       </c>
       <c r="B2" s="1">
-        <v>2530800</v>
-      </c>
-      <c r="C2" s="3">
+        <v>78</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>25000.001639999999</v>
-      </c>
-      <c r="D2" s="9">
+        <v>0.7705074</v>
+      </c>
+      <c r="D2" s="9" t="n">
         <f t="shared" ref="D2:D10" si="0">C2/B2</f>
-        <v>9.8782999999999996E-3</v>
-      </c>
-      <c r="E2" s="3">
+        <v>0.0098783</v>
+      </c>
+      <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="1">B2+C2</f>
-        <v>2555800.0016399999</v>
-      </c>
-      <c r="F2" s="2">
+        <v>78.7705074</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="2">$E2/$E$14</f>
-        <v>0.32968532157815789</v>
+        <v>1.0023149719219694E-4</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -982,23 +982,23 @@
         <v>21</v>
       </c>
       <c r="B3" s="1">
-        <v>85892</v>
-      </c>
-      <c r="C3" s="3">
+        <v>100</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="3">B3*$B$20</f>
-        <v>17178.400000000001</v>
-      </c>
-      <c r="D3" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="D3" s="6" t="n">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="n">
         <f t="shared" si="1"/>
-        <v>103070.39999999999</v>
-      </c>
-      <c r="F3" s="2">
+        <v>120.0</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <f t="shared" si="2"/>
-        <v>1.3295562229980688E-2</v>
+        <v>1.526939467583477E-4</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1007,23 +1007,23 @@
         <v>22</v>
       </c>
       <c r="B4" s="1">
-        <v>2475206</v>
-      </c>
-      <c r="C4" s="3">
-        <f t="shared" si="3"/>
-        <v>495041.2</v>
-      </c>
-      <c r="D4" s="6">
+        <v>700</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <f>B4*$B$20</f>
+        <v>140.0</v>
+      </c>
+      <c r="D4" s="6" t="n">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="n">
         <f t="shared" si="1"/>
-        <v>2970247.2</v>
-      </c>
-      <c r="F4" s="2">
+        <v>840.0</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f t="shared" si="2"/>
-        <v>0.38314692177410681</v>
+        <v>0.0010688576273084338</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1031,24 +1031,24 @@
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1">
-        <v>212558</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="1" t="n">
+        <v>789.0</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <f t="shared" si="3"/>
-        <v>42511.600000000006</v>
-      </c>
-      <c r="D5" s="6">
+        <v>157.8</v>
+      </c>
+      <c r="D5" s="6" t="n">
         <f t="shared" si="0"/>
-        <v>0.20000000000000004</v>
-      </c>
-      <c r="E5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="3" t="n">
         <f t="shared" si="1"/>
-        <v>255069.6</v>
-      </c>
-      <c r="F5" s="2">
+        <v>946.8</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <f t="shared" si="2"/>
-        <v>3.2902693108557667E-2</v>
+        <v>0.0012047552399233634</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1059,21 +1059,21 @@
       <c r="B6" s="1">
         <v>612366</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="n">
         <f t="shared" si="3"/>
         <v>122473.20000000001</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="6" t="n">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="n">
         <f t="shared" si="1"/>
         <v>734839.2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <f t="shared" si="2"/>
-        <v>9.4790553957578752E-2</v>
+        <v>0.9350458140062234</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1084,21 +1084,21 @@
       <c r="B7" s="1">
         <v>39881</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="3" t="n">
         <f t="shared" si="3"/>
-        <v>7976.2000000000007</v>
-      </c>
-      <c r="D7" s="6">
+        <v>7976.200000000001</v>
+      </c>
+      <c r="D7" s="6" t="n">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="n">
         <f t="shared" si="1"/>
         <v>47857.2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2" t="n">
         <f t="shared" si="2"/>
-        <v>6.1733376483707426E-3</v>
+        <v>0.060895872906696645</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1106,24 +1106,24 @@
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1">
-        <v>101581</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="1" t="n">
+        <v>323.0</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <f t="shared" si="3"/>
-        <v>20316.2</v>
-      </c>
-      <c r="D8" s="6">
+        <v>64.60000000000001</v>
+      </c>
+      <c r="D8" s="6" t="n">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="3">
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="E8" s="3" t="n">
         <f t="shared" si="1"/>
-        <v>121897.2</v>
-      </c>
-      <c r="F8" s="2">
+        <v>387.6</v>
+      </c>
+      <c r="F8" s="2" t="n">
         <f t="shared" si="2"/>
-        <v>1.5724124562050811E-2</v>
+        <v>4.932014480294631E-4</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1131,24 +1131,24 @@
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1">
-        <v>52000</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B9" s="1" t="n">
+        <v>666.0</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <f t="shared" si="3"/>
-        <v>10400</v>
-      </c>
-      <c r="D9" s="6">
+        <v>133.20000000000002</v>
+      </c>
+      <c r="D9" s="6" t="n">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="3">
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="E9" s="3" t="n">
         <f t="shared" si="1"/>
-        <v>62400</v>
-      </c>
-      <c r="F9" s="2">
+        <v>799.2</v>
+      </c>
+      <c r="F9" s="2" t="n">
         <f t="shared" si="2"/>
-        <v>8.049285567445115E-3</v>
+        <v>0.0010169416854105958</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1156,23 +1156,23 @@
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="10">
-        <v>901060</v>
+      <c r="B10" s="10" t="n">
+        <v>17.0</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="6" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E10" s="3" t="n">
         <f t="shared" si="1"/>
-        <v>901060</v>
-      </c>
-      <c r="F10" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f t="shared" si="2"/>
-        <v>0.11623219957375153</v>
+        <v>2.163164245743259E-5</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1189,25 +1189,25 @@
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>7011344</v>
-      </c>
-      <c r="C12" s="3">
+        <v>654920.0</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>740896.80163999996</v>
-      </c>
-      <c r="D12" s="4">
+        <v>130965.77050740001</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.10567115258358455</v>
-      </c>
-      <c r="E12" s="11">
+        <v>0.1999721653139315</v>
+      </c>
+      <c r="E12" s="11" t="n">
         <f>B12+C12</f>
-        <v>7752240.8016400002</v>
-      </c>
-      <c r="F12" s="4">
+        <v>785885.7705074</v>
+      </c>
+      <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>0.99999999999999989</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1226,25 +1226,25 @@
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>7011344</v>
-      </c>
-      <c r="C14" s="3">
+        <v>654920.0</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>740896.80163999996</v>
-      </c>
-      <c r="D14" s="3">
+        <v>130965.77050740001</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.10567115258358455</v>
-      </c>
-      <c r="E14" s="11">
+        <v>0.1999721653139315</v>
+      </c>
+      <c r="E14" s="11" t="n">
         <f>E12</f>
-        <v>7752240.8016400002</v>
-      </c>
-      <c r="F14" s="4">
+        <v>785885.7705074</v>
+      </c>
+      <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>0.99999999999999989</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1309,23 +1309,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1"/>
-    <col min="2" max="3" width="10.73046875" customWidth="1"/>
-    <col min="4" max="4" width="21.3984375" customWidth="1"/>
-    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.59765625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.3984375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
@@ -1334,9 +1334,9 @@
       <c r="B2" s="1">
         <v>6851180</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <f>$B2/$B$7</f>
-        <v>0.88376778840696368</v>
+        <v>0.999997518681772</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
@@ -1344,22 +1344,22 @@
       <c r="E2" s="1">
         <v>900000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f>$E2/$E$7</f>
-        <v>0.11609549189595419</v>
+        <v>0.1160954918959542</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="17" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>901060</v>
-      </c>
-      <c r="C3" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <f>$B3/$B$7</f>
-        <v>0.11623221159303633</v>
+        <v>2.481318228041027E-6</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>40</v>
@@ -1367,9 +1367,9 @@
       <c r="E3" s="1">
         <v>2450000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f>$E3/$E$7</f>
-        <v>0.31603772793898638</v>
+        <v>0.3160377279389864</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
@@ -1382,7 +1382,7 @@
       <c r="E4" s="1">
         <v>2250000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f>$E4/$E$7</f>
         <v>0.29023872973988546</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="E5" s="1">
         <v>2152239</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f>$E5/$E$7</f>
         <v>0.27762805042517397</v>
       </c>
@@ -1414,31 +1414,31 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <f>$E6/$E$7</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>7752240</v>
-      </c>
-      <c r="C7" s="4">
+        <v>6851197.0</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="11">
+      <c r="E7" s="11" t="n">
         <f>SUM(E2:E6)</f>
-        <v>7752239</v>
-      </c>
-      <c r="F7" s="4">
+        <v>7752239.0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f>SUM(F2:F6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1460,11 +1460,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.86328125" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" customWidth="1"/>
-    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="42.86328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.1328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.86328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -1570,25 +1570,25 @@
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="7" t="n">
         <f>SUM(B3:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f>SUM(C3:C5)</f>
-        <v>959</v>
+        <v>959.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="n">
         <f>F4</f>
-        <v>9587290</v>
-      </c>
-      <c r="G6" s="15">
+        <v>9587290.0</v>
+      </c>
+      <c r="G6" s="15" t="n">
         <f>F6</f>
-        <v>9587290</v>
+        <v>9587290.0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1678,9 +1678,9 @@
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="16" t="n">
         <f>SUM(B10:B11)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -1689,13 +1689,13 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="n">
         <f>F10</f>
-        <v>672000</v>
-      </c>
-      <c r="G12" s="15">
+        <v>672000.0</v>
+      </c>
+      <c r="G12" s="15" t="n">
         <f>F12</f>
-        <v>672000</v>
+        <v>672000.0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1735,11 +1735,11 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="1" t="s">
         <v>57</v>
       </c>
@@ -1764,9 +1764,9 @@
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="n">
         <f>$E17/$E$19</f>
-        <v>0.93449839121420686</v>
+        <v>0.9344983912142069</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -1786,9 +1786,9 @@
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="n">
         <f>$E18/$E$19</f>
-        <v>6.5501608785793169E-2</v>
+        <v>0.06550160878579317</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -1803,9 +1803,9 @@
         <v>44</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="n">
         <f>SUM(E17:E18)</f>
-        <v>10259290</v>
+        <v>1.025929E7</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1819,9 +1819,9 @@
         <v>61</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="10">
+      <c r="E20" s="10" t="n">
         <f>'Mittelverwendung - Mittelherkun'!E7</f>
-        <v>7752239</v>
+        <v>7752239.0</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1835,9 +1835,9 @@
         <v>62</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="n">
         <f>E19-E20</f>
-        <v>2507051</v>
+        <v>2507051.0</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1851,9 +1851,9 @@
         <v>63</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2">
+      <c r="E22" s="2" t="n">
         <f>E21/E20</f>
-        <v>0.32339702117027092</v>
+        <v>0.3233970211702709</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1935,6 +1935,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -2098,24 +2115,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2131,22 +2149,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Diese To Do's wurden erledigt:
Weitere TO Do's für GIK:
-Inputvalisierung:
Nur numerische Variablen sollten erlaubt sein;
Bei dem Input soll 0,7 in 0.7 konvertiert werden.
70% ebenfalls 0.7. Momentan funktioniert nur die Schreibweise 0.7
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EA562D-C3D0-47F0-8337-31B715E84CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32369BE-6D64-4210-8D3D-CE03D1493425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
@@ -759,7 +759,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -923,7 +923,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -957,11 +957,11 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>0.1</v>
+        <v>1.0</v>
       </c>
       <c r="D2" s="19" t="n">
         <f>C2/B2</f>
@@ -969,11 +969,11 @@
       </c>
       <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>1.1</v>
+        <v>11.0</v>
       </c>
       <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>2.2417457901033038E-5</v>
+        <v>1.777993292116216E-4</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -982,23 +982,23 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2.0</v>
+        <v>20.0</v>
       </c>
       <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>0.4</v>
+        <v>10.0</v>
       </c>
       <c r="D3" s="6" t="n">
-        <f t="shared" ref="D3:D10" si="3">C3/B3</f>
-        <v>0.2</v>
+        <f t="shared" ref="D3:D9" si="3">C3/B3</f>
+        <v>0.5</v>
       </c>
       <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>2.4</v>
+        <v>30.0</v>
       </c>
       <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>4.8910817238617536E-5</v>
+        <v>4.849072614862408E-4</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1007,23 +1007,23 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
-        <v>0.6000000000000001</v>
+        <v>4.0</v>
       </c>
       <c r="D4" s="6" t="n">
         <f>C4/B4</f>
-        <v>0.20000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>3.6</v>
+        <v>12.0</v>
       </c>
       <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>7.33662258579263E-5</v>
+        <v>1.939629045944963E-4</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1032,23 +1032,23 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="C5" s="3" t="n">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
+        <f>B5*$B$20</f>
+        <v>5.0</v>
       </c>
       <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>4.8</v>
+        <v>15.0</v>
       </c>
       <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>9.782163447723507E-5</v>
+        <v>2.424536307431204E-4</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1056,24 +1056,24 @@
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>5.0</v>
+      <c r="B6" s="1">
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>1.0</v>
+        <v>2.5</v>
       </c>
       <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>6.0</v>
+        <v>7.5</v>
       </c>
       <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.2227704309654384E-4</v>
+        <v>1.212268153715602E-4</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1086,19 +1086,19 @@
       </c>
       <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>7976.200000000001</v>
+        <v>19940.5</v>
       </c>
       <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>47857.2</v>
+        <v>59821.5</v>
       </c>
       <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.9753061511466529</v>
+        <v>0.9669293247666384</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1106,24 +1106,24 @@
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1">
-        <v>323</v>
+      <c r="B8" s="1" t="n">
+        <v>643.0</v>
       </c>
       <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>64.60000000000001</v>
+        <v>321.5</v>
       </c>
       <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.20000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>387.6</v>
+        <v>964.5</v>
       </c>
       <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.007899096984036732</v>
+        <v>0.01558976845678264</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1136,19 +1136,19 @@
       </c>
       <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>133.20000000000002</v>
+        <v>333.0</v>
       </c>
       <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.20000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>799.2</v>
+        <v>999.0</v>
       </c>
       <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.01628730214045964</v>
+        <v>0.016147411807491817</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1156,14 +1156,14 @@
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9" t="n">
-        <v>7.0</v>
+      <c r="B10" s="9">
+        <v>7</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.4265655027930114E-4</v>
+        <v>1.1314502768012284E-4</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1190,23 +1190,23 @@
       </c>
       <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>40892.0</v>
+        <v>41250.0</v>
       </c>
       <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>8176.900000000001</v>
+        <v>20617.5</v>
       </c>
       <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.1999633180084124</v>
+        <v>0.49981818181818183</v>
       </c>
       <c r="E12" s="10" t="n">
         <f>B12+C12</f>
-        <v>49068.9</v>
+        <v>61867.5</v>
       </c>
       <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1227,23 +1227,23 @@
       </c>
       <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>40892.0</v>
+        <v>41250.0</v>
       </c>
       <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>8176.900000000001</v>
+        <v>20617.5</v>
       </c>
       <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.1999633180084124</v>
+        <v>0.49981818181818183</v>
       </c>
       <c r="E14" s="10" t="n">
         <f>E12</f>
-        <v>49068.9</v>
+        <v>61867.5</v>
       </c>
       <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1279,7 +1279,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1454,7 +1454,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1934,6 +1934,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -2097,24 +2114,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2130,22 +2148,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Weiter Button, welcher neues JavaFX Fenster öffnet hinzugfügt ExcelToWordKonverter eingebaut WordDokument wird generiert, welches ExcelDaten von GIK enthält
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32369BE-6D64-4210-8D3D-CE03D1493425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F144117D-E1E8-42A2-88F8-ED4FC1F7D398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" firstSheet="1" activeTab="1" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -923,7 +923,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -957,23 +957,23 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>1.0</v>
+        <v>0.11</v>
       </c>
       <c r="D2" s="19" t="n">
         <f>C2/B2</f>
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>11.0</v>
+        <v>1.11</v>
       </c>
       <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>1.777993292116216E-4</v>
+        <v>0.022510646927600894</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -982,23 +982,23 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>10.0</v>
+        <v>0.24</v>
       </c>
       <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
       <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>30.0</v>
+        <v>2.24</v>
       </c>
       <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>4.849072614862408E-4</v>
+        <v>0.04542689109714054</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1007,23 +1007,23 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
-        <v>4.0</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="6" t="n">
         <f>C4/B4</f>
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
       <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>12.0</v>
+        <v>3.36</v>
       </c>
       <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.939629045944963E-4</v>
+        <v>0.0681403366457108</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1032,23 +1032,23 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" s="3" t="n">
         <f>B5*$B$20</f>
-        <v>5.0</v>
+        <v>0.48</v>
       </c>
       <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
       <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>15.0</v>
+        <v>4.48</v>
       </c>
       <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>2.424536307431204E-4</v>
+        <v>0.09085378219428109</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1056,24 +1056,24 @@
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1">
-        <v>5</v>
+      <c r="B6" s="1" t="n">
+        <v>5.0</v>
       </c>
       <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>0.6</v>
       </c>
       <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
       <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>5.6</v>
       </c>
       <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.212268153715602E-4</v>
+        <v>0.11356722774285134</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1081,24 +1081,24 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
-        <v>39881</v>
+      <c r="B7" s="1" t="n">
+        <v>6.0</v>
       </c>
       <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>19940.5</v>
+        <v>0.72</v>
       </c>
       <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
       <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>59821.5</v>
+        <v>6.72</v>
       </c>
       <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.9669293247666384</v>
+        <v>0.1362806732914216</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1107,23 +1107,23 @@
         <v>26</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>643.0</v>
+        <v>7.0</v>
       </c>
       <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>321.5</v>
+        <v>0.84</v>
       </c>
       <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
       <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>964.5</v>
+        <v>7.84</v>
       </c>
       <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.01558976845678264</v>
+        <v>0.15899411883999187</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1131,24 +1131,24 @@
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1">
-        <v>666</v>
+      <c r="B9" s="1" t="n">
+        <v>8.0</v>
       </c>
       <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>333.0</v>
+        <v>0.96</v>
       </c>
       <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
       <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>999.0</v>
+        <v>8.96</v>
       </c>
       <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.016147411807491817</v>
+        <v>0.18170756438856217</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1156,22 +1156,22 @@
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9">
-        <v>7</v>
+      <c r="B10" s="9" t="n">
+        <v>9.0</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>0.7</v>
+        <v>0.13</v>
       </c>
       <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.1314502768012284E-4</v>
+        <v>0.18251875887243965</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1190,23 +1190,23 @@
       </c>
       <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>41250.0</v>
+        <v>45.0</v>
       </c>
       <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>20617.5</v>
+        <v>4.31</v>
       </c>
       <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.49981818181818183</v>
+        <v>0.09577777777777777</v>
       </c>
       <c r="E12" s="10" t="n">
         <f>B12+C12</f>
-        <v>61867.5</v>
+        <v>49.31</v>
       </c>
       <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1227,23 +1227,23 @@
       </c>
       <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>41250.0</v>
+        <v>45.0</v>
       </c>
       <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>20617.5</v>
+        <v>4.31</v>
       </c>
       <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.49981818181818183</v>
+        <v>0.09577777777777777</v>
       </c>
       <c r="E14" s="10" t="n">
         <f>E12</f>
-        <v>61867.5</v>
+        <v>49.31</v>
       </c>
       <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1279,7 +1279,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1287,7 +1287,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="12" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="C2" s="2" t="n">
         <f>$B2/$B$7</f>
-        <v>0.9999989782792383</v>
+        <v>0.9999986863594041</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
@@ -1354,11 +1354,11 @@
       </c>
       <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="C3" s="2" t="n">
         <f>$B3/$B$7</f>
-        <v>1.0217207616723933E-6</v>
+        <v>1.3136405958148285E-6</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>40</v>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>6851187.0</v>
+        <v>6851189.0</v>
       </c>
       <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
@@ -1934,23 +1934,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -2114,25 +2097,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2148,4 +2130,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Hello Application kopiert und in GIKtoExcel und IAllRegistercars aufgeteilt um objektorientierte Struktur aufzuteilen -Bessere if-else Struktur, um Redundanzen zu vermeiden -ExceltoWord-Klasse so geändert, dass es im Querformat erstellt wird und auf 2 Nachkommastellen nur gerundet wird
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -957,23 +957,23 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1.0</v>
+        <v>110.0</v>
       </c>
       <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>0.11</v>
+        <v>36.300000000000004</v>
       </c>
       <c r="D2" s="19" t="n">
         <f>C2/B2</f>
-        <v>0.11</v>
+        <v>0.33</v>
       </c>
       <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>1.11</v>
+        <v>146.3</v>
       </c>
       <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>0.022510646927600894</v>
+        <v>0.033391915641476276</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -982,23 +982,23 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2.0</v>
+        <v>1100.0</v>
       </c>
       <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>0.24</v>
+        <v>550.0</v>
       </c>
       <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>2.24</v>
+        <v>1650.0</v>
       </c>
       <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.04542689109714054</v>
+        <v>0.37660055234747675</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1007,23 +1007,23 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>3.0</v>
+        <v>1100.0</v>
       </c>
       <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
-        <v>0.36</v>
+        <v>550.0</v>
       </c>
       <c r="D4" s="6" t="n">
         <f>C4/B4</f>
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>3.36</v>
+        <v>1650.0</v>
       </c>
       <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.0681403366457108</v>
+        <v>0.37660055234747675</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1032,23 +1032,23 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>4.0</v>
+        <v>110.0</v>
       </c>
       <c r="C5" s="3" t="n">
         <f>B5*$B$20</f>
-        <v>0.48</v>
+        <v>55.0</v>
       </c>
       <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>4.48</v>
+        <v>165.0</v>
       </c>
       <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.09085378219428109</v>
+        <v>0.03766005523474768</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1057,23 +1057,23 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>5.0</v>
+        <v>110.0</v>
       </c>
       <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>55.0</v>
       </c>
       <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>5.6</v>
+        <v>165.0</v>
       </c>
       <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.11356722774285134</v>
+        <v>0.03766005523474768</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1082,23 +1082,23 @@
         <v>25</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>6.0</v>
+        <v>110.0</v>
       </c>
       <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>0.72</v>
+        <v>55.0</v>
       </c>
       <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>6.72</v>
+        <v>165.0</v>
       </c>
       <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.1362806732914216</v>
+        <v>0.03766005523474768</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1107,23 +1107,23 @@
         <v>26</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>7.0</v>
+        <v>110.0</v>
       </c>
       <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>0.84</v>
+        <v>55.0</v>
       </c>
       <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>7.84</v>
+        <v>165.0</v>
       </c>
       <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.15899411883999187</v>
+        <v>0.03766005523474768</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1132,23 +1132,23 @@
         <v>27</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>8.0</v>
+        <v>110.0</v>
       </c>
       <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>0.96</v>
+        <v>55.0</v>
       </c>
       <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>8.96</v>
+        <v>165.0</v>
       </c>
       <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.18170756438856217</v>
+        <v>0.03766005523474768</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1157,21 +1157,21 @@
         <v>28</v>
       </c>
       <c r="B10" s="9" t="n">
-        <v>9.0</v>
+        <v>110.0</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>0.13</v>
+        <v>0.6</v>
       </c>
       <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>9.0</v>
+        <v>110.0</v>
       </c>
       <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.18251875887243965</v>
+        <v>0.025106703489831784</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1190,23 +1190,23 @@
       </c>
       <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>45.0</v>
+        <v>2970.0</v>
       </c>
       <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>4.31</v>
+        <v>1411.3</v>
       </c>
       <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.09577777777777777</v>
+        <v>0.47518518518518515</v>
       </c>
       <c r="E12" s="10" t="n">
         <f>B12+C12</f>
-        <v>49.31</v>
+        <v>4381.3</v>
       </c>
       <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1227,23 +1227,23 @@
       </c>
       <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>45.0</v>
+        <v>2970.0</v>
       </c>
       <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>4.31</v>
+        <v>1411.3</v>
       </c>
       <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.09577777777777777</v>
+        <v>0.47518518518518515</v>
       </c>
       <c r="E14" s="10" t="n">
         <f>E12</f>
-        <v>49.31</v>
+        <v>4381.3</v>
       </c>
       <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1279,7 +1279,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1287,7 +1287,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="12" t="n">
-        <v>0.11</v>
+        <v>0.33</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="C2" s="2" t="n">
         <f>$B2/$B$7</f>
-        <v>0.9999986863594041</v>
+        <v>0.9999839446294055</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
@@ -1354,11 +1354,11 @@
       </c>
       <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>9.0</v>
+        <v>110.0</v>
       </c>
       <c r="C3" s="2" t="n">
         <f>$B3/$B$7</f>
-        <v>1.3136405958148285E-6</v>
+        <v>1.60553705944428E-5</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>40</v>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>6851189.0</v>
+        <v>6851290.0</v>
       </c>
       <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>

</xml_diff>

<commit_message>
Update-Klasse erstellt und Updatefunktion reingetan, sodass sie von allen verwendet werden kann
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -957,23 +957,23 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>110.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>36.300000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="D2" s="19" t="n">
         <f>C2/B2</f>
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>146.3</v>
+        <v>1.1</v>
       </c>
       <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>0.033391915641476276</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -982,23 +982,23 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1100.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>550.0</v>
+        <v>0.22</v>
       </c>
       <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>1650.0</v>
+        <v>2.22</v>
       </c>
       <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.37660055234747675</v>
+        <v>0.045352400408580185</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1007,23 +1007,23 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>1100.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
-        <v>550.0</v>
+        <v>0.33</v>
       </c>
       <c r="D4" s="6" t="n">
         <f>C4/B4</f>
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>1650.0</v>
+        <v>3.33</v>
       </c>
       <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.37660055234747675</v>
+        <v>0.06802860061287028</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1032,23 +1032,23 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>110.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" s="3" t="n">
         <f>B5*$B$20</f>
-        <v>55.0</v>
+        <v>0.44</v>
       </c>
       <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>165.0</v>
+        <v>4.44</v>
       </c>
       <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.03766005523474768</v>
+        <v>0.09070480081716037</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1057,23 +1057,23 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>110.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>55.0</v>
+        <v>0.55</v>
       </c>
       <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.11000000000000001</v>
       </c>
       <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>165.0</v>
+        <v>5.55</v>
       </c>
       <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.03766005523474768</v>
+        <v>0.11338100102145045</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1082,23 +1082,23 @@
         <v>25</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>110.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>55.0</v>
+        <v>0.66</v>
       </c>
       <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>165.0</v>
+        <v>6.66</v>
       </c>
       <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.03766005523474768</v>
+        <v>0.13605720122574055</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1107,23 +1107,23 @@
         <v>26</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>110.0</v>
+        <v>7.0</v>
       </c>
       <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>55.0</v>
+        <v>0.77</v>
       </c>
       <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>165.0</v>
+        <v>7.77</v>
       </c>
       <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.03766005523474768</v>
+        <v>0.15873340143003062</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1132,23 +1132,23 @@
         <v>27</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>110.0</v>
+        <v>8.0</v>
       </c>
       <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>55.0</v>
+        <v>0.88</v>
       </c>
       <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>165.0</v>
+        <v>8.88</v>
       </c>
       <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.03766005523474768</v>
+        <v>0.18140960163432074</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1157,21 +1157,21 @@
         <v>28</v>
       </c>
       <c r="B10" s="9" t="n">
-        <v>110.0</v>
+        <v>9.0</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>0.6</v>
+        <v>0.12</v>
       </c>
       <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>110.0</v>
+        <v>9.0</v>
       </c>
       <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.025106703489831784</v>
+        <v>0.18386108273748722</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1190,19 +1190,19 @@
       </c>
       <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>2970.0</v>
+        <v>45.0</v>
       </c>
       <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>1411.3</v>
+        <v>3.95</v>
       </c>
       <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.47518518518518515</v>
+        <v>0.08777777777777779</v>
       </c>
       <c r="E12" s="10" t="n">
         <f>B12+C12</f>
-        <v>4381.3</v>
+        <v>48.95</v>
       </c>
       <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
@@ -1227,19 +1227,19 @@
       </c>
       <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>2970.0</v>
+        <v>45.0</v>
       </c>
       <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>1411.3</v>
+        <v>3.95</v>
       </c>
       <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.47518518518518515</v>
+        <v>0.08777777777777779</v>
       </c>
       <c r="E14" s="10" t="n">
         <f>E12</f>
-        <v>4381.3</v>
+        <v>48.95</v>
       </c>
       <c r="F14" s="4" t="n">
         <f>F12</f>
@@ -1279,7 +1279,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1287,7 +1287,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="12" t="n">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="C2" s="2" t="n">
         <f>$B2/$B$7</f>
-        <v>0.9999839446294055</v>
+        <v>0.9999986863594041</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
@@ -1354,11 +1354,11 @@
       </c>
       <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>110.0</v>
+        <v>9.0</v>
       </c>
       <c r="C3" s="2" t="n">
         <f>$B3/$B$7</f>
-        <v>1.60553705944428E-5</v>
+        <v>1.3136405958148285E-6</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>40</v>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>6851290.0</v>
+        <v>6851189.0</v>
       </c>
       <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>

</xml_diff>

<commit_message>
Basisinformationen und Stammblatt Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43677\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EA562D-C3D0-47F0-8337-31B715E84CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B420DA-F855-42C6-AFBD-EB872398AEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
-  <si>
-    <t>Basisinfomrationen</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -78,15 +75,9 @@
     <t>Ziel-Baubeginn</t>
   </si>
   <si>
-    <t>Q4/ 2023</t>
-  </si>
-  <si>
     <t>Ziel-Fertigstellung</t>
   </si>
   <si>
-    <t>Q4/ 2025</t>
-  </si>
-  <si>
     <t>netto</t>
   </si>
   <si>
@@ -246,13 +237,61 @@
     <t>Flächenwidmung -Was ist das, wuie funktioniert das?</t>
   </si>
   <si>
-    <t>Quadratmeterpreis</t>
-  </si>
-  <si>
-    <t>Userinput</t>
-  </si>
-  <si>
-    <t>Zinslast</t>
+    <t>Stammdaten</t>
+  </si>
+  <si>
+    <t>Firmenname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strasse </t>
+  </si>
+  <si>
+    <t>Postleitzahl</t>
+  </si>
+  <si>
+    <t>Ort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entfernung zur Schule </t>
+  </si>
+  <si>
+    <t>Lagebeschreibung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maps - Bild </t>
+  </si>
+  <si>
+    <t>Lage der Öffi Anbindung</t>
+  </si>
+  <si>
+    <t>oihjubjpkojk</t>
+  </si>
+  <si>
+    <t>ghetto wien</t>
+  </si>
+  <si>
+    <t>Apfelcompany</t>
+  </si>
+  <si>
+    <t>Siehdichvorstrasse 12</t>
+  </si>
+  <si>
+    <t>2231</t>
+  </si>
+  <si>
+    <t>Strasshof</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>nix</t>
+  </si>
+  <si>
+    <t>m²</t>
+  </si>
+  <si>
+    <t>Basisinformationen</t>
   </si>
 </sst>
 </file>
@@ -263,7 +302,7 @@
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,8 +333,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +388,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -404,7 +464,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -413,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -434,8 +496,18 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -443,8 +515,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,7 +532,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -756,163 +828,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.54296875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.26953125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.54296875" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>260</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>797</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19" t="str">
+        <f>+C3</f>
+        <v>m²</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>800</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>7752000</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>10260000</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
-        <v>2500000</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0.32340000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="18">
-        <v>2000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -922,260 +1076,262 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57066AFC-3CC1-4339-B554-0D5829A53635}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.1328125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.86328125" collapsed="true"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="3" t="n">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
         <f>B2*B21</f>
         <v>0.1</v>
       </c>
-      <c r="D2" s="19" t="n">
+      <c r="D2" s="18">
         <f>C2/B2</f>
         <v>0.1</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="3">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>1.1</v>
-      </c>
-      <c r="F2" s="2" t="n">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F2" s="2">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
         <v>2.2417457901033038E-5</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C3" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
         <v>0.4</v>
       </c>
-      <c r="D3" s="6" t="n">
-        <f t="shared" ref="D3:D10" si="3">C3/B3</f>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:D9" si="3">C3/B3</f>
         <v>0.2</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="3">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <f t="shared" si="1"/>
         <v>4.8910817238617536E-5</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C4" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
         <f>B4*$B$20</f>
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="D4" s="6" t="n">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="D4" s="6">
         <f>C4/B4</f>
         <v>0.20000000000000004</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <f t="shared" si="1"/>
-        <v>7.33662258579263E-5</v>
+        <v>7.3366225857926303E-5</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
         <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="6">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>9.782163447723507E-5</v>
+        <v>9.7821634477235071E-5</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="C6" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
         <f t="shared" si="2"/>
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>6.0</v>
-      </c>
-      <c r="F6" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
         <v>1.2227704309654384E-4</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>39881</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="3">
         <f t="shared" si="2"/>
-        <v>7976.200000000001</v>
-      </c>
-      <c r="D7" s="6" t="n">
+        <v>7976.2000000000007</v>
+      </c>
+      <c r="D7" s="6">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>47857.2</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>0.9753061511466529</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>0.97530615114665287</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
         <v>323</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="3">
         <f t="shared" si="2"/>
-        <v>64.60000000000001</v>
-      </c>
-      <c r="D8" s="6" t="n">
+        <v>64.600000000000009</v>
+      </c>
+      <c r="D8" s="6">
         <f t="shared" si="3"/>
         <v>0.20000000000000004</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>387.6</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>0.007899096984036732</v>
+        <v>7.8990969840367319E-3</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>666</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="3">
         <f t="shared" si="2"/>
         <v>133.20000000000002</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="6">
         <f t="shared" si="3"/>
         <v>0.20000000000000004</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>799.2</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>0.01628730214045964</v>
+        <v>1.628730214045964E-2</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="9" t="n">
-        <v>7.0</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="9">
+        <v>7</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="6">
         <v>0.3</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>7.0</v>
-      </c>
-      <c r="F10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>1.4265655027930114E-4</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1184,35 +1340,35 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3">
         <f>SUM(B2:B10)</f>
-        <v>40892.0</v>
-      </c>
-      <c r="C12" s="3" t="n">
+        <v>40892</v>
+      </c>
+      <c r="C12" s="3">
         <f>SUM(C2:C10)</f>
-        <v>8176.900000000001</v>
-      </c>
-      <c r="D12" s="4" t="n">
+        <v>8176.9000000000005</v>
+      </c>
+      <c r="D12" s="4">
         <f>C12/B12</f>
-        <v>0.1999633180084124</v>
-      </c>
-      <c r="E12" s="10" t="n">
+        <v>0.19996331800841241</v>
+      </c>
+      <c r="E12" s="10">
         <f>B12+C12</f>
         <v>49068.9</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4">
         <f>SUM(F2:F10)</f>
-        <v>0.9999999999999999</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1221,33 +1377,33 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3">
         <f>B12</f>
-        <v>40892.0</v>
-      </c>
-      <c r="C14" s="3" t="n">
+        <v>40892</v>
+      </c>
+      <c r="C14" s="3">
         <f>C12</f>
-        <v>8176.900000000001</v>
-      </c>
-      <c r="D14" s="3" t="n">
+        <v>8176.9000000000005</v>
+      </c>
+      <c r="D14" s="3">
         <f>D12</f>
-        <v>0.1999633180084124</v>
-      </c>
-      <c r="E14" s="10" t="n">
+        <v>0.19996331800841241</v>
+      </c>
+      <c r="E14" s="10">
         <f>E12</f>
         <v>49068.9</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4">
         <f>F12</f>
-        <v>0.9999999999999999</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1256,7 +1412,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1265,7 +1421,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1274,23 +1430,23 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="11" t="n">
+        <v>29</v>
+      </c>
+      <c r="B20" s="11">
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="12" t="n">
+        <v>30</v>
+      </c>
+      <c r="B21" s="12">
         <v>0.1</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1306,138 +1462,138 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="10.73046875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.3984375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="1" max="1" width="21.6328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="10.7265625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.36328125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1">
         <v>6851180</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <f>$B2/$B$7</f>
-        <v>0.9999989782792383</v>
+        <v>0.99999897827923834</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1">
         <v>900000</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <f>$E2/$E$7</f>
-        <v>0.1160954918959542</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>0.11609549189595419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="16" t="n">
+        <v>36</v>
+      </c>
+      <c r="B3" s="16">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>7.0</v>
-      </c>
-      <c r="C3" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
         <f>$B3/$B$7</f>
         <v>1.0217207616723933E-6</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1">
         <v>2450000</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <f>$E3/$E$7</f>
-        <v>0.3160377279389864</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>0.31603772793898638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
       <c r="D4" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1">
         <v>2250000</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <f>$E4/$E$7</f>
         <v>0.29023872973988546</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1">
         <v>2152239</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <f>$E5/$E$7</f>
         <v>0.27762805042517397</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="2">
         <f>$E6/$E$7</f>
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3">
         <f>SUM(B2:B6)</f>
-        <v>6851187.0</v>
-      </c>
-      <c r="C7" s="4" t="n">
+        <v>6851187</v>
+      </c>
+      <c r="C7" s="4">
         <f>SUM(C2:C6)</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10" t="n">
+      <c r="E7" s="10">
         <f>SUM(E2:E6)</f>
-        <v>7752239.0</v>
-      </c>
-      <c r="F7" s="4" t="n">
+        <v>7752239</v>
+      </c>
+      <c r="F7" s="4">
         <f>SUM(F2:F6)</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1457,41 +1613,41 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.86328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.1328125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.86328125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.1328125" collapsed="true"/>
+    <col min="1" max="1" width="42.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1506,9 +1662,9 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1525,9 +1681,9 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="15">
         <v>1</v>
@@ -1536,7 +1692,7 @@
         <v>959</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
@@ -1546,9 +1702,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -1557,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1565,34 +1721,34 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="7" t="n">
+        <v>41</v>
+      </c>
+      <c r="B6" s="7">
         <f>SUM(B3:B5)</f>
-        <v>1.0</v>
-      </c>
-      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <f>SUM(C3:C5)</f>
-        <v>959.0</v>
+        <v>959</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="1">
         <f>F4</f>
-        <v>9587290.0</v>
-      </c>
-      <c r="G6" s="14" t="n">
+        <v>9587290</v>
+      </c>
+      <c r="G6" s="14">
         <f>F6</f>
-        <v>9587290.0</v>
+        <v>9587290</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1603,9 +1759,9 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1616,9 +1772,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1635,9 +1791,9 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
@@ -1654,9 +1810,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
@@ -1673,13 +1829,13 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="15" t="n">
+        <v>41</v>
+      </c>
+      <c r="B12" s="15">
         <f>SUM(B10:B11)</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -1688,18 +1844,18 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="1">
         <f>F10</f>
-        <v>672000.0</v>
-      </c>
-      <c r="G12" s="14" t="n">
+        <v>672000</v>
+      </c>
+      <c r="G12" s="14">
         <f>F12</f>
-        <v>672000.0</v>
+        <v>672000</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1710,7 +1866,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1721,7 +1877,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1732,40 +1888,40 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="2">
         <f>$E17/$E$19</f>
-        <v>0.9344983912142069</v>
+        <v>0.93449839121420686</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -1773,21 +1929,21 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="2">
         <f>$E18/$E$19</f>
-        <v>0.06550160878579317</v>
+        <v>6.5501608785793169E-2</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -1795,71 +1951,71 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="3">
         <f>SUM(E17:E18)</f>
-        <v>1.025929E7</v>
+        <v>10259290</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="9" t="n">
+      <c r="E20" s="9">
         <f>'Mittelverwendung - Mittelherkun'!E7</f>
-        <v>7752239.0</v>
+        <v>7752239</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="3">
         <f>E19-E20</f>
-        <v>2507051.0</v>
+        <v>2507051</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="2">
         <f>E21/E20</f>
-        <v>0.3233970211702709</v>
+        <v>0.32339702117027092</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1870,7 +2026,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1881,7 +2037,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1906,26 +2062,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1934,6 +2090,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -2097,15 +2262,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2115,6 +2271,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2132,14 +2296,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Weiter-Klasse hinzugefügt und Weiterbutton hinzugefügt, welche eine Klasse schließt und die nächste öffnet.
Außerdem habe ich eine Mainapplication hinzugefügt, aber ich weiß nicht, ob das relevant ist und notwendig.

Außerdem habe ich das ScrollPane bei Basisinformation korrigiert (minHeight war auf 1000, ich habe es jetzt auf -Infinity gesetzt.
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43677\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B420DA-F855-42C6-AFBD-EB872398AEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA8B656-E595-4850-AC20-43C30C4ADBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -515,8 +515,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,7 +532,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -830,18 +830,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.54296875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.26953125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.54296875" collapsed="true"/>
+    <col min="1" max="1" width="29.53125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.265625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.53125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="25" t="s">
         <v>83</v>
       </c>
@@ -859,7 +859,7 @@
       <c r="K1" s="26"/>
       <c r="L1" s="27"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -879,7 +879,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -901,7 +901,7 @@
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
@@ -924,7 +924,7 @@
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -944,7 +944,7 @@
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
@@ -964,7 +964,7 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
@@ -1022,7 +1022,7 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -1038,7 +1038,7 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
@@ -1077,17 +1077,17 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.08984375" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.81640625" collapsed="true"/>
+    <col min="1" max="1" width="31.06640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
         <v>12</v>
@@ -1106,214 +1106,214 @@
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="C2" s="3" t="n">
+      <c r="B2" s="1">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3">
         <f>B2*B21</f>
-        <v>1.1</v>
-      </c>
-      <c r="D2" s="18" t="n">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2" s="18">
         <f>C2/B2</f>
         <v>0.1</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="3">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
         <v>12.1</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>0.02111324376199616</v>
+        <v>2.1113243761996161E-2</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="C3" s="3" t="n">
+      <c r="B3" s="1">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>4.4</v>
-      </c>
-      <c r="D3" s="6" t="n">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D3" s="6">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
         <v>0.2</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="3">
         <f t="shared" si="0"/>
         <v>26.4</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <f t="shared" si="1"/>
-        <v>0.04606525911708253</v>
+        <v>4.6065259117082528E-2</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="C4" s="3" t="n">
+      <c r="B4" s="1">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3">
         <f>B4*$B$20</f>
         <v>6.6000000000000005</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="6">
         <f>C4/B4</f>
         <v>0.2</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <f t="shared" si="1"/>
-        <v>0.0690978886756238</v>
+        <v>6.9097888675623803E-2</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="C5" s="3" t="n">
+      <c r="B5" s="1">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3">
         <f t="shared" si="2"/>
-        <v>8.8</v>
-      </c>
-      <c r="D5" s="6" t="n">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D5" s="6">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>52.8</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>0.09213051823416506</v>
+        <v>9.2130518234165057E-2</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="C6" s="3" t="n">
+      <c r="B6" s="1">
+        <v>55</v>
+      </c>
+      <c r="C6" s="3">
         <f t="shared" si="2"/>
-        <v>11.0</v>
-      </c>
-      <c r="D6" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>66.0</v>
-      </c>
-      <c r="F6" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
         <v>0.11516314779270632</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="C7" s="3" t="n">
+      <c r="B7" s="1">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3">
         <f t="shared" si="2"/>
         <v>13.200000000000001</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="6">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>79.2</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>0.1381957773512476</v>
+        <v>0.13819577735124761</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>77.0</v>
-      </c>
-      <c r="C8" s="3" t="n">
+      <c r="B8" s="1">
+        <v>77</v>
+      </c>
+      <c r="C8" s="3">
         <f t="shared" si="2"/>
         <v>15.4</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="6">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>92.4</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>0.16122840690978887</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>88.0</v>
-      </c>
-      <c r="C9" s="3" t="n">
+      <c r="B9" s="1">
+        <v>88</v>
+      </c>
+      <c r="C9" s="3">
         <f t="shared" si="2"/>
-        <v>17.6</v>
-      </c>
-      <c r="D9" s="6" t="n">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D9" s="6">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>105.6</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>0.1842610364683301</v>
+        <v>0.18426103646833011</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="9" t="n">
-        <v>99.0</v>
+      <c r="B10" s="9">
+        <v>99</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -1321,17 +1321,17 @@
       <c r="D10" s="6">
         <v>0.3</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>99.0</v>
-      </c>
-      <c r="F10" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>0.1727447216890595</v>
+        <v>0.17274472168905949</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1340,33 +1340,33 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="3">
         <f>SUM(B2:B10)</f>
-        <v>495.0</v>
-      </c>
-      <c r="C12" s="3" t="n">
+        <v>495</v>
+      </c>
+      <c r="C12" s="3">
         <f>SUM(C2:C10)</f>
-        <v>78.1</v>
-      </c>
-      <c r="D12" s="4" t="n">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="D12" s="4">
         <f>C12/B12</f>
         <v>0.15777777777777777</v>
       </c>
-      <c r="E12" s="10" t="n">
+      <c r="E12" s="10">
         <f>B12+C12</f>
         <v>573.1</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4">
         <f>SUM(F2:F10)</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1377,33 +1377,33 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="3">
         <f>B12</f>
-        <v>495.0</v>
-      </c>
-      <c r="C14" s="3" t="n">
+        <v>495</v>
+      </c>
+      <c r="C14" s="3">
         <f>C12</f>
-        <v>78.1</v>
-      </c>
-      <c r="D14" s="3" t="n">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="D14" s="3">
         <f>D12</f>
         <v>0.15777777777777777</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="E14" s="10">
         <f>E12</f>
         <v>573.1</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4">
         <f>F12</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1412,7 +1412,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1421,7 +1421,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1430,7 +1430,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1462,15 +1462,15 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.6328125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="10.73046875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="28" t="s">
         <v>32</v>
       </c>
@@ -1482,16 +1482,16 @@
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="1">
         <v>6851180</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <f>$B2/$B$7</f>
-        <v>0.9999855501432652</v>
+        <v>0.99998555014326518</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
@@ -1499,20 +1499,20 @@
       <c r="E2" s="1">
         <v>900000</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <f>$E2/$E$7</f>
-        <v>0.1160954918959542</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>0.11609549189595419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="16" t="n">
+      <c r="B3" s="16">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99.0</v>
-      </c>
-      <c r="C3" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="C3" s="2">
         <f>$B3/$B$7</f>
         <v>1.444985673477901E-5</v>
       </c>
@@ -1522,12 +1522,12 @@
       <c r="E3" s="1">
         <v>2450000</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <f>$E3/$E$7</f>
-        <v>0.3160377279389864</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>0.31603772793898638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
@@ -1537,12 +1537,12 @@
       <c r="E4" s="1">
         <v>2250000</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <f>$E4/$E$7</f>
         <v>0.29023872973988546</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
@@ -1552,12 +1552,12 @@
       <c r="E5" s="1">
         <v>2152239</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <f>$E5/$E$7</f>
         <v>0.27762805042517397</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -1569,31 +1569,31 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="2">
         <f>$E6/$E$7</f>
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="3">
         <f>SUM(B2:B6)</f>
-        <v>6851279.0</v>
-      </c>
-      <c r="C7" s="4" t="n">
+        <v>6851279</v>
+      </c>
+      <c r="C7" s="4">
         <f>SUM(C2:C6)</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10" t="n">
+      <c r="E7" s="10">
         <f>SUM(E2:E6)</f>
-        <v>7752239.0</v>
-      </c>
-      <c r="F7" s="4" t="n">
+        <v>7752239</v>
+      </c>
+      <c r="F7" s="4">
         <f>SUM(F2:F6)</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1613,16 +1613,16 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.81640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.08984375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="1" max="1" width="42.796875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.06640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.06640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>42</v>
       </c>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>48</v>
       </c>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -1702,7 +1702,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1721,34 +1721,34 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="7">
         <f>SUM(B3:B5)</f>
-        <v>1.0</v>
-      </c>
-      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <f>SUM(C3:C5)</f>
-        <v>959.0</v>
+        <v>959</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="1">
         <f>F4</f>
-        <v>9587290.0</v>
-      </c>
-      <c r="G6" s="14" t="n">
+        <v>9587290</v>
+      </c>
+      <c r="G6" s="14">
         <f>F6</f>
-        <v>9587290.0</v>
+        <v>9587290</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1759,7 +1759,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>52</v>
       </c>
@@ -1772,7 +1772,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -1829,13 +1829,13 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="15" t="n">
+      <c r="B12" s="15">
         <f>SUM(B10:B11)</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -1844,18 +1844,18 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="1">
         <f>F10</f>
-        <v>672000.0</v>
-      </c>
-      <c r="G12" s="14" t="n">
+        <v>672000</v>
+      </c>
+      <c r="G12" s="14">
         <f>F12</f>
-        <v>672000.0</v>
+        <v>672000</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1866,7 +1866,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1877,7 +1877,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1888,7 +1888,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="32" t="s">
         <v>53</v>
@@ -1907,7 +1907,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -1919,9 +1919,9 @@
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="2">
         <f>$E17/$E$19</f>
-        <v>0.9344983912142069</v>
+        <v>0.93449839121420686</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -1929,7 +1929,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -1941,9 +1941,9 @@
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="2">
         <f>$E18/$E$19</f>
-        <v>0.06550160878579317</v>
+        <v>6.5501608785793169E-2</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -1951,71 +1951,71 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="3">
         <f>SUM(E17:E18)</f>
-        <v>1.025929E7</v>
+        <v>10259290</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="9" t="n">
+      <c r="E20" s="9">
         <f>'Mittelverwendung - Mittelherkun'!E7</f>
-        <v>7752239.0</v>
+        <v>7752239</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="3">
         <f>E19-E20</f>
-        <v>2507051.0</v>
+        <v>2507051</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="2">
         <f>E21/E20</f>
-        <v>0.3233970211702709</v>
+        <v>0.32339702117027092</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2026,7 +2026,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2037,7 +2037,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2062,24 +2062,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2090,12 +2090,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2263,17 +2262,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2297,11 +2299,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Validierung, String-Eingabe der Tranchen, FE korr
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\IdeaProjects\SEPJ\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA8B656-E595-4850-AC20-43C30C4ADBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C80B610-D632-4F15-8D9E-CF0833C4AC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -162,9 +162,6 @@
     <t>BTVG Erlöse</t>
   </si>
   <si>
-    <t>Vst-Korrektur</t>
-  </si>
-  <si>
     <t>Summe</t>
   </si>
   <si>
@@ -292,6 +289,21 @@
   </si>
   <si>
     <t>Basisinformationen</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 3</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 2</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 1</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 4</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 5</t>
   </si>
 </sst>
 </file>
@@ -515,8 +527,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,7 +544,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -830,20 +842,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.53125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.265625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.53125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -852,14 +864,14 @@
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
       <c r="L1" s="27"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -870,38 +882,38 @@
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
@@ -915,16 +927,16 @@
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -935,16 +947,16 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
@@ -955,16 +967,16 @@
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
@@ -975,16 +987,16 @@
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
@@ -995,14 +1007,14 @@
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
@@ -1013,16 +1025,16 @@
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -1038,7 +1050,7 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1066,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
@@ -1077,17 +1089,17 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.06640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
         <v>12</v>
@@ -1106,209 +1118,209 @@
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D2" s="18">
+        <v>1.1</v>
+      </c>
+      <c r="D2" s="18" t="n">
         <f>C2/B2</f>
         <v>0.1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
         <v>12.1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>2.1113243761996161E-2</v>
+        <v>0.02111324376199616</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>22</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D3" s="6">
+        <v>4.4</v>
+      </c>
+      <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
         <v>0.2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
         <v>26.4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>4.6065259117082528E-2</v>
+        <v>0.04606525911708253</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>33</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
         <v>6.6000000000000005</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="6" t="n">
         <f>C4/B4</f>
         <v>0.2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>6.9097888675623803E-2</v>
+        <v>0.0690978886756238</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>44</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D5" s="6">
+        <v>8.8</v>
+      </c>
+      <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
         <v>52.8</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>9.2130518234165057E-2</v>
+        <v>0.09213051823416506</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1">
         <v>55</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="D6" s="6">
+        <v>11.0</v>
+      </c>
+      <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="F6" s="2">
+        <v>66.0</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
         <v>0.11516314779270632</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>66</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
         <v>13.200000000000001</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
         <v>79.2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.13819577735124761</v>
+        <v>0.1381957773512476</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1">
         <v>77</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
         <v>15.4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
         <v>92.4</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
         <v>0.16122840690978887</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>88</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="D9" s="6">
+        <v>17.6</v>
+      </c>
+      <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
         <v>105.6</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.18426103646833011</v>
+        <v>0.1842610364683301</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1321,17 +1333,17 @@
       <c r="D10" s="6">
         <v>0.3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="F10" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.17274472168905949</v>
+        <v>0.1727447216890595</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1340,33 +1352,33 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>495</v>
-      </c>
-      <c r="C12" s="3">
+        <v>495.0</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>78.099999999999994</v>
-      </c>
-      <c r="D12" s="4">
+        <v>78.1</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <f>C12/B12</f>
         <v>0.15777777777777777</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="10" t="n">
         <f>B12+C12</f>
         <v>573.1</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1377,33 +1389,33 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>495</v>
-      </c>
-      <c r="C14" s="3">
+        <v>495.0</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>78.099999999999994</v>
-      </c>
-      <c r="D14" s="3">
+        <v>78.1</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <f>D12</f>
         <v>0.15777777777777777</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="10" t="n">
         <f>E12</f>
         <v>573.1</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1412,7 +1424,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1421,7 +1433,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1430,7 +1442,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1438,7 +1450,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1456,21 +1468,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C08536-E6A3-4E31-88A7-DF1DE6751CED}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.73046875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>32</v>
       </c>
@@ -1482,124 +1494,664 @@
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1">
-        <v>6851180</v>
-      </c>
-      <c r="C2" s="2">
-        <f>$B2/$B$7</f>
-        <v>0.99998555014326518</v>
+      <c r="B2" s="1" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <f>$B2/$B7</f>
+        <v>0.5540540540540541</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1">
-        <v>900000</v>
-      </c>
-      <c r="F2" s="2">
-        <f>$E2/$E$7</f>
-        <v>0.11609549189595419</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E2" s="1" t="n">
+        <v>234.0</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <f>$E2/$E7</f>
+        <v>0.22941176470588234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99</v>
-      </c>
-      <c r="C3" s="2">
-        <f>$B3/$B$7</f>
-        <v>1.444985673477901E-5</v>
+        <v>99.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <f>$B3/$B7</f>
+        <v>0.44594594594594594</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="1">
-        <v>2450000</v>
-      </c>
-      <c r="F3" s="2">
-        <f>$E3/$E$7</f>
-        <v>0.31603772793898638</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E3" s="1" t="n">
+        <v>321.0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <f>$E3/$E7</f>
+        <v>0.31470588235294117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
       <c r="D4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="1">
-        <v>2250000</v>
-      </c>
-      <c r="F4" s="2">
-        <f>$E4/$E$7</f>
-        <v>0.29023872973988546</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E4" s="1" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <f>$E4/$E7</f>
+        <v>0.12058823529411765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="1">
-        <v>2152239</v>
-      </c>
-      <c r="F5" s="2">
-        <f>$E5/$E$7</f>
-        <v>0.27762805042517397</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="E5" s="1" t="n">
+        <v>342.0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <f>$E5/$E7</f>
+        <v>0.3352941176470588</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <f>$E6/$E$7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>6851279</v>
-      </c>
-      <c r="C7" s="4">
+        <v>222.0</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10">
+      <c r="E7" s="10" t="n">
         <f>SUM(E2:E6)</f>
-        <v>7752239</v>
-      </c>
-      <c r="F7" s="4">
+        <v>1020.0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f>SUM(F2:F6)</f>
-        <v>1</v>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <f>$B11/$B15</f>
+        <v>0.5540540540540541</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>234.0</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <f>$E11/$E15</f>
+        <v>0.20689655172413793</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="16" t="n">
+        <f>Gesamtinvestitionskosten!B10</f>
+        <v>99.0</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <f>$B12/$B15</f>
+        <v>0.44594594594594594</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>555.0</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <f>$E12/$E15</f>
+        <v>0.4907161803713528</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>342.0</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <f>$E13/$E15</f>
+        <v>0.30238726790450926</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <f>SUM(B11:B14)</f>
+        <v>222.0</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <f>SUM(C11:C14)</f>
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="10" t="n">
+        <f>SUM(E11:E14)</f>
+        <v>1131.0</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <f>SUM(F11:F14)</f>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <f>$B19/$B25</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1">
+        <v>23</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <f>$E19/$E25</f>
+        <v>0.0756578947368421</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="16" t="n">
+        <f>Gesamtinvestitionskosten!B10</f>
+        <v>99.0</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <f>$B20/$B25</f>
+        <v>0.8918918918918919</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="1">
+        <v>22</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <f>$E20/$E25</f>
+        <v>0.07236842105263158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="1">
+        <v>222</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <f>$E21/$E25</f>
+        <v>0.7302631578947368</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <f>$E22/$E25</f>
+        <v>0.009868421052631578</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="1">
+        <v>34</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <f>$E23/$E25</f>
+        <v>0.1118421052631579</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <f>SUM(B19:B24)</f>
+        <v>111.0</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <f>SUM(C19:C24)</f>
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="10" t="n">
+        <f>SUM(E19:E24)</f>
+        <v>304.0</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <f>SUM(F19:F24)</f>
+        <v>0.9999999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="1">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <f>$B29/$B36</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="1">
+        <v>23</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <f>$E29/$E36</f>
+        <v>0.06005221932114883</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="16">
+        <v>99</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <f>$B30/$B36</f>
+        <v>0.8918918918918919</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="1">
+        <v>98</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <f>$E30/$E36</f>
+        <v>0.2558746736292428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="1">
+        <v>87</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <f>$E31/$E36</f>
+        <v>0.22715404699738903</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="1">
+        <v>76</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <f>$E32/$E36</f>
+        <v>0.19843342036553524</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="1">
+        <v>65</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <f>$E33/$E36</f>
+        <v>0.16971279373368145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="1">
+        <v>34</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <f>$E34/$E36</f>
+        <v>0.08877284595300261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <f>SUM(B29:B35)</f>
+        <v>111.0</v>
+      </c>
+      <c r="C36" s="4" t="n">
+        <f>SUM(C29:C35)</f>
+        <v>1.0</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="10" t="n">
+        <f>SUM(E29:E35)</f>
+        <v>383.0</v>
+      </c>
+      <c r="F36" s="4" t="n">
+        <f>SUM(F29:F35)</f>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="1">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <f>$B40/$B48</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="1">
+        <v>23</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <f>$E40/$E48</f>
+        <v>0.058673469387755105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="16">
+        <v>99</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <f>$B41/$B48</f>
+        <v>0.8918918918918919</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="1">
+        <v>45</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <f>$E41/$E48</f>
+        <v>0.11479591836734694</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="1">
+        <v>56</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <f>$E42/$E48</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="1">
+        <v>67</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <f>$E43/$E48</f>
+        <v>0.17091836734693877</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="1">
+        <v>78</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <f>$E44/$E48</f>
+        <v>0.1989795918367347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="1">
+        <v>89</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <f>$E45/$E48</f>
+        <v>0.22704081632653061</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="1">
+        <v>34</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <f>$E46/$E48</f>
+        <v>0.08673469387755102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="3" t="n">
+        <f>SUM(B40:B47)</f>
+        <v>111.0</v>
+      </c>
+      <c r="C48" s="4" t="n">
+        <f>SUM(C40:C47)</f>
+        <v>1.0</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="10" t="n">
+        <f>SUM(E40:E47)</f>
+        <v>392.0</v>
+      </c>
+      <c r="F48" s="4" t="n">
+        <f>SUM(F40:F47)</f>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="10">
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:F39"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1613,41 +2165,41 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.06640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.06640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1662,9 +2214,9 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1681,9 +2233,9 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="15">
         <v>1</v>
@@ -1702,9 +2254,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -1721,34 +2273,34 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="7">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <f>SUM(B3:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f>SUM(C3:C5)</f>
-        <v>959</v>
+        <v>959.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="n">
         <f>F4</f>
-        <v>9587290</v>
-      </c>
-      <c r="G6" s="14">
+        <v>9587290.0</v>
+      </c>
+      <c r="G6" s="14" t="n">
         <f>F6</f>
-        <v>9587290</v>
+        <v>9587290.0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1759,9 +2311,9 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1772,9 +2324,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1791,9 +2343,9 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
@@ -1810,9 +2362,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
@@ -1829,13 +2381,13 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="15">
+        <v>40</v>
+      </c>
+      <c r="B12" s="15" t="n">
         <f>SUM(B10:B11)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -1844,18 +2396,18 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="n">
         <f>F10</f>
-        <v>672000</v>
-      </c>
-      <c r="G12" s="14">
+        <v>672000.0</v>
+      </c>
+      <c r="G12" s="14" t="n">
         <f>F12</f>
-        <v>672000</v>
+        <v>672000.0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1866,7 +2418,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1877,7 +2429,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1888,40 +2440,40 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
       <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="n">
         <f>$E17/$E$19</f>
-        <v>0.93449839121420686</v>
+        <v>0.9344983912142069</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -1929,21 +2481,21 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="n">
         <f>$E18/$E$19</f>
-        <v>6.5501608785793169E-2</v>
+        <v>0.06550160878579317</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -1951,71 +2503,71 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="n">
         <f>SUM(E17:E18)</f>
-        <v>10259290</v>
+        <v>1.025929E7</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="9">
+      <c r="E20" s="9" t="n">
         <f>'Mittelverwendung - Mittelherkun'!E7</f>
-        <v>7752239</v>
+        <v>1020.0</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="n">
         <f>E19-E20</f>
-        <v>2507051</v>
+        <v>1.025827E7</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2">
+      <c r="E22" s="2" t="n">
         <f>E21/E20</f>
-        <v>0.32339702117027092</v>
+        <v>10057.127450980392</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2026,7 +2578,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2037,7 +2589,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2062,26 +2614,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2090,11 +2642,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2262,20 +2815,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2299,9 +2849,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Alle Tabellen sind im pdf drinnen
To do's:
- Überlappungen bei den Wörtern regeln
- Schöne Tsbellen machen
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -832,9 +832,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.53125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.265625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.53125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.53125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.265625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.53125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -1076,9 +1076,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.06640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.06640625" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -1104,24 +1104,24 @@
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="1" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="D2" s="18">
+        <v>11.100000000000001</v>
+      </c>
+      <c r="D2" s="18" t="n">
         <f>C2/B2</f>
         <v>0.10000000000000002</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>13.2</v>
-      </c>
-      <c r="F2" s="2">
+        <v>122.1</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>2.5703436861065136E-2</v>
+        <v>0.14265685243603224</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1129,24 +1129,24 @@
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="1" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="D3" s="6">
+        <v>16.65</v>
+      </c>
+      <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
         <v>0.15</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>13.8</v>
-      </c>
-      <c r="F3" s="2">
+        <v>127.65</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>2.6871774900204464E-2</v>
+        <v>0.14914125481948826</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1154,24 +1154,24 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="1" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
-        <v>1.05</v>
-      </c>
-      <c r="D4" s="6">
+        <v>16.65</v>
+      </c>
+      <c r="D4" s="6" t="n">
         <f>C4/B4</f>
         <v>0.15</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="F4" s="2">
+        <v>127.65</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.567520202511927E-2</v>
+        <v>0.14914125481948826</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1182,21 +1182,21 @@
       <c r="B5" s="1">
         <v>44</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <f t="shared" si="2"/>
         <v>6.6</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
         <v>50.6</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>9.8529841300749696E-2</v>
+        <v>0.05911905596448184</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1207,21 +1207,21 @@
       <c r="B6" s="1">
         <v>55</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
         <v>8.25</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
         <v>63.25</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.12316230162593711</v>
+        <v>0.0738988199556023</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1232,21 +1232,21 @@
       <c r="B7" s="1">
         <v>66</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
         <v>9.9</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>75.900000000000006</v>
-      </c>
-      <c r="F7" s="2">
+        <v>75.9</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.14779476195112454</v>
+        <v>0.08867858394672276</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1257,21 +1257,21 @@
       <c r="B8" s="1">
         <v>77</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
         <v>11.549999999999999</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
         <v>88.55</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.17242722227631196</v>
+        <v>0.10345834793784321</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1282,21 +1282,21 @@
       <c r="B9" s="1">
         <v>88</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
         <v>13.2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
         <v>101.2</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.19705968260149939</v>
+        <v>0.11823811192896368</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1313,13 +1313,13 @@
       <c r="D10" s="6">
         <v>0.3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="F10" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.19277577645798852</v>
+        <v>0.1156677181913775</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1336,25 +1336,25 @@
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>460</v>
-      </c>
-      <c r="C12" s="3">
+        <v>762.0</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>53.55</v>
-      </c>
-      <c r="D12" s="4">
+        <v>93.9</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.11641304347826087</v>
-      </c>
-      <c r="E12" s="10">
+        <v>0.12322834645669292</v>
+      </c>
+      <c r="E12" s="10" t="n">
         <f>B12+C12</f>
-        <v>513.54999999999995</v>
-      </c>
-      <c r="F12" s="4">
+        <v>855.9</v>
+      </c>
+      <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1373,25 +1373,25 @@
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>460</v>
-      </c>
-      <c r="C14" s="3">
+        <v>762.0</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>53.55</v>
-      </c>
-      <c r="D14" s="3">
+        <v>93.9</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.11641304347826087</v>
-      </c>
-      <c r="E14" s="10">
+        <v>0.12322834645669292</v>
+      </c>
+      <c r="E14" s="10" t="n">
         <f>E12</f>
-        <v>513.54999999999995</v>
-      </c>
-      <c r="F14" s="4">
+        <v>855.9</v>
+      </c>
+      <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1456,10 +1456,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.73046875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.59765625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -1481,9 +1481,9 @@
       <c r="B2" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <f>$B2/$B$7</f>
-        <v>9.1743119266055051E-2</v>
+        <v>0.09174311926605505</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
@@ -1491,7 +1491,7 @@
       <c r="E2" s="1">
         <v>20</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f>$E2/$E$7</f>
         <v>0.37735849056603776</v>
       </c>
@@ -1500,13 +1500,13 @@
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99</v>
-      </c>
-      <c r="C3" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <f>$B3/$B$7</f>
-        <v>0.90825688073394495</v>
+        <v>0.908256880733945</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>37</v>
@@ -1514,9 +1514,9 @@
       <c r="E3" s="1">
         <v>30</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f>$E3/$E$7</f>
-        <v>0.56603773584905659</v>
+        <v>0.5660377358490566</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
@@ -1529,9 +1529,9 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f>$E4/$E$7</f>
-        <v>1.8867924528301886E-2</v>
+        <v>0.018867924528301886</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -1544,9 +1544,9 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f>$E5/$E$7</f>
-        <v>3.7735849056603772E-2</v>
+        <v>0.03773584905660377</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1561,31 +1561,31 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <f>$E6/$E$7</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>109</v>
-      </c>
-      <c r="C7" s="4">
+        <v>109.0</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10">
+      <c r="E7" s="10" t="n">
         <f>SUM(E2:E6)</f>
-        <v>53</v>
-      </c>
-      <c r="F7" s="4">
+        <v>53.0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f>SUM(F2:F6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1604,11 +1604,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.06640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.06640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.796875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.06640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.06640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -1714,25 +1714,25 @@
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="7" t="n">
         <f>SUM(B3:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f>SUM(C3:C5)</f>
-        <v>959</v>
+        <v>959.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="n">
         <f>F4</f>
-        <v>9587290</v>
-      </c>
-      <c r="G6" s="14">
+        <v>9587290.0</v>
+      </c>
+      <c r="G6" s="14" t="n">
         <f>F6</f>
-        <v>9587290</v>
+        <v>9587290.0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1822,9 +1822,9 @@
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="15" t="n">
         <f>SUM(B10:B11)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -1833,13 +1833,13 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="n">
         <f>F10</f>
-        <v>672000</v>
-      </c>
-      <c r="G12" s="14">
+        <v>672000.0</v>
+      </c>
+      <c r="G12" s="14" t="n">
         <f>F12</f>
-        <v>672000</v>
+        <v>672000.0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1908,9 +1908,9 @@
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="n">
         <f>$E17/$E$19</f>
-        <v>0.93449839121420686</v>
+        <v>0.9344983912142069</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -1930,9 +1930,9 @@
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="n">
         <f>$E18/$E$19</f>
-        <v>6.5501608785793169E-2</v>
+        <v>0.06550160878579317</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -1947,9 +1947,9 @@
         <v>41</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="n">
         <f>SUM(E17:E18)</f>
-        <v>10259290</v>
+        <v>1.025929E7</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1963,9 +1963,9 @@
         <v>58</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="9">
+      <c r="E20" s="9" t="n">
         <f>'Mittelverwendung - Mittelherkun'!E7</f>
-        <v>53</v>
+        <v>53.0</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1979,9 +1979,9 @@
         <v>59</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="n">
         <f>E19-E20</f>
-        <v>10259237</v>
+        <v>1.0259237E7</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1995,7 +1995,7 @@
         <v>60</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2">
+      <c r="E22" s="2" t="n">
         <f>E21/E20</f>
         <v>193570.50943396226</v>
       </c>

</xml_diff>

<commit_message>
bilder eingefügt, logo einfügen, pdf combination
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43677\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA8B656-E595-4850-AC20-43C30C4ADBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5502D352-6E3C-4ED0-A0D5-F4A429267A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="37185" yWindow="1065" windowWidth="14400" windowHeight="14415" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="95">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -261,37 +283,70 @@
     <t xml:space="preserve">Maps - Bild </t>
   </si>
   <si>
-    <t>Lage der Öffi Anbindung</t>
-  </si>
-  <si>
     <t>oihjubjpkojk</t>
   </si>
   <si>
-    <t>ghetto wien</t>
-  </si>
-  <si>
-    <t>Apfelcompany</t>
-  </si>
-  <si>
-    <t>Siehdichvorstrasse 12</t>
-  </si>
-  <si>
-    <t>2231</t>
-  </si>
-  <si>
-    <t>Strasshof</t>
-  </si>
-  <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>nix</t>
-  </si>
-  <si>
     <t>m²</t>
   </si>
   <si>
     <t>Basisinformationen</t>
+  </si>
+  <si>
+    <t>Öffi Anbindung</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>firma a</t>
+  </si>
+  <si>
+    <t>strasse 1</t>
+  </si>
+  <si>
+    <t>1220</t>
+  </si>
+  <si>
+    <t>wien</t>
+  </si>
+  <si>
+    <t>wundervoll</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilder </t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>1g</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>frerunl</t>
+  </si>
+  <si>
+    <t>d55</t>
   </si>
 </sst>
 </file>
@@ -515,8 +570,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -531,8 +586,125 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE7753D-920E-EAAF-3EE5-6752319EE12A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3600450"/>
+          <a:ext cx="18288000" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -828,22 +1000,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.53125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.265625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.53125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.08984375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.26953125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.54296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -859,11 +1031,13 @@
       <c r="K1" s="26"/>
       <c r="L1" s="27"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -873,19 +1047,21 @@
         <v>66</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C3" s="19" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -895,17 +1071,19 @@
         <v>67</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C4" s="19" t="str">
         <f>+C3</f>
         <v>m²</v>
@@ -918,17 +1096,19 @@
         <v>68</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -938,17 +1118,19 @@
         <v>69</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -958,17 +1140,19 @@
         <v>70</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -978,17 +1162,19 @@
         <v>71</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
@@ -1002,31 +1188,35 @@
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="21"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1038,11 +1228,13 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="24" t="s">
+        <v>78</v>
+      </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1054,21 +1246,41 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
+    <row r="17" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+    </row>
+    <row r="19" spans="1:5" ht="163" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="164" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:5" ht="112" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="H1:L1"/>
+    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1080,14 +1292,14 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.06640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.08984375" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
         <v>12</v>
@@ -1106,209 +1318,209 @@
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D2" s="18">
+        <v>1.1</v>
+      </c>
+      <c r="D2" s="18" t="n">
         <f>C2/B2</f>
         <v>0.1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
         <v>12.1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>2.1113243761996161E-2</v>
+        <v>0.02111324376199616</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>22</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D3" s="6">
+        <v>4.4</v>
+      </c>
+      <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
         <v>0.2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
         <v>26.4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>4.6065259117082528E-2</v>
+        <v>0.04606525911708253</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>33</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
         <v>6.6000000000000005</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="6" t="n">
         <f>C4/B4</f>
         <v>0.2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>6.9097888675623803E-2</v>
+        <v>0.0690978886756238</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>44</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D5" s="6">
+        <v>8.8</v>
+      </c>
+      <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
         <v>52.8</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>9.2130518234165057E-2</v>
+        <v>0.09213051823416506</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1">
         <v>55</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="D6" s="6">
+        <v>11.0</v>
+      </c>
+      <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="F6" s="2">
+        <v>66.0</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
         <v>0.11516314779270632</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>66</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
         <v>13.200000000000001</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
         <v>79.2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.13819577735124761</v>
+        <v>0.1381957773512476</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1">
         <v>77</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
         <v>15.4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
         <v>92.4</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
         <v>0.16122840690978887</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>88</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="D9" s="6">
+        <v>17.6</v>
+      </c>
+      <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
         <v>105.6</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.18426103646833011</v>
+        <v>0.1842610364683301</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1321,17 +1533,17 @@
       <c r="D10" s="6">
         <v>0.3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="F10" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.17274472168905949</v>
+        <v>0.1727447216890595</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1340,33 +1552,33 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>495</v>
-      </c>
-      <c r="C12" s="3">
+        <v>495.0</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>78.099999999999994</v>
-      </c>
-      <c r="D12" s="4">
+        <v>78.1</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <f>C12/B12</f>
         <v>0.15777777777777777</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="10" t="n">
         <f>B12+C12</f>
         <v>573.1</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1377,33 +1589,33 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>495</v>
-      </c>
-      <c r="C14" s="3">
+        <v>495.0</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>78.099999999999994</v>
-      </c>
-      <c r="D14" s="3">
+        <v>78.1</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <f>D12</f>
         <v>0.15777777777777777</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="10" t="n">
         <f>E12</f>
         <v>573.1</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1412,7 +1624,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1421,7 +1633,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1430,7 +1642,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1438,7 +1650,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1462,15 +1674,15 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.73046875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.6328125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>32</v>
       </c>
@@ -1482,16 +1694,16 @@
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="1">
         <v>6851180</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <f>$B2/$B$7</f>
-        <v>0.99998555014326518</v>
+        <v>0.9999855501432652</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
@@ -1499,20 +1711,20 @@
       <c r="E2" s="1">
         <v>900000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f>$E2/$E$7</f>
-        <v>0.11609549189595419</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>0.1160954918959542</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99</v>
-      </c>
-      <c r="C3" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <f>$B3/$B$7</f>
         <v>1.444985673477901E-5</v>
       </c>
@@ -1522,12 +1734,12 @@
       <c r="E3" s="1">
         <v>2450000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f>$E3/$E$7</f>
-        <v>0.31603772793898638</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>0.3160377279389864</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
@@ -1537,12 +1749,12 @@
       <c r="E4" s="1">
         <v>2250000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f>$E4/$E$7</f>
         <v>0.29023872973988546</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
@@ -1552,12 +1764,12 @@
       <c r="E5" s="1">
         <v>2152239</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f>$E5/$E$7</f>
         <v>0.27762805042517397</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -1569,31 +1781,31 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <f>$E6/$E$7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>6851279</v>
-      </c>
-      <c r="C7" s="4">
+        <v>6851279.0</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10">
+      <c r="E7" s="10" t="n">
         <f>SUM(E2:E6)</f>
-        <v>7752239</v>
-      </c>
-      <c r="F7" s="4">
+        <v>7752239.0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f>SUM(F2:F6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1613,16 +1825,16 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.06640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.06640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.81640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.08984375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.81640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.08984375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>42</v>
       </c>
@@ -1645,7 +1857,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>48</v>
       </c>
@@ -1662,7 +1874,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -1681,7 +1893,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -1702,7 +1914,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1721,34 +1933,34 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="7" t="n">
         <f>SUM(B3:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f>SUM(C3:C5)</f>
-        <v>959</v>
+        <v>959.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="n">
         <f>F4</f>
-        <v>9587290</v>
-      </c>
-      <c r="G6" s="14">
+        <v>9587290.0</v>
+      </c>
+      <c r="G6" s="14" t="n">
         <f>F6</f>
-        <v>9587290</v>
+        <v>9587290.0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1759,7 +1971,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>52</v>
       </c>
@@ -1772,7 +1984,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1791,7 +2003,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -1810,7 +2022,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -1829,13 +2041,13 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="15" t="n">
         <f>SUM(B10:B11)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -1844,18 +2056,18 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="n">
         <f>F10</f>
-        <v>672000</v>
-      </c>
-      <c r="G12" s="14">
+        <v>672000.0</v>
+      </c>
+      <c r="G12" s="14" t="n">
         <f>F12</f>
-        <v>672000</v>
+        <v>672000.0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1866,7 +2078,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1877,7 +2089,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1888,7 +2100,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="32" t="s">
         <v>53</v>
@@ -1907,7 +2119,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -1919,9 +2131,9 @@
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="n">
         <f>$E17/$E$19</f>
-        <v>0.93449839121420686</v>
+        <v>0.9344983912142069</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -1929,7 +2141,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -1941,9 +2153,9 @@
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="n">
         <f>$E18/$E$19</f>
-        <v>6.5501608785793169E-2</v>
+        <v>0.06550160878579317</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -1951,71 +2163,71 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="n">
         <f>SUM(E17:E18)</f>
-        <v>10259290</v>
+        <v>1.025929E7</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="9">
+      <c r="E20" s="9" t="n">
         <f>'Mittelverwendung - Mittelherkun'!E7</f>
-        <v>7752239</v>
+        <v>7752239.0</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="n">
         <f>E19-E20</f>
-        <v>2507051</v>
+        <v>2507051.0</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2">
+      <c r="E22" s="2" t="n">
         <f>E21/E20</f>
-        <v>0.32339702117027092</v>
+        <v>0.3233970211702709</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2026,7 +2238,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2037,7 +2249,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2062,24 +2274,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2090,14 +2302,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -2261,6 +2465,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2271,16 +2483,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2298,6 +2500,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
- TabControl ist eingebaut - Text kann man hinzufügen
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -1122,12 +1122,12 @@
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1">
-        <v>11</v>
+      <c r="B2" s="1" t="n">
+        <v>100.0</v>
       </c>
       <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>1.1</v>
+        <v>10.0</v>
       </c>
       <c r="D2" s="18" t="n">
         <f>C2/B2</f>
@@ -1135,11 +1135,11 @@
       </c>
       <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>12.1</v>
+        <v>110.0</v>
       </c>
       <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>0.02111324376199616</v>
+        <v>0.07136184347104006</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1147,24 +1147,24 @@
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1">
-        <v>22</v>
+      <c r="B3" s="1" t="n">
+        <v>110.0</v>
       </c>
       <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>4.4</v>
+        <v>59.400000000000006</v>
       </c>
       <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
-        <v>0.2</v>
+        <v>0.54</v>
       </c>
       <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>26.4</v>
+        <v>169.4</v>
       </c>
       <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.04606525911708253</v>
+        <v>0.1098972389454017</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1172,24 +1172,24 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1">
-        <v>33</v>
+      <c r="B4" s="1" t="n">
+        <v>120.0</v>
       </c>
       <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
-        <v>6.6000000000000005</v>
+        <v>64.80000000000001</v>
       </c>
       <c r="D4" s="6" t="n">
         <f>C4/B4</f>
-        <v>0.2</v>
+        <v>0.5400000000000001</v>
       </c>
       <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>39.6</v>
+        <v>184.8</v>
       </c>
       <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.0690978886756238</v>
+        <v>0.11988789703134732</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1197,24 +1197,24 @@
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1">
-        <v>44</v>
+      <c r="B5" s="1" t="n">
+        <v>130.0</v>
       </c>
       <c r="C5" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>8.8</v>
+        <v>70.2</v>
       </c>
       <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.54</v>
       </c>
       <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>52.8</v>
+        <v>200.2</v>
       </c>
       <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.09213051823416506</v>
+        <v>0.1298785551172929</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1222,24 +1222,24 @@
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1">
-        <v>55</v>
+      <c r="B6" s="1" t="n">
+        <v>140.0</v>
       </c>
       <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>11.0</v>
+        <v>75.60000000000001</v>
       </c>
       <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.54</v>
       </c>
       <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>66.0</v>
+        <v>215.60000000000002</v>
       </c>
       <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.11516314779270632</v>
+        <v>0.13986921320323853</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1247,24 +1247,24 @@
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1">
-        <v>66</v>
+      <c r="B7" s="1" t="n">
+        <v>150.0</v>
       </c>
       <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>13.200000000000001</v>
+        <v>81.0</v>
       </c>
       <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.54</v>
       </c>
       <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>79.2</v>
+        <v>231.0</v>
       </c>
       <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.1381957773512476</v>
+        <v>0.14985987128918413</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>73</v>
@@ -1274,24 +1274,24 @@
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1">
-        <v>77</v>
+      <c r="B8" s="1" t="n">
+        <v>160.0</v>
       </c>
       <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>15.4</v>
+        <v>86.4</v>
       </c>
       <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.54</v>
       </c>
       <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>92.4</v>
+        <v>246.4</v>
       </c>
       <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.16122840690978887</v>
+        <v>0.15985052937512975</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1299,24 +1299,24 @@
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1">
-        <v>88</v>
+      <c r="B9" s="1" t="n">
+        <v>76.0</v>
       </c>
       <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>17.6</v>
+        <v>41.040000000000006</v>
       </c>
       <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.54</v>
       </c>
       <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>105.6</v>
+        <v>117.04</v>
       </c>
       <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.1842610364683301</v>
+        <v>0.07592900145318664</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1324,22 +1324,22 @@
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="9">
-        <v>99</v>
+      <c r="B10" s="9" t="n">
+        <v>67.0</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
-      <c r="D10" s="6">
-        <v>0.3</v>
+      <c r="D10" s="6" t="n">
+        <v>0.77</v>
       </c>
       <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>99.0</v>
+        <v>67.0</v>
       </c>
       <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.1727447216890595</v>
+        <v>0.04346585011417895</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1358,23 +1358,23 @@
       </c>
       <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>495.0</v>
+        <v>1053.0</v>
       </c>
       <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>78.1</v>
+        <v>488.4400000000001</v>
       </c>
       <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.15777777777777777</v>
+        <v>0.4638556505223173</v>
       </c>
       <c r="E12" s="10" t="n">
         <f>B12+C12</f>
-        <v>573.1</v>
+        <v>1541.44</v>
       </c>
       <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1395,23 +1395,23 @@
       </c>
       <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>495.0</v>
+        <v>1053.0</v>
       </c>
       <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>78.1</v>
+        <v>488.4400000000001</v>
       </c>
       <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.15777777777777777</v>
+        <v>0.4638556505223173</v>
       </c>
       <c r="E14" s="10" t="n">
         <f>E12</f>
-        <v>573.1</v>
+        <v>1541.44</v>
       </c>
       <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1446,15 +1446,15 @@
       <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="11">
-        <v>0.2</v>
+      <c r="B20" s="11" t="n">
+        <v>0.54</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="12" t="n">
         <v>0.1</v>
       </c>
       <c r="C21" t="s">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="C2" s="2" t="n">
         <f>$B2/$B7</f>
-        <v>0.5540540540540541</v>
+        <v>0.6473684210526316</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
@@ -1522,11 +1522,11 @@
       </c>
       <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99.0</v>
+        <v>67.0</v>
       </c>
       <c r="C3" s="2" t="n">
         <f>$B3/$B7</f>
-        <v>0.44594594594594594</v>
+        <v>0.3526315789473684</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>37</v>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>222.0</v>
+        <v>190.0</v>
       </c>
       <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="C11" s="2" t="n">
         <f>$B11/$B15</f>
-        <v>0.5540540540540541</v>
+        <v>0.6473684210526316</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>35</v>
@@ -1639,11 +1639,11 @@
       </c>
       <c r="B12" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99.0</v>
+        <v>67.0</v>
       </c>
       <c r="C12" s="2" t="n">
         <f>$B12/$B15</f>
-        <v>0.44594594594594594</v>
+        <v>0.3526315789473684</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>85</v>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="B15" s="3" t="n">
         <f>SUM(B11:B14)</f>
-        <v>222.0</v>
+        <v>190.0</v>
       </c>
       <c r="C15" s="4" t="n">
         <f>SUM(C11:C14)</f>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C19" s="2" t="n">
         <f>$B19/$B25</f>
-        <v>0.10810810810810811</v>
+        <v>0.1518987341772152</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>35</v>
@@ -1741,11 +1741,11 @@
       </c>
       <c r="B20" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99.0</v>
+        <v>67.0</v>
       </c>
       <c r="C20" s="2" t="n">
         <f>$B20/$B25</f>
-        <v>0.8918918918918919</v>
+        <v>0.8481012658227848</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>85</v>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="B25" s="3" t="n">
         <f>SUM(B19:B24)</f>
-        <v>111.0</v>
+        <v>79.0</v>
       </c>
       <c r="C25" s="4" t="n">
         <f>SUM(C19:C24)</f>

</xml_diff>

<commit_message>
Flächenwidmung scripting, check update
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\IdeaProjects\SEPJ\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A85E7F-75A6-419D-A2D6-54741B9FCA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3D1A93-E4EE-4DF1-977C-76AB0AE3017A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="28965" yWindow="645" windowWidth="21600" windowHeight="11325" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="106">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -301,6 +301,65 @@
   </si>
   <si>
     <t>Braumüllergasse 21</t>
+  </si>
+  <si>
+    <t>IG III = Bauklasse 3</t>
+  </si>
+  <si>
+    <t>g = geschlossene Bauweise</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>WGV I = Bauklasse 1</t>
+  </si>
+  <si>
+    <t>WGV III = Bauklasse 3</t>
+  </si>
+  <si>
+    <t>gk = gekuppelte Bauweise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>W II = Bauklasse 2</t>
+  </si>
+  <si>
+    <t>W II = Bauklasse 2 beschränkt auf 20%</t>
+  </si>
+  <si>
+    <t>G = Gärtnerische Ausgestaltung</t>
+  </si>
+  <si>
+    <t>ÖZ = Grundflächen für öffentliche Zwecke (Enteignung möglich)</t>
+  </si>
+  <si>
+    <t>WGV II = Bauklasse 2</t>
+  </si>
+  <si>
+    <t>GB II = Bauklasse 2</t>
+  </si>
+  <si>
+    <t>ÖZ = Grundflächen für öffentliche Zwecke (Enteignung möglich)
+Test = test</t>
+  </si>
+  <si>
+    <t>Ekz = für Einkaufszentren</t>
+  </si>
+  <si>
+    <t>Ekz = für Einkaufszentren bestimmt</t>
+  </si>
+  <si>
+    <t>W III = Bauklasse 3</t>
+  </si>
+  <si>
+    <t>o = offene Bauweise</t>
+  </si>
+  <si>
+    <t>GS II = Bauklasse 2</t>
   </si>
 </sst>
 </file>
@@ -837,17 +896,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
@@ -1071,6 +1130,26 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1091,9 +1170,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -1122,21 +1201,21 @@
       <c r="B2" s="1">
         <v>11</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D2" s="18">
+        <v>1.1</v>
+      </c>
+      <c r="D2" s="18" t="n">
         <f>C2/B2</f>
         <v>0.1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
         <v>12.1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>2.1113243761996161E-2</v>
+        <v>0.02111324376199616</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1147,21 +1226,21 @@
       <c r="B3" s="1">
         <v>22</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D3" s="6">
+        <v>4.4</v>
+      </c>
+      <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
         <v>0.2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
         <v>26.4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>4.6065259117082528E-2</v>
+        <v>0.04606525911708253</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1172,21 +1251,21 @@
       <c r="B4" s="1">
         <v>33</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
         <v>6.6000000000000005</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="6" t="n">
         <f>C4/B4</f>
         <v>0.2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>6.9097888675623803E-2</v>
+        <v>0.0690978886756238</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1197,21 +1276,21 @@
       <c r="B5" s="1">
         <v>44</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D5" s="6">
+        <v>8.8</v>
+      </c>
+      <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
         <v>52.8</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>9.2130518234165057E-2</v>
+        <v>0.09213051823416506</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1222,19 +1301,19 @@
       <c r="B6" s="1">
         <v>55</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="D6" s="6">
+        <v>11.0</v>
+      </c>
+      <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="F6" s="2">
+        <v>66.0</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
         <v>0.11516314779270632</v>
       </c>
@@ -1247,21 +1326,21 @@
       <c r="B7" s="1">
         <v>66</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
         <v>13.200000000000001</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
         <v>79.2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.13819577735124761</v>
+        <v>0.1381957773512476</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>73</v>
@@ -1274,19 +1353,19 @@
       <c r="B8" s="1">
         <v>77</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
         <v>15.4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
         <v>92.4</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
         <v>0.16122840690978887</v>
       </c>
@@ -1299,21 +1378,21 @@
       <c r="B9" s="1">
         <v>88</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="D9" s="6">
+        <v>17.6</v>
+      </c>
+      <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
         <v>105.6</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.18426103646833011</v>
+        <v>0.1842610364683301</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1330,13 +1409,13 @@
       <c r="D10" s="6">
         <v>0.3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="F10" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.17274472168905949</v>
+        <v>0.1727447216890595</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1353,25 +1432,25 @@
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>495</v>
-      </c>
-      <c r="C12" s="3">
+        <v>495.0</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>78.099999999999994</v>
-      </c>
-      <c r="D12" s="4">
+        <v>78.1</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <f>C12/B12</f>
         <v>0.15777777777777777</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="10" t="n">
         <f>B12+C12</f>
         <v>573.1</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1390,25 +1469,25 @@
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>495</v>
-      </c>
-      <c r="C14" s="3">
+        <v>495.0</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>78.099999999999994</v>
-      </c>
-      <c r="D14" s="3">
+        <v>78.1</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <f>D12</f>
         <v>0.15777777777777777</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="10" t="n">
         <f>E12</f>
         <v>573.1</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1473,10 +1552,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -1498,9 +1577,9 @@
       <c r="B2" s="1">
         <v>123</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <f>$B2/$B7</f>
-        <v>0.55405405405405406</v>
+        <v>0.5540540540540541</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
@@ -1508,7 +1587,7 @@
       <c r="E2" s="1">
         <v>234</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f>$E2/$E7</f>
         <v>0.22941176470588234</v>
       </c>
@@ -1517,11 +1596,11 @@
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99</v>
-      </c>
-      <c r="C3" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <f>$B3/$B7</f>
         <v>0.44594594594594594</v>
       </c>
@@ -1531,7 +1610,7 @@
       <c r="E3" s="1">
         <v>321</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f>$E3/$E7</f>
         <v>0.31470588235294117</v>
       </c>
@@ -1546,7 +1625,7 @@
       <c r="E4" s="1">
         <v>123</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f>$E4/$E7</f>
         <v>0.12058823529411765</v>
       </c>
@@ -1561,7 +1640,7 @@
       <c r="E5" s="1">
         <v>342</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f>$E5/$E7</f>
         <v>0.3352941176470588</v>
       </c>
@@ -1578,22 +1657,22 @@
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>222</v>
-      </c>
-      <c r="C7" s="4">
+        <v>222.0</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10">
+      <c r="E7" s="10" t="n">
         <f>SUM(E2:E6)</f>
-        <v>1020</v>
-      </c>
-      <c r="F7" s="4">
+        <v>1020.0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f>SUM(F2:F6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -1615,9 +1694,9 @@
       <c r="B11" s="1">
         <v>123</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="2" t="n">
         <f>$B11/$B15</f>
-        <v>0.55405405405405406</v>
+        <v>0.5540540540540541</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>35</v>
@@ -1625,7 +1704,7 @@
       <c r="E11" s="1">
         <v>234</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="2" t="n">
         <f>$E11/$E15</f>
         <v>0.20689655172413793</v>
       </c>
@@ -1634,11 +1713,11 @@
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99</v>
-      </c>
-      <c r="C12" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <f>$B12/$B15</f>
         <v>0.44594594594594594</v>
       </c>
@@ -1648,9 +1727,9 @@
       <c r="E12" s="1">
         <v>555</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="2" t="n">
         <f>$E12/$E15</f>
-        <v>0.49071618037135278</v>
+        <v>0.4907161803713528</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1663,7 +1742,7 @@
       <c r="E13" s="1">
         <v>342</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="2" t="n">
         <f>$E13/$E15</f>
         <v>0.30238726790450926</v>
       </c>
@@ -1680,22 +1759,22 @@
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="3" t="n">
         <f>SUM(B11:B14)</f>
-        <v>222</v>
-      </c>
-      <c r="C15" s="4">
+        <v>222.0</v>
+      </c>
+      <c r="C15" s="4" t="n">
         <f>SUM(C11:C14)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="10">
+      <c r="E15" s="10" t="n">
         <f>SUM(E11:E14)</f>
-        <v>1131</v>
-      </c>
-      <c r="F15" s="4">
+        <v>1131.0</v>
+      </c>
+      <c r="F15" s="4" t="n">
         <f>SUM(F11:F14)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -1717,7 +1796,7 @@
       <c r="B19" s="1">
         <v>12</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="2" t="n">
         <f>$B19/$B25</f>
         <v>0.10810810810810811</v>
       </c>
@@ -1727,22 +1806,22 @@
       <c r="E19" s="1">
         <v>23</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="2" t="n">
         <f>$E19/$E25</f>
-        <v>7.5657894736842105E-2</v>
+        <v>0.0756578947368421</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>99</v>
-      </c>
-      <c r="C20" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="C20" s="2" t="n">
         <f>$B20/$B25</f>
-        <v>0.89189189189189189</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>82</v>
@@ -1750,9 +1829,9 @@
       <c r="E20" s="1">
         <v>22</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="2" t="n">
         <f>$E20/$E25</f>
-        <v>7.2368421052631582E-2</v>
+        <v>0.07236842105263158</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1765,9 +1844,9 @@
       <c r="E21" s="1">
         <v>222</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="2" t="n">
         <f>$E21/$E25</f>
-        <v>0.73026315789473684</v>
+        <v>0.7302631578947368</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1780,9 +1859,9 @@
       <c r="E22" s="1">
         <v>3</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="2" t="n">
         <f>$E22/$E25</f>
-        <v>9.8684210526315784E-3</v>
+        <v>0.009868421052631578</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1795,7 +1874,7 @@
       <c r="E23" s="1">
         <v>34</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="2" t="n">
         <f>$E23/$E25</f>
         <v>0.1118421052631579</v>
       </c>
@@ -1812,22 +1891,22 @@
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="3" t="n">
         <f>SUM(B19:B24)</f>
-        <v>111</v>
-      </c>
-      <c r="C25" s="4">
+        <v>111.0</v>
+      </c>
+      <c r="C25" s="4" t="n">
         <f>SUM(C19:C24)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="10">
+      <c r="E25" s="10" t="n">
         <f>SUM(E19:E24)</f>
-        <v>304</v>
-      </c>
-      <c r="F25" s="4">
+        <v>304.0</v>
+      </c>
+      <c r="F25" s="4" t="n">
         <f>SUM(F19:F24)</f>
-        <v>0.99999999999999989</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -1849,7 +1928,7 @@
       <c r="B29" s="1">
         <v>12</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="2" t="n">
         <f>$B29/$B36</f>
         <v>0.10810810810810811</v>
       </c>
@@ -1859,9 +1938,9 @@
       <c r="E29" s="1">
         <v>23</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="2" t="n">
         <f>$E29/$E36</f>
-        <v>6.0052219321148827E-2</v>
+        <v>0.06005221932114883</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1871,9 +1950,9 @@
       <c r="B30" s="16">
         <v>99</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="2" t="n">
         <f>$B30/$B36</f>
-        <v>0.89189189189189189</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>82</v>
@@ -1881,9 +1960,9 @@
       <c r="E30" s="1">
         <v>98</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="2" t="n">
         <f>$E30/$E36</f>
-        <v>0.25587467362924282</v>
+        <v>0.2558746736292428</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1896,7 +1975,7 @@
       <c r="E31" s="1">
         <v>87</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="2" t="n">
         <f>$E31/$E36</f>
         <v>0.22715404699738903</v>
       </c>
@@ -1911,7 +1990,7 @@
       <c r="E32" s="1">
         <v>76</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="2" t="n">
         <f>$E32/$E36</f>
         <v>0.19843342036553524</v>
       </c>
@@ -1926,7 +2005,7 @@
       <c r="E33" s="1">
         <v>65</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="2" t="n">
         <f>$E33/$E36</f>
         <v>0.16971279373368145</v>
       </c>
@@ -1941,9 +2020,9 @@
       <c r="E34" s="1">
         <v>34</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="2" t="n">
         <f>$E34/$E36</f>
-        <v>8.877284595300261E-2</v>
+        <v>0.08877284595300261</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1958,22 +2037,22 @@
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="3" t="n">
         <f>SUM(B29:B35)</f>
-        <v>111</v>
-      </c>
-      <c r="C36" s="4">
+        <v>111.0</v>
+      </c>
+      <c r="C36" s="4" t="n">
         <f>SUM(C29:C35)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="10">
+      <c r="E36" s="10" t="n">
         <f>SUM(E29:E35)</f>
-        <v>383</v>
-      </c>
-      <c r="F36" s="4">
+        <v>383.0</v>
+      </c>
+      <c r="F36" s="4" t="n">
         <f>SUM(F29:F35)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -1995,7 +2074,7 @@
       <c r="B40" s="1">
         <v>12</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="2" t="n">
         <f>$B40/$B48</f>
         <v>0.10810810810810811</v>
       </c>
@@ -2005,9 +2084,9 @@
       <c r="E40" s="1">
         <v>23</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="2" t="n">
         <f>$E40/$E48</f>
-        <v>5.8673469387755105E-2</v>
+        <v>0.058673469387755105</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2017,9 +2096,9 @@
       <c r="B41" s="16">
         <v>99</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="2" t="n">
         <f>$B41/$B48</f>
-        <v>0.89189189189189189</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="D41" s="13" t="s">
         <v>82</v>
@@ -2027,7 +2106,7 @@
       <c r="E41" s="1">
         <v>45</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="2" t="n">
         <f>$E41/$E48</f>
         <v>0.11479591836734694</v>
       </c>
@@ -2042,7 +2121,7 @@
       <c r="E42" s="1">
         <v>56</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="2" t="n">
         <f>$E42/$E48</f>
         <v>0.14285714285714285</v>
       </c>
@@ -2057,7 +2136,7 @@
       <c r="E43" s="1">
         <v>67</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="2" t="n">
         <f>$E43/$E48</f>
         <v>0.17091836734693877</v>
       </c>
@@ -2072,9 +2151,9 @@
       <c r="E44" s="1">
         <v>78</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="2" t="n">
         <f>$E44/$E48</f>
-        <v>0.19897959183673469</v>
+        <v>0.1989795918367347</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2087,7 +2166,7 @@
       <c r="E45" s="1">
         <v>89</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="2" t="n">
         <f>$E45/$E48</f>
         <v>0.22704081632653061</v>
       </c>
@@ -2102,9 +2181,9 @@
       <c r="E46" s="1">
         <v>34</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="2" t="n">
         <f>$E46/$E48</f>
-        <v>8.673469387755102E-2</v>
+        <v>0.08673469387755102</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2119,22 +2198,22 @@
       <c r="A48" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="3" t="n">
         <f>SUM(B40:B47)</f>
-        <v>111</v>
-      </c>
-      <c r="C48" s="4">
+        <v>111.0</v>
+      </c>
+      <c r="C48" s="4" t="n">
         <f>SUM(C40:C47)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D48" s="3"/>
-      <c r="E48" s="10">
+      <c r="E48" s="10" t="n">
         <f>SUM(E40:E47)</f>
-        <v>392</v>
-      </c>
-      <c r="F48" s="4">
+        <v>392.0</v>
+      </c>
+      <c r="F48" s="4" t="n">
         <f>SUM(F40:F47)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -2164,11 +2243,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -2274,25 +2353,25 @@
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="7" t="n">
         <f>SUM(B3:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f>SUM(C3:C5)</f>
-        <v>959</v>
+        <v>959.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="n">
         <f>F4</f>
-        <v>9587290</v>
-      </c>
-      <c r="G6" s="14">
+        <v>9587290.0</v>
+      </c>
+      <c r="G6" s="14" t="n">
         <f>F6</f>
-        <v>9587290</v>
+        <v>9587290.0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2382,9 +2461,9 @@
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="15" t="n">
         <f>SUM(B10:B11)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -2393,13 +2472,13 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="n">
         <f>F10</f>
-        <v>672000</v>
-      </c>
-      <c r="G12" s="14">
+        <v>672000.0</v>
+      </c>
+      <c r="G12" s="14" t="n">
         <f>F12</f>
-        <v>672000</v>
+        <v>672000.0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2468,9 +2547,9 @@
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="n">
         <f>$E17/$E$19</f>
-        <v>0.93449839121420686</v>
+        <v>0.9344983912142069</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -2490,9 +2569,9 @@
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="n">
         <f>$E18/$E$19</f>
-        <v>6.5501608785793169E-2</v>
+        <v>0.06550160878579317</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -2507,9 +2586,9 @@
         <v>40</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="n">
         <f>SUM(E17:E18)</f>
-        <v>10259290</v>
+        <v>1.025929E7</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2523,9 +2602,9 @@
         <v>57</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="9">
+      <c r="E20" s="9" t="n">
         <f>'Mittelverwendung - Mittelherkun'!E7</f>
-        <v>1020</v>
+        <v>1020.0</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -2539,9 +2618,9 @@
         <v>58</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="n">
         <f>E19-E20</f>
-        <v>10258270</v>
+        <v>1.025827E7</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2555,7 +2634,7 @@
         <v>59</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2">
+      <c r="E22" s="2" t="n">
         <f>E21/E20</f>
         <v>10057.127450980392</v>
       </c>
@@ -2639,11 +2718,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2811,20 +2891,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2848,9 +2925,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Flächenwidmung scripting, insert update
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\IdeaProjects\SEPJ\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3D1A93-E4EE-4DF1-977C-76AB0AE3017A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CD493C-B1C2-466C-9033-E253F563F071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28965" yWindow="645" windowWidth="21600" windowHeight="11325" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -303,63 +303,35 @@
     <t>Braumüllergasse 21</t>
   </si>
   <si>
-    <t>IG III = Bauklasse 3</t>
-  </si>
-  <si>
     <t>g = geschlossene Bauweise</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>WGV I = Bauklasse 1</t>
-  </si>
-  <si>
-    <t>WGV III = Bauklasse 3</t>
-  </si>
-  <si>
-    <t>gk = gekuppelte Bauweise</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
+    <t>IG VI = Bauklasse 6 beschränkt auf 30m</t>
+  </si>
+  <si>
+    <t>Ekz = für Einkaufszentren bestimmt</t>
+  </si>
+  <si>
+    <t>Flächenwidmung – laut BWO</t>
+  </si>
+  <si>
+    <t>GB V = Bauklasse 5 beschränkt auf 20m und 60%</t>
+  </si>
+  <si>
+    <t>gk = gekuppelte Bauweise</t>
+  </si>
+  <si>
+    <t>ÖZ = Grundflächen für öffentliche Zwecke (Enteignung möglich)</t>
+  </si>
+  <si>
+    <t>WGV II = Bauklasse 2</t>
+  </si>
+  <si>
     <t>W II = Bauklasse 2</t>
-  </si>
-  <si>
-    <t>W II = Bauklasse 2 beschränkt auf 20%</t>
-  </si>
-  <si>
-    <t>G = Gärtnerische Ausgestaltung</t>
-  </si>
-  <si>
-    <t>ÖZ = Grundflächen für öffentliche Zwecke (Enteignung möglich)</t>
-  </si>
-  <si>
-    <t>WGV II = Bauklasse 2</t>
-  </si>
-  <si>
-    <t>GB II = Bauklasse 2</t>
-  </si>
-  <si>
-    <t>ÖZ = Grundflächen für öffentliche Zwecke (Enteignung möglich)
-Test = test</t>
-  </si>
-  <si>
-    <t>Ekz = für Einkaufszentren</t>
-  </si>
-  <si>
-    <t>Ekz = für Einkaufszentren bestimmt</t>
-  </si>
-  <si>
-    <t>W III = Bauklasse 3</t>
-  </si>
-  <si>
-    <t>o = offene Bauweise</t>
-  </si>
-  <si>
-    <t>GS II = Bauklasse 2</t>
   </si>
 </sst>
 </file>
@@ -543,7 +515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -581,6 +553,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,20 +869,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="50.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>79</v>
       </c>
@@ -926,8 +900,11 @@
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
       <c r="L1" s="27"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O1" s="33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -946,8 +923,11 @@
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O2" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -968,8 +948,11 @@
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O3" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
@@ -991,8 +974,11 @@
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O4" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -1011,8 +997,11 @@
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O5" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1021,7 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
@@ -1052,7 +1041,7 @@
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1059,7 @@
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
@@ -1090,7 +1079,7 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -1106,7 +1095,7 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
@@ -1122,7 +1111,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
@@ -1130,26 +1119,6 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>93</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1168,14 +1137,14 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="31.109375" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
         <v>12</v>
@@ -1194,7 +1163,7 @@
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1219,7 +1188,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -1244,7 +1213,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1269,7 +1238,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1294,7 +1263,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1319,7 +1288,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1346,7 +1315,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1371,7 +1340,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1396,7 +1365,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1419,7 +1388,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1428,7 +1397,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1454,7 +1423,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1465,7 +1434,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1491,7 +1460,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1500,7 +1469,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1509,7 +1478,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1518,7 +1487,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1526,7 +1495,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1544,21 +1513,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C08536-E6A3-4E31-88A7-DF1DE6751CED}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:AL10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="26" max="27" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="29" max="30" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="34" max="35" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="37" max="38" customWidth="true" width="10.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>32</v>
       </c>
@@ -1569,8 +1555,48 @@
       </c>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="30"/>
+      <c r="N1" s="31"/>
+      <c r="Q1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="30"/>
+      <c r="V1" s="31"/>
+      <c r="Y1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="31"/>
+      <c r="AG1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="31"/>
+    </row>
+    <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1591,8 +1617,88 @@
         <f>$E2/$E7</f>
         <v>0.22941176470588234</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1">
+        <v>123</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <f>$J2/$J6</f>
+        <v>0.5540540540540541</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1">
+        <v>234</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <f>$M2/$M6</f>
+        <v>0.20689655172413793</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="1">
+        <v>12</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <f>$R2/$R8</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="1">
+        <v>23</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <f>$U2/$U8</f>
+        <v>0.0756578947368421</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>12</v>
+      </c>
+      <c r="AA2" s="2" t="n">
+        <f>$Z2/$Z9</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>23</v>
+      </c>
+      <c r="AD2" s="2" t="n">
+        <f>$AC2/$AC9</f>
+        <v>0.06005221932114883</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>12</v>
+      </c>
+      <c r="AI2" s="2" t="n">
+        <f>$AH2/$AH10</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>23</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <f>$AK2/$AK10</f>
+        <v>0.058673469387755105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1614,8 +1720,90 @@
         <f>$E3/$E7</f>
         <v>0.31470588235294117</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="16" t="n">
+        <f>Gesamtinvestitionskosten!B10</f>
+        <v>99.0</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <f>$J3/$J6</f>
+        <v>0.44594594594594594</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M3" s="1">
+        <v>555</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <f>$M3/$M6</f>
+        <v>0.4907161803713528</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="16" t="n">
+        <f>Gesamtinvestitionskosten!B10</f>
+        <v>99.0</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <f>$R3/$R8</f>
+        <v>0.8918918918918919</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="U3" s="1">
+        <v>22</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <f>$U3/$U8</f>
+        <v>0.07236842105263158</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" s="16">
+        <v>99</v>
+      </c>
+      <c r="AA3" s="2" t="n">
+        <f>$Z3/$Z9</f>
+        <v>0.8918918918918919</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>98</v>
+      </c>
+      <c r="AD3" s="2" t="n">
+        <f>$AC3/$AC9</f>
+        <v>0.2558746736292428</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH3" s="16">
+        <v>99</v>
+      </c>
+      <c r="AI3" s="2" t="n">
+        <f>$AH3/$AH10</f>
+        <v>0.8918918918918919</v>
+      </c>
+      <c r="AJ3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>45</v>
+      </c>
+      <c r="AL3" s="2" t="n">
+        <f>$AK3/$AK10</f>
+        <v>0.11479591836734694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
@@ -1629,8 +1817,60 @@
         <f>$E4/$E7</f>
         <v>0.12058823529411765</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="1">
+        <v>342</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <f>$M4/$M6</f>
+        <v>0.30238726790450926</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="U4" s="1">
+        <v>222</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <f>$U4/$U8</f>
+        <v>0.7302631578947368</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>87</v>
+      </c>
+      <c r="AD4" s="2" t="n">
+        <f>$AC4/$AC9</f>
+        <v>0.22715404699738903</v>
+      </c>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>56</v>
+      </c>
+      <c r="AL4" s="2" t="n">
+        <f>$AK4/$AK10</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
@@ -1644,16 +1884,120 @@
         <f>$E5/$E7</f>
         <v>0.3352941176470588</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="2"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="U5" s="1">
+        <v>3</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <f>$U5/$U8</f>
+        <v>0.009868421052631578</v>
+      </c>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>76</v>
+      </c>
+      <c r="AD5" s="2" t="n">
+        <f>$AC5/$AC9</f>
+        <v>0.19843342036553524</v>
+      </c>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>67</v>
+      </c>
+      <c r="AL5" s="2" t="n">
+        <f>$AK5/$AK10</f>
+        <v>0.17091836734693877</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <f>SUM(J2:J5)</f>
+        <v>222.0</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <f>SUM(K2:K5)</f>
+        <v>1.0</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="10" t="n">
+        <f>SUM(M2:M5)</f>
+        <v>1131.0</v>
+      </c>
+      <c r="N6" s="4" t="n">
+        <f>SUM(N2:N5)</f>
+        <v>1.0</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="1">
+        <v>34</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <f>$U6/$U8</f>
+        <v>0.1118421052631579</v>
+      </c>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>65</v>
+      </c>
+      <c r="AD6" s="2" t="n">
+        <f>$AC6/$AC9</f>
+        <v>0.16971279373368145</v>
+      </c>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>78</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <f>$AK6/$AK10</f>
+        <v>0.1989795918367347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -1674,560 +2018,142 @@
         <f>SUM(F2:F6)</f>
         <v>1.0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="2"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC7" s="1">
         <v>34</v>
       </c>
-      <c r="B11" s="1">
-        <v>123</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <f>$B11/$B15</f>
-        <v>0.5540540540540541</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1">
-        <v>234</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <f>$E11/$E15</f>
-        <v>0.20689655172413793</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="16" t="n">
-        <f>Gesamtinvestitionskosten!B10</f>
-        <v>99.0</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <f>$B12/$B15</f>
-        <v>0.44594594594594594</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="1">
-        <v>555</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <f>$E12/$E15</f>
-        <v>0.4907161803713528</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1" t="s">
+      <c r="AD7" s="2" t="n">
+        <f>$AC7/$AC9</f>
+        <v>0.08877284595300261</v>
+      </c>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>89</v>
+      </c>
+      <c r="AL7" s="2" t="n">
+        <f>$AK7/$AK10</f>
+        <v>0.22704081632653061</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="3" t="n">
+        <f>SUM(R2:R7)</f>
+        <v>111.0</v>
+      </c>
+      <c r="S8" s="4" t="n">
+        <f>SUM(S2:S7)</f>
+        <v>1.0</v>
+      </c>
+      <c r="T8" s="3"/>
+      <c r="U8" s="10" t="n">
+        <f>SUM(U2:U7)</f>
+        <v>304.0</v>
+      </c>
+      <c r="V8" s="4" t="n">
+        <f>SUM(V2:V7)</f>
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="2"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="1">
-        <v>342</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <f>$E13/$E15</f>
-        <v>0.30238726790450926</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="AK8" s="1">
+        <v>34</v>
+      </c>
+      <c r="AL8" s="2" t="n">
+        <f>$AK8/$AK10</f>
+        <v>0.08673469387755102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3" t="n">
-        <f>SUM(B11:B14)</f>
-        <v>222.0</v>
-      </c>
-      <c r="C15" s="4" t="n">
-        <f>SUM(C11:C14)</f>
+      <c r="Z9" s="3" t="n">
+        <f>SUM(Z2:Z8)</f>
+        <v>111.0</v>
+      </c>
+      <c r="AA9" s="4" t="n">
+        <f>SUM(AA2:AA8)</f>
         <v>1.0</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="10" t="n">
-        <f>SUM(E11:E14)</f>
-        <v>1131.0</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <f>SUM(F11:F14)</f>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="10" t="n">
+        <f>SUM(AC2:AC8)</f>
+        <v>383.0</v>
+      </c>
+      <c r="AD9" s="4" t="n">
+        <f>SUM(AD2:AD8)</f>
         <v>1.0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="1">
-        <v>12</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <f>$B19/$B25</f>
-        <v>0.10810810810810811</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="1">
-        <v>23</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <f>$E19/$E25</f>
-        <v>0.0756578947368421</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="16" t="n">
-        <f>Gesamtinvestitionskosten!B10</f>
-        <v>99.0</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <f>$B20/$B25</f>
-        <v>0.8918918918918919</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="1">
-        <v>22</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <f>$E20/$E25</f>
-        <v>0.07236842105263158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="1">
-        <v>222</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <f>$E21/$E25</f>
-        <v>0.7302631578947368</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="1">
-        <v>3</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <f>$E22/$E25</f>
-        <v>0.009868421052631578</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="1">
-        <v>34</v>
-      </c>
-      <c r="F23" s="2" t="n">
-        <f>$E23/$E25</f>
-        <v>0.1118421052631579</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="2"/>
+    </row>
+    <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="3" t="n">
-        <f>SUM(B19:B24)</f>
+      <c r="AH10" s="3" t="n">
+        <f>SUM(AH2:AH9)</f>
         <v>111.0</v>
       </c>
-      <c r="C25" s="4" t="n">
-        <f>SUM(C19:C24)</f>
+      <c r="AI10" s="4" t="n">
+        <f>SUM(AI2:AI9)</f>
         <v>1.0</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="10" t="n">
-        <f>SUM(E19:E24)</f>
-        <v>304.0</v>
-      </c>
-      <c r="F25" s="4" t="n">
-        <f>SUM(F19:F24)</f>
-        <v>0.9999999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="1">
-        <v>12</v>
-      </c>
-      <c r="C29" s="2" t="n">
-        <f>$B29/$B36</f>
-        <v>0.10810810810810811</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="1">
-        <v>23</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <f>$E29/$E36</f>
-        <v>0.06005221932114883</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="16">
-        <v>99</v>
-      </c>
-      <c r="C30" s="2" t="n">
-        <f>$B30/$B36</f>
-        <v>0.8918918918918919</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="1">
-        <v>98</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <f>$E30/$E36</f>
-        <v>0.2558746736292428</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="1">
-        <v>87</v>
-      </c>
-      <c r="F31" s="2" t="n">
-        <f>$E31/$E36</f>
-        <v>0.22715404699738903</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" s="1">
-        <v>76</v>
-      </c>
-      <c r="F32" s="2" t="n">
-        <f>$E32/$E36</f>
-        <v>0.19843342036553524</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" s="1">
-        <v>65</v>
-      </c>
-      <c r="F33" s="2" t="n">
-        <f>$E33/$E36</f>
-        <v>0.16971279373368145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="1">
-        <v>34</v>
-      </c>
-      <c r="F34" s="2" t="n">
-        <f>$E34/$E36</f>
-        <v>0.08877284595300261</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="3" t="n">
-        <f>SUM(B29:B35)</f>
-        <v>111.0</v>
-      </c>
-      <c r="C36" s="4" t="n">
-        <f>SUM(C29:C35)</f>
-        <v>1.0</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="10" t="n">
-        <f>SUM(E29:E35)</f>
-        <v>383.0</v>
-      </c>
-      <c r="F36" s="4" t="n">
-        <f>SUM(F29:F35)</f>
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="1">
-        <v>12</v>
-      </c>
-      <c r="C40" s="2" t="n">
-        <f>$B40/$B48</f>
-        <v>0.10810810810810811</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40" s="1">
-        <v>23</v>
-      </c>
-      <c r="F40" s="2" t="n">
-        <f>$E40/$E48</f>
-        <v>0.058673469387755105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="16">
-        <v>99</v>
-      </c>
-      <c r="C41" s="2" t="n">
-        <f>$B41/$B48</f>
-        <v>0.8918918918918919</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="1">
-        <v>45</v>
-      </c>
-      <c r="F41" s="2" t="n">
-        <f>$E41/$E48</f>
-        <v>0.11479591836734694</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E42" s="1">
-        <v>56</v>
-      </c>
-      <c r="F42" s="2" t="n">
-        <f>$E42/$E48</f>
-        <v>0.14285714285714285</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" s="1">
-        <v>67</v>
-      </c>
-      <c r="F43" s="2" t="n">
-        <f>$E43/$E48</f>
-        <v>0.17091836734693877</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="1">
-        <v>78</v>
-      </c>
-      <c r="F44" s="2" t="n">
-        <f>$E44/$E48</f>
-        <v>0.1989795918367347</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E45" s="1">
-        <v>89</v>
-      </c>
-      <c r="F45" s="2" t="n">
-        <f>$E45/$E48</f>
-        <v>0.22704081632653061</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E46" s="1">
-        <v>34</v>
-      </c>
-      <c r="F46" s="2" t="n">
-        <f>$E46/$E48</f>
-        <v>0.08673469387755102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" s="3" t="n">
-        <f>SUM(B40:B47)</f>
-        <v>111.0</v>
-      </c>
-      <c r="C48" s="4" t="n">
-        <f>SUM(C40:C47)</f>
-        <v>1.0</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="10" t="n">
-        <f>SUM(E40:E47)</f>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="10" t="n">
+        <f>SUM(AK2:AK9)</f>
         <v>392.0</v>
       </c>
-      <c r="F48" s="4" t="n">
-        <f>SUM(F40:F47)</f>
+      <c r="AL10" s="4" t="n">
+        <f>SUM(AL2:AL9)</f>
         <v>1.0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AD1"/>
+    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="AJ1:AL1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2241,16 +2167,16 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="42.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>41</v>
       </c>
@@ -2273,7 +2199,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
@@ -2290,7 +2216,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
@@ -2309,7 +2235,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -2330,7 +2256,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -2349,7 +2275,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -2376,7 +2302,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2387,7 +2313,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>51</v>
       </c>
@@ -2400,7 +2326,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -2419,7 +2345,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -2438,7 +2364,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -2457,7 +2383,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2483,7 +2409,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2494,7 +2420,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2505,7 +2431,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2516,7 +2442,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="32" t="s">
         <v>52</v>
@@ -2535,7 +2461,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -2557,7 +2483,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -2579,7 +2505,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -2595,7 +2521,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2611,7 +2537,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
@@ -2627,7 +2553,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
@@ -2643,7 +2569,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2654,7 +2580,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2665,7 +2591,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2690,24 +2616,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
- Tabpane funktioniert vollständig - PDf Konvertierungstab im Tabpane - Finanzierungskoten werden auchh im TabPane übertragen
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\IdeaProjects\SEPJ\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C80B610-D632-4F15-8D9E-CF0833C4AC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7FEA1F-0A77-4C20-85B1-CF5EC4D8C785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="2" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="112">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Finanzierungskosten</t>
   </si>
   <si>
-    <t>Fremdkapital Tranche 1 (bis Baubeginn)</t>
-  </si>
-  <si>
-    <t>Fremdkapital Tranche 2 (ab Baubeginn)</t>
-  </si>
-  <si>
     <t>BTVG Erlöse</t>
   </si>
   <si>
@@ -264,27 +258,6 @@
     <t>oihjubjpkojk</t>
   </si>
   <si>
-    <t>ghetto wien</t>
-  </si>
-  <si>
-    <t>Apfelcompany</t>
-  </si>
-  <si>
-    <t>Siehdichvorstrasse 12</t>
-  </si>
-  <si>
-    <t>2231</t>
-  </si>
-  <si>
-    <t>Strasshof</t>
-  </si>
-  <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>nix</t>
-  </si>
-  <si>
     <t>m²</t>
   </si>
   <si>
@@ -304,6 +277,105 @@
   </si>
   <si>
     <t>Fremdkapital Tranche 5</t>
+  </si>
+  <si>
+    <t>Heydari GmbH</t>
+  </si>
+  <si>
+    <t>Höchstädtplatz</t>
+  </si>
+  <si>
+    <t>1090</t>
+  </si>
+  <si>
+    <t>Wien</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>gute Lage</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Immo 42</t>
+  </si>
+  <si>
+    <t>Höchstädtplatz 23</t>
+  </si>
+  <si>
+    <t>1080</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Immo 34</t>
+  </si>
+  <si>
+    <t>In wien</t>
+  </si>
+  <si>
+    <t>240000</t>
+  </si>
+  <si>
+    <t>900</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
   </si>
 </sst>
 </file>
@@ -527,8 +599,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -544,7 +616,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -842,20 +914,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="29.59765625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.265625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.59765625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="25" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -864,60 +936,66 @@
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
       <c r="L1" s="27"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="19" t="s">
+        <v>104</v>
+      </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="C3" s="19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="19" t="s">
+        <v>106</v>
+      </c>
       <c r="C4" s="19" t="str">
         <f>+C3</f>
         <v>m²</v>
@@ -927,118 +1005,130 @@
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="19" t="s">
+        <v>107</v>
+      </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="19" t="s">
+        <v>108</v>
+      </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="19" t="s">
+        <v>95</v>
+      </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="21"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1050,11 +1140,13 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="24" t="s">
+        <v>111</v>
+      </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1066,11 +1158,13 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1089,17 +1183,17 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="31.1328125" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.86328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
         <v>12</v>
@@ -1118,16 +1212,16 @@
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>10.0</v>
+        <v>0.1</v>
       </c>
       <c r="D2" s="18" t="n">
         <f>C2/B2</f>
@@ -1135,215 +1229,215 @@
       </c>
       <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>110.0</v>
+        <v>1.1</v>
       </c>
       <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>0.07136184347104006</v>
+        <v>0.020637898686679177</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>110.0</v>
+        <v>23.0</v>
       </c>
       <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>59.400000000000006</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
-        <v>0.54</v>
+        <v>0.2</v>
       </c>
       <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>169.4</v>
+        <v>27.6</v>
       </c>
       <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.1098972389454017</v>
+        <v>0.5178236397748593</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>120.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
-        <v>64.80000000000001</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="D4" s="6" t="n">
         <f>C4/B4</f>
-        <v>0.5400000000000001</v>
+        <v>0.20000000000000004</v>
       </c>
       <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>184.8</v>
+        <v>3.6</v>
       </c>
       <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.11988789703134732</v>
+        <v>0.0675422138836773</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>130.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>70.2</v>
+        <v>0.8</v>
       </c>
       <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.54</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>200.2</v>
+        <v>4.8</v>
       </c>
       <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.1298785551172929</v>
+        <v>0.0900562851782364</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>140.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>75.60000000000001</v>
+        <v>1.0</v>
       </c>
       <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.54</v>
+        <v>0.2</v>
       </c>
       <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>215.60000000000002</v>
+        <v>6.0</v>
       </c>
       <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.13986921320323853</v>
+        <v>0.11257035647279551</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>150.0</v>
+        <v>3.0</v>
       </c>
       <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>81.0</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.54</v>
+        <v>0.20000000000000004</v>
       </c>
       <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>231.0</v>
+        <v>3.6</v>
       </c>
       <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.14985987128918413</v>
+        <v>0.0675422138836773</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>160.0</v>
+        <v>1.0</v>
       </c>
       <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>86.4</v>
+        <v>0.2</v>
       </c>
       <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.54</v>
+        <v>0.2</v>
       </c>
       <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>246.4</v>
+        <v>1.2</v>
       </c>
       <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.15985052937512975</v>
+        <v>0.0225140712945591</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>76.0</v>
+        <v>2.0</v>
       </c>
       <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>41.040000000000006</v>
+        <v>0.4</v>
       </c>
       <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.54</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>117.04</v>
+        <v>2.4</v>
       </c>
       <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.07592900145318664</v>
+        <v>0.0450281425891182</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="9" t="n">
-        <v>67.0</v>
+        <v>3.0</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>67.0</v>
+        <v>3.0</v>
       </c>
       <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.04346585011417895</v>
+        <v>0.056285178236397754</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1352,33 +1446,33 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>1053.0</v>
+        <v>45.0</v>
       </c>
       <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>488.4400000000001</v>
+        <v>8.3</v>
       </c>
       <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.4638556505223173</v>
+        <v>0.18444444444444447</v>
       </c>
       <c r="E12" s="10" t="n">
         <f>B12+C12</f>
-        <v>1541.44</v>
+        <v>53.3</v>
       </c>
       <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>0.9999999999999999</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1389,33 +1483,33 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>1053.0</v>
+        <v>45.0</v>
       </c>
       <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>488.4400000000001</v>
+        <v>8.3</v>
       </c>
       <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.4638556505223173</v>
+        <v>0.18444444444444447</v>
       </c>
       <c r="E14" s="10" t="n">
         <f>E12</f>
-        <v>1541.44</v>
+        <v>53.3</v>
       </c>
       <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>0.9999999999999999</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1424,7 +1518,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1433,7 +1527,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1442,15 +1536,15 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1471,18 +1565,18 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.59765625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.3984375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="28" t="s">
         <v>32</v>
       </c>
@@ -1494,82 +1588,82 @@
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>123.0</v>
+      <c r="B2" s="1">
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="n">
         <f>$B2/$B7</f>
-        <v>0.6473684210526316</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>234.0</v>
+      <c r="E2" s="1">
+        <v>200</v>
       </c>
       <c r="F2" s="2" t="n">
         <f>$E2/$E7</f>
-        <v>0.22941176470588234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>0.49627791563275436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>67.0</v>
+        <v>3.0</v>
       </c>
       <c r="C3" s="2" t="n">
         <f>$B3/$B7</f>
-        <v>0.3526315789473684</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>321.0</v>
+        <v>76</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="n">
         <f>$E3/$E7</f>
-        <v>0.31470588235294117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>0.0024813895781637717</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
       <c r="D4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>123.0</v>
+        <v>75</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
       </c>
       <c r="F4" s="2" t="n">
         <f>$E4/$E7</f>
-        <v>0.12058823529411765</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.004962779156327543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>342.0</v>
+        <v>37</v>
+      </c>
+      <c r="E5" s="1">
+        <v>200</v>
       </c>
       <c r="F5" s="2" t="n">
         <f>$E5/$E7</f>
-        <v>0.3352941176470588</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.49627791563275436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
@@ -1577,13 +1671,13 @@
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>190.0</v>
+        <v>13.0</v>
       </c>
       <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
@@ -1592,14 +1686,14 @@
       <c r="D7" s="3"/>
       <c r="E7" s="10" t="n">
         <f>SUM(E2:E6)</f>
-        <v>1020.0</v>
+        <v>403.0</v>
       </c>
       <c r="F7" s="4" t="n">
         <f>SUM(F2:F6)</f>
         <v>1.0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="28" t="s">
         <v>32</v>
       </c>
@@ -1611,67 +1705,67 @@
       <c r="E10" s="30"/>
       <c r="F10" s="31"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>123.0</v>
+        <v>56.0</v>
       </c>
       <c r="C11" s="2" t="n">
         <f>$B11/$B15</f>
-        <v>0.6473684210526316</v>
+        <v>0.9491525423728814</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>234.0</v>
+        <v>12.0</v>
       </c>
       <c r="F11" s="2" t="n">
         <f>$E11/$E15</f>
-        <v>0.20689655172413793</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>67.0</v>
+        <v>3.0</v>
       </c>
       <c r="C12" s="2" t="n">
         <f>$B12/$B15</f>
-        <v>0.3526315789473684</v>
+        <v>0.05084745762711865</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>555.0</v>
+        <v>1.0</v>
       </c>
       <c r="F12" s="2" t="n">
         <f>$E12/$E15</f>
-        <v>0.4907161803713528</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.06666666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>342.0</v>
+        <v>2.0</v>
       </c>
       <c r="F13" s="2" t="n">
         <f>$E13/$E15</f>
-        <v>0.30238726790450926</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
@@ -1679,13 +1773,13 @@
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="3" t="n">
         <f>SUM(B11:B14)</f>
-        <v>190.0</v>
+        <v>59.0</v>
       </c>
       <c r="C15" s="4" t="n">
         <f>SUM(C11:C14)</f>
@@ -1694,14 +1788,14 @@
       <c r="D15" s="3"/>
       <c r="E15" s="10" t="n">
         <f>SUM(E11:E14)</f>
-        <v>1131.0</v>
+        <v>15.0</v>
       </c>
       <c r="F15" s="4" t="n">
         <f>SUM(F11:F14)</f>
         <v>1.0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="28" t="s">
         <v>32</v>
       </c>
@@ -1713,97 +1807,97 @@
       <c r="E18" s="30"/>
       <c r="F18" s="31"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1">
-        <v>12</v>
+      <c r="B19" s="1" t="n">
+        <v>10.0</v>
       </c>
       <c r="C19" s="2" t="n">
         <f>$B19/$B25</f>
-        <v>0.1518987341772152</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="1">
-        <v>23</v>
+      <c r="E19" s="1" t="n">
+        <v>200.0</v>
       </c>
       <c r="F19" s="2" t="n">
         <f>$E19/$E25</f>
-        <v>0.0756578947368421</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="16" t="n">
         <f>Gesamtinvestitionskosten!B10</f>
-        <v>67.0</v>
+        <v>3.0</v>
       </c>
       <c r="C20" s="2" t="n">
         <f>$B20/$B25</f>
-        <v>0.8481012658227848</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="1">
-        <v>22</v>
+        <v>76</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>10.0</v>
       </c>
       <c r="F20" s="2" t="n">
         <f>$E20/$E25</f>
-        <v>0.07236842105263158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>0.03571428571428571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" s="1">
-        <v>222</v>
+        <v>75</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>20.0</v>
       </c>
       <c r="F21" s="2" t="n">
         <f>$E21/$E25</f>
-        <v>0.7302631578947368</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>0.07142857142857142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="13" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>3.0</v>
+        <v>30.0</v>
       </c>
       <c r="F22" s="2" t="n">
         <f>$E22/$E25</f>
-        <v>0.009868421052631578</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.10714285714285714</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="1">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>20.0</v>
       </c>
       <c r="F23" s="2" t="n">
         <f>$E23/$E25</f>
-        <v>0.1118421052631579</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.07142857142857142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
@@ -1811,13 +1905,13 @@
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="3" t="n">
         <f>SUM(B19:B24)</f>
-        <v>79.0</v>
+        <v>13.0</v>
       </c>
       <c r="C25" s="4" t="n">
         <f>SUM(C19:C24)</f>
@@ -1826,14 +1920,14 @@
       <c r="D25" s="3"/>
       <c r="E25" s="10" t="n">
         <f>SUM(E19:E24)</f>
-        <v>304.0</v>
+        <v>280.0</v>
       </c>
       <c r="F25" s="4" t="n">
         <f>SUM(F19:F24)</f>
         <v>0.9999999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="28" t="s">
         <v>32</v>
       </c>
@@ -1845,7 +1939,7 @@
       <c r="E28" s="30"/>
       <c r="F28" s="31"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1867,7 +1961,7 @@
         <v>0.06005221932114883</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1879,7 +1973,7 @@
         <v>0.8918918918918919</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E30" s="1">
         <v>98</v>
@@ -1889,12 +1983,12 @@
         <v>0.2558746736292428</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
       <c r="D31" s="13" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E31" s="1">
         <v>87</v>
@@ -1904,12 +1998,12 @@
         <v>0.22715404699738903</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="3"/>
       <c r="D32" s="13" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E32" s="1">
         <v>76</v>
@@ -1919,12 +2013,12 @@
         <v>0.19843342036553524</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="3"/>
       <c r="D33" s="13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E33" s="1">
         <v>65</v>
@@ -1934,12 +2028,12 @@
         <v>0.16971279373368145</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E34" s="1">
         <v>34</v>
@@ -1949,7 +2043,7 @@
         <v>0.08877284595300261</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
@@ -1957,9 +2051,9 @@
       <c r="E35" s="1"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="n">
         <f>SUM(B29:B35)</f>
@@ -1979,7 +2073,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="28" t="s">
         <v>32</v>
       </c>
@@ -1991,7 +2085,7 @@
       <c r="E39" s="30"/>
       <c r="F39" s="31"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -2013,7 +2107,7 @@
         <v>0.058673469387755105</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -2025,7 +2119,7 @@
         <v>0.8918918918918919</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E41" s="1">
         <v>45</v>
@@ -2035,12 +2129,12 @@
         <v>0.11479591836734694</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="13" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E42" s="1">
         <v>56</v>
@@ -2050,12 +2144,12 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="13" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E43" s="1">
         <v>67</v>
@@ -2065,12 +2159,12 @@
         <v>0.17091836734693877</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E44" s="1">
         <v>78</v>
@@ -2080,12 +2174,12 @@
         <v>0.1989795918367347</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="13" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E45" s="1">
         <v>89</v>
@@ -2095,12 +2189,12 @@
         <v>0.22704081632653061</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E46" s="1">
         <v>34</v>
@@ -2110,7 +2204,7 @@
         <v>0.08673469387755102</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
@@ -2118,9 +2212,9 @@
       <c r="E47" s="1"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B48" s="3" t="n">
         <f>SUM(B40:B47)</f>
@@ -2162,44 +2256,44 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="42.86328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.1328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.86328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.1328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2214,9 +2308,9 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2233,9 +2327,9 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="15">
         <v>1</v>
@@ -2254,9 +2348,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -2273,9 +2367,9 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="7" t="n">
         <f>SUM(B3:B5)</f>
@@ -2300,7 +2394,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2311,9 +2405,9 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2324,9 +2418,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2343,9 +2437,9 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
@@ -2362,9 +2456,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
@@ -2381,9 +2475,9 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="15" t="n">
         <f>SUM(B10:B11)</f>
@@ -2407,7 +2501,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2418,7 +2512,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2429,7 +2523,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2440,33 +2534,33 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
       <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17" s="1">
         <v>9587290</v>
@@ -2481,14 +2575,14 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1">
         <v>672000</v>
@@ -2503,11 +2597,11 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="3" t="n">
@@ -2519,55 +2613,55 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="9" t="n">
         <f>'Mittelverwendung - Mittelherkun'!E7</f>
-        <v>1020.0</v>
+        <v>403.0</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="3" t="n">
         <f>E19-E20</f>
-        <v>1.025827E7</v>
+        <v>1.0258887E7</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2" t="n">
         <f>E21/E20</f>
-        <v>10057.127450980392</v>
+        <v>25456.2952853598</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2578,7 +2672,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2589,7 +2683,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2614,26 +2708,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2642,12 +2736,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2815,17 +2908,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2849,11 +2945,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- ExecutiveSummary teilweise fertig - Daten werden übergeben - Widmungsdaten über Eventbus übergeben
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A9075B-6F4F-4DE4-AEF9-027F8D78E3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E039F596-EB4B-4057-B418-5883AC714C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="2" activeTab="3" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Finanzierungskosten</t>
   </si>
   <si>
-    <t>Fremdkapital Tranche 1 (bis Baubeginn)</t>
-  </si>
-  <si>
-    <t>Fremdkapital Tranche 2 (ab Baubeginn)</t>
-  </si>
-  <si>
     <t>BTVG Erlöse</t>
   </si>
   <si>
@@ -261,18 +255,6 @@
     <t>Lage der Öffi Anbindung</t>
   </si>
   <si>
-    <t>ghetto wien</t>
-  </si>
-  <si>
-    <t>Apfelcompany</t>
-  </si>
-  <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>nix</t>
-  </si>
-  <si>
     <t>m²</t>
   </si>
   <si>
@@ -295,12 +277,6 @@
   </si>
   <si>
     <t>Flächenwidmung – laut BWO</t>
-  </si>
-  <si>
-    <t>W II = Bauklasse 2</t>
-  </si>
-  <si>
-    <t>Braumüllergasse 21</t>
   </si>
   <si>
     <t>gk = gekuppelte Bauweise</t>
@@ -314,6 +290,45 @@
   <si>
     <t xml:space="preserve">
 </t>
+  </si>
+  <si>
+    <t>Hallo</t>
+  </si>
+  <si>
+    <t>1080</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>Strozzigasse 26</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>W III = Bauklasse 3 beschränkt auf 20%</t>
   </si>
 </sst>
 </file>
@@ -862,12 +877,12 @@
     <col min="1" max="1" width="29.53125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="25.33203125" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="24.53125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="50.796875" customWidth="1"/>
+    <col min="15" max="15" width="50.796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="26" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -876,69 +891,75 @@
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
       <c r="K1" s="27"/>
       <c r="L1" s="28"/>
       <c r="O1" s="25" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
       <c r="O2" s="19" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="C3" s="19" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
       <c r="O3" s="19" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="19" t="s">
+        <v>93</v>
+      </c>
       <c r="C4" s="19" t="str">
         <f>+C3</f>
         <v>m²</v>
@@ -948,56 +969,60 @@
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="23">
-        <v>1210</v>
+        <v>65</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
       <c r="O4" s="19" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
       <c r="O5" s="19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
@@ -1007,17 +1032,19 @@
       <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="19" t="s">
+        <v>90</v>
+      </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
@@ -1027,14 +1054,16 @@
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="19" t="s">
+        <v>94</v>
+      </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
@@ -1045,17 +1074,19 @@
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="21"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
@@ -1065,7 +1096,9 @@
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="19" t="s">
+        <v>90</v>
+      </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1081,7 +1114,9 @@
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="24" t="s">
+        <v>90</v>
+      </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1097,7 +1132,9 @@
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1150,23 +1187,23 @@
         <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3">
         <f>B2*B21</f>
-        <v>1.1000000000000001</v>
+        <v>1.44</v>
       </c>
       <c r="D2" s="18">
         <f>C2/B2</f>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="E2" s="3">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>12.1</v>
+        <v>13.44</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>2.1113243761996161E-2</v>
+        <v>2.562391565461097E-2</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1175,23 +1212,23 @@
         <v>18</v>
       </c>
       <c r="B3" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>4.4000000000000004</v>
+        <v>9.89</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
-        <v>0.2</v>
+        <v>0.43000000000000005</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" si="0"/>
-        <v>26.4</v>
+        <v>32.89</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" si="1"/>
-        <v>4.6065259117082528E-2</v>
+        <v>6.270614478274962E-2</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1200,23 +1237,23 @@
         <v>19</v>
       </c>
       <c r="B4" s="1">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3">
         <f>B4*$B$20</f>
-        <v>6.6000000000000005</v>
+        <v>5.16</v>
       </c>
       <c r="D4" s="6">
         <f>C4/B4</f>
-        <v>0.2</v>
+        <v>0.43</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
-        <v>39.6</v>
+        <v>17.16</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="1"/>
-        <v>6.9097888675623803E-2</v>
+        <v>3.2716249451869364E-2</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1225,23 +1262,23 @@
         <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>44</v>
+        <v>233</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
+        <v>100.19</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.43</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>52.8</v>
+        <v>333.19</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>9.2130518234165057E-2</v>
+        <v>0.63524051019046346</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1250,23 +1287,23 @@
         <v>21</v>
       </c>
       <c r="B6" s="1">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>5.16</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.43</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>17.16</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="1"/>
-        <v>0.11516314779270632</v>
+        <v>3.2716249451869364E-2</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1275,23 +1312,23 @@
         <v>22</v>
       </c>
       <c r="B7" s="1">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="2"/>
-        <v>13.200000000000001</v>
+        <v>9.89</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.43000000000000005</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>79.2</v>
+        <v>32.89</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>0.13819577735124761</v>
+        <v>6.270614478274962E-2</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1300,23 +1337,23 @@
         <v>23</v>
       </c>
       <c r="B8" s="1">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="2"/>
-        <v>15.4</v>
+        <v>9.89</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.43000000000000005</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>92.4</v>
+        <v>32.89</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>0.16122840690978887</v>
+        <v>6.270614478274962E-2</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1325,23 +1362,23 @@
         <v>24</v>
       </c>
       <c r="B9" s="1">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="2"/>
-        <v>17.600000000000001</v>
+        <v>9.89</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.43000000000000005</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>105.6</v>
+        <v>32.89</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>0.18426103646833011</v>
+        <v>6.270614478274962E-2</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1350,21 +1387,21 @@
         <v>25</v>
       </c>
       <c r="B10" s="9">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>0.17274472168905949</v>
+        <v>2.2878496120188368E-2</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1383,23 +1420,23 @@
       </c>
       <c r="B12" s="3">
         <f>SUM(B2:B10)</f>
-        <v>495</v>
+        <v>373</v>
       </c>
       <c r="C12" s="3">
         <f>SUM(C2:C10)</f>
-        <v>78.099999999999994</v>
+        <v>151.51</v>
       </c>
       <c r="D12" s="4">
         <f>C12/B12</f>
-        <v>0.15777777777777777</v>
+        <v>0.40619302949061659</v>
       </c>
       <c r="E12" s="10">
         <f>B12+C12</f>
-        <v>573.1</v>
+        <v>524.51</v>
       </c>
       <c r="F12" s="4">
         <f>SUM(F2:F10)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1420,23 +1457,23 @@
       </c>
       <c r="B14" s="3">
         <f>B12</f>
-        <v>495</v>
+        <v>373</v>
       </c>
       <c r="C14" s="3">
         <f>C12</f>
-        <v>78.099999999999994</v>
+        <v>151.51</v>
       </c>
       <c r="D14" s="3">
         <f>D12</f>
-        <v>0.15777777777777777</v>
+        <v>0.40619302949061659</v>
       </c>
       <c r="E14" s="10">
         <f>E12</f>
-        <v>573.1</v>
+        <v>524.51</v>
       </c>
       <c r="F14" s="4">
         <f>F12</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1472,7 +1509,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="11">
-        <v>0.2</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1480,7 +1517,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="12">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -1504,24 +1541,23 @@
     <col min="1" max="1" width="20.796875" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="10.796875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.796875" customWidth="1"/>
-    <col min="9" max="9" width="20.796875" customWidth="1"/>
-    <col min="10" max="11" width="10.796875" customWidth="1"/>
-    <col min="12" max="12" width="20.796875" customWidth="1"/>
-    <col min="13" max="14" width="10.796875" customWidth="1"/>
-    <col min="17" max="17" width="20.796875" customWidth="1"/>
-    <col min="18" max="19" width="10.796875" customWidth="1"/>
-    <col min="20" max="20" width="20.796875" customWidth="1"/>
-    <col min="21" max="22" width="10.796875" customWidth="1"/>
-    <col min="25" max="25" width="20.796875" customWidth="1"/>
-    <col min="26" max="27" width="10.796875" customWidth="1"/>
-    <col min="28" max="28" width="20.796875" customWidth="1"/>
-    <col min="29" max="30" width="10.796875" customWidth="1"/>
-    <col min="33" max="33" width="20.796875" customWidth="1"/>
-    <col min="34" max="35" width="10.796875" customWidth="1"/>
-    <col min="36" max="36" width="20.796875" customWidth="1"/>
-    <col min="37" max="38" width="10.796875" customWidth="1"/>
+    <col min="5" max="6" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.796875" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="20.796875" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.796875" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="20.796875" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.796875" customWidth="1" collapsed="1"/>
+    <col min="26" max="27" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="20.796875" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="20.796875" customWidth="1" collapsed="1"/>
+    <col min="34" max="35" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="20.796875" customWidth="1" collapsed="1"/>
+    <col min="37" max="38" width="10.796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1581,21 +1617,21 @@
         <v>34</v>
       </c>
       <c r="B2" s="1">
-        <v>123</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <f>$B2/$B7</f>
-        <v>0.55405405405405406</v>
+        <v>9.1743119266055051E-2</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E2" s="1">
-        <v>234</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2">
         <f>$E2/$E7</f>
-        <v>0.22941176470588234</v>
+        <v>0.24489795918367346</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>34</v>
@@ -1687,17 +1723,17 @@
       </c>
       <c r="C3" s="2">
         <f>$B3/$B7</f>
-        <v>0.44594594594594594</v>
+        <v>0.90825688073394495</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1">
-        <v>321</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2">
         <f>$E3/$E7</f>
-        <v>0.31470588235294117</v>
+        <v>0.24489795918367346</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
@@ -1710,7 +1746,7 @@
         <v>0.44594594594594594</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="M3" s="1">
         <v>555</v>
@@ -1730,7 +1766,7 @@
         <v>0.89189189189189189</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="U3" s="1">
         <v>22</v>
@@ -1750,7 +1786,7 @@
         <v>0.89189189189189189</v>
       </c>
       <c r="AB3" s="13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AC3" s="1">
         <v>98</v>
@@ -1770,7 +1806,7 @@
         <v>0.89189189189189189</v>
       </c>
       <c r="AJ3" s="13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AK3" s="1">
         <v>45</v>
@@ -1785,20 +1821,20 @@
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
       <c r="D4" s="13" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="E4" s="1">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2">
         <f>$E4/$E7</f>
-        <v>0.12058823529411765</v>
+        <v>0.24489795918367346</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="3"/>
       <c r="L4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M4" s="1">
         <v>342</v>
@@ -1811,7 +1847,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="3"/>
       <c r="T4" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="U4" s="1">
         <v>222</v>
@@ -1824,7 +1860,7 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AC4" s="1">
         <v>87</v>
@@ -1837,7 +1873,7 @@
       <c r="AH4" s="1"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AK4" s="1">
         <v>56</v>
@@ -1852,14 +1888,14 @@
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1">
-        <v>342</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2">
         <f>$E5/$E7</f>
-        <v>0.3352941176470588</v>
+        <v>0.26530612244897961</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1871,7 +1907,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="3"/>
       <c r="T5" s="13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="U5" s="1">
         <v>3</v>
@@ -1884,7 +1920,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AC5" s="1">
         <v>76</v>
@@ -1897,7 +1933,7 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AK5" s="1">
         <v>67</v>
@@ -1915,7 +1951,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="I6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J6" s="3">
         <f>SUM(J2:J5)</f>
@@ -1938,7 +1974,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="3"/>
       <c r="T6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U6" s="1">
         <v>34</v>
@@ -1951,7 +1987,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AC6" s="1">
         <v>65</v>
@@ -1964,7 +2000,7 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AK6" s="1">
         <v>78</v>
@@ -1976,11 +2012,11 @@
     </row>
     <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3">
         <f>SUM(B2:B6)</f>
-        <v>222</v>
+        <v>109</v>
       </c>
       <c r="C7" s="4">
         <f>SUM(C2:C6)</f>
@@ -1989,7 +2025,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="10">
         <f>SUM(E2:E6)</f>
-        <v>1020</v>
+        <v>49</v>
       </c>
       <c r="F7" s="4">
         <f>SUM(F2:F6)</f>
@@ -2005,7 +2041,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AC7" s="1">
         <v>34</v>
@@ -2018,7 +2054,7 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AK7" s="1">
         <v>89</v>
@@ -2030,7 +2066,7 @@
     </row>
     <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="Q8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R8" s="3">
         <f>SUM(R2:R7)</f>
@@ -2059,7 +2095,7 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AK8" s="1">
         <v>34</v>
@@ -2071,7 +2107,7 @@
     </row>
     <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="Y9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Z9" s="3">
         <f>SUM(Z2:Z8)</f>
@@ -2099,7 +2135,7 @@
     </row>
     <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AG10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AH10" s="3">
         <f>SUM(AH2:AH9)</f>
@@ -2141,7 +2177,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2155,30 +2191,30 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2195,7 +2231,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2214,7 +2250,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="15">
         <v>1</v>
@@ -2235,7 +2271,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -2254,7 +2290,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="7">
         <f>SUM(B3:B5)</f>
@@ -2292,7 +2328,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2305,7 +2341,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2324,7 +2360,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
@@ -2343,7 +2379,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
@@ -2362,7 +2398,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="15">
         <f>SUM(B10:B11)</f>
@@ -2422,18 +2458,18 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
       <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2442,10 +2478,10 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17" s="1">
         <v>9587290</v>
@@ -2464,10 +2500,10 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1">
         <v>672000</v>
@@ -2486,7 +2522,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="3">
@@ -2502,7 +2538,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="9">
@@ -2517,7 +2553,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="3">
@@ -2533,7 +2569,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2">
@@ -2596,22 +2632,22 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2620,23 +2656,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -2800,31 +2819,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2840,4 +2852,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Tranchenanpassung in der PDF je nach Wahl - Finanzierungskosten und Adresse in MVMH Contrroller und WidmungController angepasst
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="112">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -341,6 +341,42 @@
   </si>
   <si>
     <t>Tranche</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>WGV II = Bauklasse 2 beschränkt auf 20%</t>
+  </si>
+  <si>
+    <t>ÖZ = Grundflächen für öffentliche Zwecke (Enteignung möglich)</t>
+  </si>
+  <si>
+    <t>G = Gärtnerische Ausgestaltung</t>
+  </si>
+  <si>
+    <t>Piaristengasse</t>
+  </si>
+  <si>
+    <t>Piaristengasse 4</t>
+  </si>
+  <si>
+    <t>u4</t>
+  </si>
+  <si>
+    <t>Juliastraße 10</t>
   </si>
 </sst>
 </file>
@@ -893,10 +929,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.53125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.53125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="50.796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.53125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.53125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="50.796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -925,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -942,11 +978,11 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
       <c r="O2" s="19" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="P2" t="str">
         <f>LEFT(O2,SEARCH("=",O2)-2)</f>
-        <v>W III</v>
+        <v>WGV II</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
@@ -954,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>71</v>
@@ -967,7 +1003,7 @@
         <v>64</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
@@ -985,7 +1021,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C4" s="19" t="str">
         <f>+C3</f>
@@ -1005,19 +1041,19 @@
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
       <c r="O4" s="19" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="P4" s="26" t="str">
         <f>CONCATENATE(P2," ",P3)</f>
-        <v>W III gk</v>
+        <v>WGV II gk</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19">
-        <v>7</v>
+      <c r="B5" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -1034,7 +1070,7 @@
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
       <c r="O5" s="19" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
@@ -1042,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -1065,7 +1101,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -1076,7 +1112,7 @@
         <v>68</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
@@ -1088,7 +1124,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -1109,7 +1145,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1132,7 +1168,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -1150,7 +1186,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -1168,7 +1204,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1193,9 +1229,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.86328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.1328125" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -1221,24 +1257,24 @@
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <f>B2*B21</f>
-        <v>0.1</v>
-      </c>
-      <c r="D2" s="18">
+        <v>1.44</v>
+      </c>
+      <c r="D2" s="18" t="n">
         <f>C2/B2</f>
-        <v>0.1</v>
-      </c>
-      <c r="E2" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F2" s="2">
+        <v>13.44</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>1.1593591905564925E-2</v>
+        <v>0.036226415094339624</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1246,24 +1282,24 @@
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="1" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
-        <v>0.04</v>
-      </c>
-      <c r="D3" s="6">
+        <v>7.82</v>
+      </c>
+      <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
-        <v>0.02</v>
-      </c>
-      <c r="E3" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>2.04</v>
-      </c>
-      <c r="F3" s="2">
+        <v>41.82</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>2.1500843170320406E-2</v>
+        <v>0.11272237196765499</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1271,24 +1307,24 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
-        <v>0.06</v>
-      </c>
-      <c r="D4" s="6">
+        <v>2.7600000000000002</v>
+      </c>
+      <c r="D4" s="6" t="n">
         <f>C4/B4</f>
-        <v>0.02</v>
-      </c>
-      <c r="E4" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>3.06</v>
-      </c>
-      <c r="F4" s="2">
+        <v>14.76</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>3.225126475548061E-2</v>
+        <v>0.039784366576819406</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1296,24 +1332,24 @@
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="1" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>0.08</v>
-      </c>
-      <c r="D5" s="6">
+        <v>7.82</v>
+      </c>
+      <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="E5" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>4.08</v>
-      </c>
-      <c r="F5" s="2">
+        <v>41.82</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>4.3001686340640811E-2</v>
+        <v>0.11272237196765499</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1321,24 +1357,24 @@
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="D6" s="6">
+        <v>2.7600000000000002</v>
+      </c>
+      <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="E6" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="F6" s="2">
+        <v>14.76</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>5.3752107925801013E-2</v>
+        <v>0.039784366576819406</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1346,24 +1382,24 @@
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1">
-        <v>67</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="1" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>1.34</v>
-      </c>
-      <c r="D7" s="6">
+        <v>7.82</v>
+      </c>
+      <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="E7" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>68.34</v>
-      </c>
-      <c r="F7" s="2">
+        <v>41.82</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.72027824620573366</v>
+        <v>0.11272237196765499</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1371,24 +1407,24 @@
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="1" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D8" s="6">
+        <v>28.290000000000003</v>
+      </c>
+      <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="E8" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>7.14</v>
-      </c>
-      <c r="F8" s="2">
+        <v>151.29</v>
+      </c>
+      <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>7.5252951096121415E-2</v>
+        <v>0.4077897574123989</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1396,24 +1432,24 @@
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B9" s="1" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>0.02</v>
-      </c>
-      <c r="D9" s="6">
+        <v>5.29</v>
+      </c>
+      <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="E9" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>1.02</v>
-      </c>
-      <c r="F9" s="2">
+        <v>28.29</v>
+      </c>
+      <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.0750421585160203E-2</v>
+        <v>0.07625336927223719</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1421,22 +1457,22 @@
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="9">
-        <v>3</v>
+      <c r="B10" s="9" t="n">
+        <v>23.0</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
-      <c r="D10" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="6" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F10" s="2">
+        <v>23.0</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>3.1618887015177066E-2</v>
+        <v>0.06199460916442048</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1453,25 +1489,25 @@
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>93</v>
-      </c>
-      <c r="C12" s="3">
+        <v>307.0</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
-        <v>1.8800000000000003</v>
-      </c>
-      <c r="D12" s="4">
+        <v>64.00000000000001</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>2.0215053763440863E-2</v>
-      </c>
-      <c r="E12" s="10">
+        <v>0.20846905537459287</v>
+      </c>
+      <c r="E12" s="10" t="n">
         <f>B12+C12</f>
-        <v>94.88</v>
-      </c>
-      <c r="F12" s="4">
+        <v>371.0</v>
+      </c>
+      <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1490,25 +1526,25 @@
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>93</v>
-      </c>
-      <c r="C14" s="3">
+        <v>307.0</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <f>C12</f>
-        <v>1.8800000000000003</v>
-      </c>
-      <c r="D14" s="3">
+        <v>64.00000000000001</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>2.0215053763440863E-2</v>
-      </c>
-      <c r="E14" s="10">
+        <v>0.20846905537459287</v>
+      </c>
+      <c r="E14" s="10" t="n">
         <f>E12</f>
-        <v>94.88</v>
-      </c>
-      <c r="F14" s="4">
+        <v>371.0</v>
+      </c>
+      <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1543,16 +1579,16 @@
       <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="11">
-        <v>0.02</v>
+      <c r="B20" s="11" t="n">
+        <v>0.23</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="12">
-        <v>0.1</v>
+      <c r="B21" s="12" t="n">
+        <v>0.12</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -1573,26 +1609,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="37" max="38" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="26" max="27" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="29" max="30" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="34" max="35" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="37" max="38" customWidth="true" width="10.796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1651,22 +1687,22 @@
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <f>$B2/$B7</f>
-        <v>9.1743119266055051E-2</v>
+        <v>0.09174311926605505</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="1" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <f>$E2/$E7</f>
-        <v>0.24489795918367346</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>34</v>
@@ -1674,9 +1710,9 @@
       <c r="J2" s="1">
         <v>123</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="2" t="n">
         <f>$J2/$J6</f>
-        <v>0.55405405405405406</v>
+        <v>0.5540540540540541</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>35</v>
@@ -1684,69 +1720,69 @@
       <c r="M2" s="1">
         <v>234</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="2" t="n">
         <f>$M2/$M6</f>
         <v>0.20689655172413793</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="1">
-        <v>12</v>
-      </c>
-      <c r="S2" s="2">
+      <c r="R2" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="S2" s="2" t="n">
         <f>$R2/$R8</f>
-        <v>0.10810810810810811</v>
+        <v>0.019801980198019802</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="1">
-        <v>23</v>
-      </c>
-      <c r="V2" s="2">
+      <c r="U2" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V2" s="2" t="n">
         <f>$U2/$U8</f>
-        <v>7.5657894736842105E-2</v>
+        <v>0.012345679012345678</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="1">
-        <v>12</v>
-      </c>
-      <c r="AA2" s="2">
+      <c r="Z2" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="AA2" s="2" t="n">
         <f>$Z2/$Z9</f>
-        <v>0.10810810810810811</v>
+        <v>0.09174311926605505</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" s="1">
-        <v>23</v>
-      </c>
-      <c r="AD2" s="2">
+      <c r="AC2" s="1" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="AD2" s="2" t="n">
         <f>$AC2/$AC9</f>
-        <v>6.0052219321148827E-2</v>
+        <v>0.37735849056603776</v>
       </c>
       <c r="AG2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="1">
-        <v>12</v>
-      </c>
-      <c r="AI2" s="2">
+      <c r="AH2" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AI2" s="2" t="n">
         <f>$AH2/$AH10</f>
-        <v>0.10810810810810811</v>
+        <v>0.01</v>
       </c>
       <c r="AJ2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK2" s="1">
-        <v>23</v>
-      </c>
-      <c r="AL2" s="2">
+      <c r="AK2" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AL2" s="2" t="n">
         <f>$AK2/$AK10</f>
-        <v>5.8673469387755105E-2</v>
+        <v>0.011428571428571429</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1756,19 +1792,19 @@
       <c r="B3" s="16">
         <v>99</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <f>$B3/$B7</f>
-        <v>0.90825688073394495</v>
+        <v>0.908256880733945</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="1">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <f>$E3/$E7</f>
-        <v>0.24489795918367346</v>
+        <v>0.02857142857142857</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
@@ -1776,7 +1812,7 @@
       <c r="J3" s="16">
         <v>99</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="2" t="n">
         <f>$J3/$J6</f>
         <v>0.44594594594594594</v>
       </c>
@@ -1786,9 +1822,9 @@
       <c r="M3" s="1">
         <v>555</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="2" t="n">
         <f>$M3/$M6</f>
-        <v>0.49071618037135278</v>
+        <v>0.4907161803713528</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>36</v>
@@ -1796,19 +1832,19 @@
       <c r="R3" s="16">
         <v>99</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="2" t="n">
         <f>$R3/$R8</f>
-        <v>0.89189189189189189</v>
+        <v>0.9801980198019802</v>
       </c>
       <c r="T3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="U3" s="1">
-        <v>22</v>
-      </c>
-      <c r="V3" s="2">
+      <c r="U3" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="V3" s="2" t="n">
         <f>$U3/$U8</f>
-        <v>7.2368421052631582E-2</v>
+        <v>0.12345679012345678</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>36</v>
@@ -1816,19 +1852,19 @@
       <c r="Z3" s="16">
         <v>99</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3" s="2" t="n">
         <f>$Z3/$Z9</f>
-        <v>0.89189189189189189</v>
+        <v>0.908256880733945</v>
       </c>
       <c r="AB3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AC3" s="1">
-        <v>98</v>
-      </c>
-      <c r="AD3" s="2">
+      <c r="AC3" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AD3" s="2" t="n">
         <f>$AC3/$AC9</f>
-        <v>0.25587467362924282</v>
+        <v>0.018867924528301886</v>
       </c>
       <c r="AG3" s="1" t="s">
         <v>36</v>
@@ -1836,19 +1872,19 @@
       <c r="AH3" s="16">
         <v>99</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AI3" s="2" t="n">
         <f>$AH3/$AH10</f>
-        <v>0.89189189189189189</v>
+        <v>0.99</v>
       </c>
       <c r="AJ3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AK3" s="1">
-        <v>45</v>
-      </c>
-      <c r="AL3" s="2">
+      <c r="AK3" s="1" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="AL3" s="2" t="n">
         <f>$AK3/$AK10</f>
-        <v>0.11479591836734694</v>
+        <v>0.13142857142857142</v>
       </c>
     </row>
     <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1858,12 +1894,12 @@
       <c r="D4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="1">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f>$E4/$E7</f>
-        <v>0.24489795918367346</v>
+        <v>0.05714285714285714</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1874,7 +1910,7 @@
       <c r="M4" s="1">
         <v>342</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="2" t="n">
         <f>$M4/$M6</f>
         <v>0.30238726790450926</v>
       </c>
@@ -1884,12 +1920,12 @@
       <c r="T4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="U4" s="1">
-        <v>222</v>
-      </c>
-      <c r="V4" s="2">
+      <c r="U4" s="1" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="V4" s="2" t="n">
         <f>$U4/$U8</f>
-        <v>0.73026315789473684</v>
+        <v>0.2839506172839506</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
@@ -1897,12 +1933,12 @@
       <c r="AB4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="AC4" s="1">
-        <v>87</v>
-      </c>
-      <c r="AD4" s="2">
+      <c r="AC4" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AD4" s="2" t="n">
         <f>$AC4/$AC9</f>
-        <v>0.22715404699738903</v>
+        <v>0.03773584905660377</v>
       </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
@@ -1910,12 +1946,12 @@
       <c r="AJ4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="AK4" s="1">
-        <v>56</v>
-      </c>
-      <c r="AL4" s="2">
+      <c r="AK4" s="1" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AL4" s="2" t="n">
         <f>$AK4/$AK10</f>
-        <v>0.14285714285714285</v>
+        <v>0.19428571428571428</v>
       </c>
     </row>
     <row r="5" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1925,12 +1961,12 @@
       <c r="D5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="1">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <f>$E5/$E7</f>
-        <v>0.26530612244897961</v>
+        <v>0.34285714285714286</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1944,12 +1980,12 @@
       <c r="T5" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="U5" s="1">
-        <v>3</v>
-      </c>
-      <c r="V5" s="2">
+      <c r="U5" s="1" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="V5" s="2" t="n">
         <f>$U5/$U8</f>
-        <v>9.8684210526315784E-3</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -1957,12 +1993,12 @@
       <c r="AB5" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="1">
-        <v>76</v>
-      </c>
-      <c r="AD5" s="2">
+      <c r="AC5" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="AD5" s="2" t="n">
         <f>$AC5/$AC9</f>
-        <v>0.19843342036553524</v>
+        <v>0.05660377358490566</v>
       </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
@@ -1970,12 +2006,12 @@
       <c r="AJ5" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="AK5" s="1">
-        <v>67</v>
-      </c>
-      <c r="AL5" s="2">
+      <c r="AK5" s="1" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="AL5" s="2" t="n">
         <f>$AK5/$AK10</f>
-        <v>0.17091836734693877</v>
+        <v>0.5085714285714286</v>
       </c>
     </row>
     <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1988,22 +2024,22 @@
       <c r="I6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="3" t="n">
         <f>SUM(J2:J5)</f>
-        <v>222</v>
-      </c>
-      <c r="K6" s="4">
+        <v>222.0</v>
+      </c>
+      <c r="K6" s="4" t="n">
         <f>SUM(K2:K5)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="10">
+      <c r="M6" s="10" t="n">
         <f>SUM(M2:M5)</f>
-        <v>1131</v>
-      </c>
-      <c r="N6" s="4">
+        <v>1131.0</v>
+      </c>
+      <c r="N6" s="4" t="n">
         <f>SUM(N2:N5)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -2011,12 +2047,12 @@
       <c r="T6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="1">
-        <v>34</v>
-      </c>
-      <c r="V6" s="2">
+      <c r="U6" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V6" s="2" t="n">
         <f>$U6/$U8</f>
-        <v>0.1118421052631579</v>
+        <v>0.024691358024691357</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
@@ -2024,12 +2060,12 @@
       <c r="AB6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AC6" s="1">
-        <v>65</v>
-      </c>
-      <c r="AD6" s="2">
+      <c r="AC6" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="AD6" s="2" t="n">
         <f>$AC6/$AC9</f>
-        <v>0.16971279373368145</v>
+        <v>0.07547169811320754</v>
       </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
@@ -2037,34 +2073,34 @@
       <c r="AJ6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AK6" s="1">
-        <v>78</v>
-      </c>
-      <c r="AL6" s="2">
+      <c r="AK6" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="AL6" s="2" t="n">
         <f>$AK6/$AK10</f>
-        <v>0.19897959183673469</v>
+        <v>0.06857142857142857</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>109</v>
-      </c>
-      <c r="C7" s="4">
+        <v>109.0</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10">
+      <c r="E7" s="10" t="n">
         <f>SUM(E2:E6)</f>
-        <v>49</v>
-      </c>
-      <c r="F7" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f>SUM(F2:F6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -2078,12 +2114,12 @@
       <c r="AB7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AC7" s="1">
-        <v>34</v>
-      </c>
-      <c r="AD7" s="2">
+      <c r="AC7" s="1" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="AD7" s="2" t="n">
         <f>$AC7/$AC9</f>
-        <v>8.877284595300261E-2</v>
+        <v>0.4339622641509434</v>
       </c>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
@@ -2091,34 +2127,34 @@
       <c r="AJ7" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="AK7" s="1">
-        <v>89</v>
-      </c>
-      <c r="AL7" s="2">
+      <c r="AK7" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="AL7" s="2" t="n">
         <f>$AK7/$AK10</f>
-        <v>0.22704081632653061</v>
+        <v>0.06857142857142857</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="Q8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="3" t="n">
         <f>SUM(R2:R7)</f>
-        <v>111</v>
-      </c>
-      <c r="S8" s="4">
+        <v>101.0</v>
+      </c>
+      <c r="S8" s="4" t="n">
         <f>SUM(S2:S7)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="T8" s="3"/>
-      <c r="U8" s="10">
+      <c r="U8" s="10" t="n">
         <f>SUM(U2:U7)</f>
-        <v>304</v>
-      </c>
-      <c r="V8" s="4">
+        <v>81.0</v>
+      </c>
+      <c r="V8" s="4" t="n">
         <f>SUM(V2:V7)</f>
-        <v>0.99999999999999989</v>
+        <v>1.0</v>
       </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
@@ -2132,34 +2168,34 @@
       <c r="AJ8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AK8" s="1">
-        <v>34</v>
-      </c>
-      <c r="AL8" s="2">
+      <c r="AK8" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="AL8" s="2" t="n">
         <f>$AK8/$AK10</f>
-        <v>8.673469387755102E-2</v>
+        <v>0.017142857142857144</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="Y9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z9" s="3">
+      <c r="Z9" s="3" t="n">
         <f>SUM(Z2:Z8)</f>
-        <v>111</v>
-      </c>
-      <c r="AA9" s="4">
+        <v>109.0</v>
+      </c>
+      <c r="AA9" s="4" t="n">
         <f>SUM(AA2:AA8)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AB9" s="3"/>
-      <c r="AC9" s="10">
+      <c r="AC9" s="10" t="n">
         <f>SUM(AC2:AC8)</f>
-        <v>383</v>
-      </c>
-      <c r="AD9" s="4">
+        <v>53.0</v>
+      </c>
+      <c r="AD9" s="4" t="n">
         <f>SUM(AD2:AD8)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
@@ -2172,29 +2208,31 @@
       <c r="AG10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH10" s="3">
+      <c r="AH10" s="3" t="n">
         <f>SUM(AH2:AH9)</f>
-        <v>111</v>
-      </c>
-      <c r="AI10" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="AI10" s="4" t="n">
         <f>SUM(AI2:AI9)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AJ10" s="3"/>
-      <c r="AK10" s="10">
+      <c r="AK10" s="10" t="n">
         <f>SUM(AK2:AK9)</f>
-        <v>392</v>
-      </c>
-      <c r="AL10" s="4">
+        <v>175.0</v>
+      </c>
+      <c r="AL10" s="4" t="n">
         <f>SUM(AL2:AL9)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.45">
       <c r="G11" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2223,11 +2261,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.86328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.86328125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.1328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.86328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.1328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.86328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -2280,12 +2318,12 @@
       <c r="E3" s="1">
         <v>9091</v>
       </c>
-      <c r="F3" s="16">
-        <v>10000</v>
+      <c r="F3" s="16" t="n">
+        <v>125.0</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="17">
-        <v>10909</v>
+      <c r="H3" s="17" t="n">
+        <v>12.0</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -2293,8 +2331,8 @@
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="15">
-        <v>1</v>
+      <c r="B4" s="15" t="n">
+        <v>35.0</v>
       </c>
       <c r="C4" s="1">
         <v>959</v>
@@ -2314,8 +2352,8 @@
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="15">
-        <v>0</v>
+      <c r="B5" s="15" t="n">
+        <v>12.0</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -2333,25 +2371,25 @@
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="7" t="n">
         <f>SUM(B3:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f>SUM(C3:C5)</f>
-        <v>959</v>
+        <v>959.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="n">
         <f>F4</f>
-        <v>9587290</v>
-      </c>
-      <c r="G6" s="14">
+        <v>9587290.0</v>
+      </c>
+      <c r="G6" s="14" t="n">
         <f>F6</f>
-        <v>9587290</v>
+        <v>9587290.0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2390,12 +2428,12 @@
       <c r="E9" s="1">
         <v>38182</v>
       </c>
-      <c r="F9" s="1">
-        <v>42000</v>
+      <c r="F9" s="1" t="n">
+        <v>34.0</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="14">
-        <v>45818</v>
+      <c r="H9" s="14" t="n">
+        <v>12.0</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -2406,8 +2444,8 @@
       <c r="B10" s="15">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
-        <v>16</v>
+      <c r="C10" s="1" t="n">
+        <v>12.0</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2425,8 +2463,8 @@
       <c r="B11" s="15">
         <v>0</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
+      <c r="C11" s="1" t="n">
+        <v>34.0</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
@@ -2441,9 +2479,9 @@
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="15" t="n">
         <f>SUM(B10:B11)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -2452,13 +2490,13 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="n">
         <f>F10</f>
-        <v>672000</v>
-      </c>
-      <c r="G12" s="14">
+        <v>672000.0</v>
+      </c>
+      <c r="G12" s="14" t="n">
         <f>F12</f>
-        <v>672000</v>
+        <v>672000.0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2527,9 +2565,9 @@
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="n">
         <f>$E17/$E$19</f>
-        <v>0.93449839121420686</v>
+        <v>0.9344983912142069</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -2549,9 +2587,9 @@
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="n">
         <f>$E18/$E$19</f>
-        <v>6.5501608785793169E-2</v>
+        <v>0.06550160878579317</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -2566,9 +2604,9 @@
         <v>38</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="n">
         <f>SUM(E17:E18)</f>
-        <v>10259290</v>
+        <v>1.025929E7</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2597,9 +2635,9 @@
         <v>56</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="n">
         <f>E19-E20</f>
-        <v>10258270</v>
+        <v>1.025827E7</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2613,7 +2651,7 @@
         <v>57</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2">
+      <c r="E22" s="2" t="n">
         <f>E21/E20</f>
         <v>10057.127450980392</v>
       </c>

</xml_diff>

<commit_message>
frontend von stammdaten und basisinformationen hübsch gemacht
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43677\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E039F596-EB4B-4057-B418-5883AC714C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E464CF6-7819-4582-AD72-0A9BF217D649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="2" activeTab="3" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="100">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Garagenstellplätze</t>
   </si>
   <si>
-    <t>GIK</t>
-  </si>
-  <si>
     <t>Prognostozierter Verkaufserlös</t>
   </si>
   <si>
@@ -243,16 +240,10 @@
     <t>Ort</t>
   </si>
   <si>
-    <t xml:space="preserve">Entfernung zur Schule </t>
-  </si>
-  <si>
     <t>Lagebeschreibung</t>
   </si>
   <si>
     <t xml:space="preserve">Maps - Bild </t>
-  </si>
-  <si>
-    <t>Lage der Öffi Anbindung</t>
   </si>
   <si>
     <t>m²</t>
@@ -292,43 +283,64 @@
 </t>
   </si>
   <si>
-    <t>Hallo</t>
-  </si>
-  <si>
-    <t>1080</t>
+    <t>W III = Bauklasse 3 beschränkt auf 20%</t>
+  </si>
+  <si>
+    <t>Öffi-Anbindung</t>
+  </si>
+  <si>
+    <t>Außenfläche</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Unteres Belvedere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1100 </t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>Strozzigasse 26</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>23</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>neueoeffi</t>
+  </si>
+  <si>
+    <t>fdsfsdf</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>W III = Bauklasse 3 beschränkt auf 20%</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -512,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -537,7 +549,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -553,8 +564,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,7 +581,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -868,45 +879,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.53125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.53125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="50.796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.54296875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.36328125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.54296875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="50.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+    <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
-      <c r="H1" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
-      <c r="O1" s="25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="H1" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
+      <c r="O1" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -914,51 +925,51 @@
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
       <c r="O2" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
       <c r="O3" s="19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C4" s="19" t="str">
         <f>+C3</f>
@@ -969,19 +980,19 @@
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>84</v>
+        <v>64</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
       <c r="O4" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -994,24 +1005,24 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
       <c r="O5" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -1019,21 +1030,21 @@
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>85</v>
+        <v>66</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -1041,21 +1052,19 @@
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>86</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -1063,38 +1072,36 @@
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="19"/>
+        <v>81</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="21"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>88</v>
-      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>90</v>
@@ -1110,16 +1117,16 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A11" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="19"/>
@@ -1128,12 +1135,12 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1156,235 +1163,235 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.86328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.08984375" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>12</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="3" t="n">
         <f>B2*B21</f>
         <v>1.44</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="18" t="n">
         <f>C2/B2</f>
         <v>0.12</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <f t="shared" ref="E2:E10" si="0">B2+C2</f>
         <v>13.44</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
-        <v>2.562391565461097E-2</v>
+        <v>0.02562391565461097</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>23</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="3" t="n">
         <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
         <v>9.89</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="6" t="n">
         <f t="shared" ref="D3:D9" si="3">C3/B3</f>
         <v>0.43000000000000005</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="n">
         <f t="shared" si="0"/>
         <v>32.89</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>6.270614478274962E-2</v>
+        <v>0.06270614478274962</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="3" t="n">
         <f>B4*$B$20</f>
         <v>5.16</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="6" t="n">
         <f>C4/B4</f>
         <v>0.43</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
         <v>17.16</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>3.2716249451869364E-2</v>
+        <v>0.032716249451869364</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
         <v>233</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <f t="shared" si="2"/>
         <v>100.19</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.43</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
         <v>333.19</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.63524051019046346</v>
+        <v>0.6352405101904635</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
         <v>5.16</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.43</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
         <v>17.16</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>3.2716249451869364E-2</v>
+        <v>0.032716249451869364</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>23</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
         <v>9.89</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.43000000000000005</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
         <v>32.89</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>6.270614478274962E-2</v>
+        <v>0.06270614478274962</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>23</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
         <v>9.89</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.43000000000000005</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
         <v>32.89</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>6.270614478274962E-2</v>
+        <v>0.06270614478274962</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
         <v>23</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
         <v>9.89</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
         <v>0.43000000000000005</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
         <v>32.89</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>6.270614478274962E-2</v>
+        <v>0.06270614478274962</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="9">
         <v>12</v>
@@ -1395,17 +1402,17 @@
       <c r="D10" s="6">
         <v>0.12</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F10" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>2.2878496120188368E-2</v>
+        <v>0.022878496120188368</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1414,35 +1421,35 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="3">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="n">
         <f>SUM(B2:B10)</f>
-        <v>373</v>
-      </c>
-      <c r="C12" s="3">
+        <v>373.0</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <f>SUM(C2:C10)</f>
         <v>151.51</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="4" t="n">
         <f>C12/B12</f>
-        <v>0.40619302949061659</v>
-      </c>
-      <c r="E12" s="10">
+        <v>0.4061930294906166</v>
+      </c>
+      <c r="E12" s="10" t="n">
         <f>B12+C12</f>
         <v>524.51</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="4" t="n">
         <f>SUM(F2:F10)</f>
-        <v>0.99999999999999989</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1451,33 +1458,33 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="3">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="n">
         <f>B12</f>
-        <v>373</v>
-      </c>
-      <c r="C14" s="3">
+        <v>373.0</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <f>C12</f>
         <v>151.51</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="3" t="n">
         <f>D12</f>
-        <v>0.40619302949061659</v>
-      </c>
-      <c r="E14" s="10">
+        <v>0.4061930294906166</v>
+      </c>
+      <c r="E14" s="10" t="n">
         <f>E12</f>
         <v>524.51</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="4" t="n">
         <f>F12</f>
-        <v>0.99999999999999989</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1486,7 +1493,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1495,7 +1502,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1504,23 +1511,23 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="11">
         <v>0.43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="12">
         <v>0.12</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1536,297 +1543,297 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="10.796875" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="20.796875" customWidth="1" collapsed="1"/>
-    <col min="37" max="38" width="10.796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="26" max="27" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="29" max="30" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="34" max="35" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="37" max="38" customWidth="true" width="10.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="I1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="30"/>
+      <c r="N1" s="31"/>
+      <c r="Q1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="30"/>
+      <c r="V1" s="31"/>
+      <c r="Y1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="31"/>
+      <c r="AG1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="31"/>
+    </row>
+    <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32"/>
-      <c r="I1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="32"/>
-      <c r="Q1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="32"/>
-      <c r="Y1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="32"/>
-      <c r="AG1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="32"/>
-    </row>
-    <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B2" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <f>$B2/$B7</f>
-        <v>9.1743119266055051E-2</v>
+        <v>0.09174311926605505</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1">
         <v>12</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <f>$E2/$E7</f>
         <v>0.24489795918367346</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1">
         <v>123</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="2" t="n">
         <f>$J2/$J6</f>
-        <v>0.55405405405405406</v>
+        <v>0.5540540540540541</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" s="1">
         <v>234</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="2" t="n">
         <f>$M2/$M6</f>
         <v>0.20689655172413793</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R2" s="1">
         <v>12</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="2" t="n">
         <f>$R2/$R8</f>
         <v>0.10810810810810811</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U2" s="1">
         <v>23</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="2" t="n">
         <f>$U2/$U8</f>
-        <v>7.5657894736842105E-2</v>
+        <v>0.0756578947368421</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z2" s="1">
         <v>12</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="2" t="n">
         <f>$Z2/$Z9</f>
         <v>0.10810810810810811</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC2" s="1">
         <v>23</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="2" t="n">
         <f>$AC2/$AC9</f>
-        <v>6.0052219321148827E-2</v>
+        <v>0.06005221932114883</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH2" s="1">
         <v>12</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AI2" s="2" t="n">
         <f>$AH2/$AH10</f>
         <v>0.10810810810810811</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AK2" s="1">
         <v>23</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="AL2" s="2" t="n">
         <f>$AK2/$AK10</f>
-        <v>5.8673469387755105E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+        <v>0.058673469387755105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="16">
         <v>99</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <f>$B3/$B7</f>
-        <v>0.90825688073394495</v>
+        <v>0.908256880733945</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E3" s="1">
         <v>12</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f>$E3/$E7</f>
         <v>0.24489795918367346</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="16">
         <v>99</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="2" t="n">
         <f>$J3/$J6</f>
         <v>0.44594594594594594</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M3" s="1">
         <v>555</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="2" t="n">
         <f>$M3/$M6</f>
-        <v>0.49071618037135278</v>
+        <v>0.4907161803713528</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R3" s="16">
         <v>99</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="2" t="n">
         <f>$R3/$R8</f>
-        <v>0.89189189189189189</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U3" s="1">
         <v>22</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3" s="2" t="n">
         <f>$U3/$U8</f>
-        <v>7.2368421052631582E-2</v>
+        <v>0.07236842105263158</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z3" s="16">
         <v>99</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3" s="2" t="n">
         <f>$Z3/$Z9</f>
-        <v>0.89189189189189189</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="AB3" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AC3" s="1">
         <v>98</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AD3" s="2" t="n">
         <f>$AC3/$AC9</f>
-        <v>0.25587467362924282</v>
+        <v>0.2558746736292428</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH3" s="16">
         <v>99</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AI3" s="2" t="n">
         <f>$AH3/$AH10</f>
-        <v>0.89189189189189189</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="AJ3" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AK3" s="1">
         <v>45</v>
       </c>
-      <c r="AL3" s="2">
+      <c r="AL3" s="2" t="n">
         <f>$AK3/$AK10</f>
         <v>0.11479591836734694</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
       <c r="D4" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1">
         <v>12</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f>$E4/$E7</f>
         <v>0.24489795918367346</v>
       </c>
@@ -1834,12 +1841,12 @@
       <c r="J4" s="1"/>
       <c r="K4" s="3"/>
       <c r="L4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="1">
         <v>342</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="2" t="n">
         <f>$M4/$M6</f>
         <v>0.30238726790450926</v>
       </c>
@@ -1847,25 +1854,25 @@
       <c r="R4" s="1"/>
       <c r="S4" s="3"/>
       <c r="T4" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="U4" s="1">
         <v>222</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="2" t="n">
         <f>$U4/$U8</f>
-        <v>0.73026315789473684</v>
+        <v>0.7302631578947368</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AC4" s="1">
         <v>87</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD4" s="2" t="n">
         <f>$AC4/$AC9</f>
         <v>0.22715404699738903</v>
       </c>
@@ -1873,29 +1880,29 @@
       <c r="AH4" s="1"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AK4" s="1">
         <v>56</v>
       </c>
-      <c r="AL4" s="2">
+      <c r="AL4" s="2" t="n">
         <f>$AK4/$AK10</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1">
         <v>13</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f>$E5/$E7</f>
-        <v>0.26530612244897961</v>
+        <v>0.2653061224489796</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1907,25 +1914,25 @@
       <c r="R5" s="1"/>
       <c r="S5" s="3"/>
       <c r="T5" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="U5" s="1">
         <v>3</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="2" t="n">
         <f>$U5/$U8</f>
-        <v>9.8684210526315784E-3</v>
+        <v>0.009868421052631578</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AC5" s="1">
         <v>76</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5" s="2" t="n">
         <f>$AC5/$AC9</f>
         <v>0.19843342036553524</v>
       </c>
@@ -1933,17 +1940,17 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AK5" s="1">
         <v>67</v>
       </c>
-      <c r="AL5" s="2">
+      <c r="AL5" s="2" t="n">
         <f>$AK5/$AK10</f>
         <v>0.17091836734693877</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
@@ -1951,35 +1958,35 @@
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="I6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="3">
+        <v>37</v>
+      </c>
+      <c r="J6" s="3" t="n">
         <f>SUM(J2:J5)</f>
-        <v>222</v>
-      </c>
-      <c r="K6" s="4">
+        <v>222.0</v>
+      </c>
+      <c r="K6" s="4" t="n">
         <f>SUM(K2:K5)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="10">
+      <c r="M6" s="10" t="n">
         <f>SUM(M2:M5)</f>
-        <v>1131</v>
-      </c>
-      <c r="N6" s="4">
+        <v>1131.0</v>
+      </c>
+      <c r="N6" s="4" t="n">
         <f>SUM(N2:N5)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="3"/>
       <c r="T6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U6" s="1">
         <v>34</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6" s="2" t="n">
         <f>$U6/$U8</f>
         <v>0.1118421052631579</v>
       </c>
@@ -1987,12 +1994,12 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AC6" s="1">
         <v>65</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD6" s="2" t="n">
         <f>$AC6/$AC9</f>
         <v>0.16971279373368145</v>
       </c>
@@ -2000,36 +2007,36 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AK6" s="1">
         <v>78</v>
       </c>
-      <c r="AL6" s="2">
+      <c r="AL6" s="2" t="n">
         <f>$AK6/$AK10</f>
-        <v>0.19897959183673469</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+        <v>0.1989795918367347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="3">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="n">
         <f>SUM(B2:B6)</f>
-        <v>109</v>
-      </c>
-      <c r="C7" s="4">
+        <v>109.0</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <f>SUM(C2:C6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10">
+      <c r="E7" s="10" t="n">
         <f>SUM(E2:E6)</f>
-        <v>49</v>
-      </c>
-      <c r="F7" s="4">
+        <v>49.0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f>SUM(F2:F6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -2041,49 +2048,49 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC7" s="1">
         <v>34</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AD7" s="2" t="n">
         <f>$AC7/$AC9</f>
-        <v>8.877284595300261E-2</v>
+        <v>0.08877284595300261</v>
       </c>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AK7" s="1">
         <v>89</v>
       </c>
-      <c r="AL7" s="2">
+      <c r="AL7" s="2" t="n">
         <f>$AK7/$AK10</f>
         <v>0.22704081632653061</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Q8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R8" s="3">
+        <v>37</v>
+      </c>
+      <c r="R8" s="3" t="n">
         <f>SUM(R2:R7)</f>
-        <v>111</v>
-      </c>
-      <c r="S8" s="4">
+        <v>111.0</v>
+      </c>
+      <c r="S8" s="4" t="n">
         <f>SUM(S2:S7)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="T8" s="3"/>
-      <c r="U8" s="10">
+      <c r="U8" s="10" t="n">
         <f>SUM(U2:U7)</f>
-        <v>304</v>
-      </c>
-      <c r="V8" s="4">
+        <v>304.0</v>
+      </c>
+      <c r="V8" s="4" t="n">
         <f>SUM(V2:V7)</f>
-        <v>0.99999999999999989</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
@@ -2095,36 +2102,36 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AK8" s="1">
         <v>34</v>
       </c>
-      <c r="AL8" s="2">
+      <c r="AL8" s="2" t="n">
         <f>$AK8/$AK10</f>
-        <v>8.673469387755102E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+        <v>0.08673469387755102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Y9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z9" s="3">
+        <v>37</v>
+      </c>
+      <c r="Z9" s="3" t="n">
         <f>SUM(Z2:Z8)</f>
-        <v>111</v>
-      </c>
-      <c r="AA9" s="4">
+        <v>111.0</v>
+      </c>
+      <c r="AA9" s="4" t="n">
         <f>SUM(AA2:AA8)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AB9" s="3"/>
-      <c r="AC9" s="10">
+      <c r="AC9" s="10" t="n">
         <f>SUM(AC2:AC8)</f>
-        <v>383</v>
-      </c>
-      <c r="AD9" s="4">
+        <v>383.0</v>
+      </c>
+      <c r="AD9" s="4" t="n">
         <f>SUM(AD2:AD8)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
@@ -2133,26 +2140,26 @@
       <c r="AK9" s="1"/>
       <c r="AL9" s="2"/>
     </row>
-    <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AG10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH10" s="3">
+        <v>37</v>
+      </c>
+      <c r="AH10" s="3" t="n">
         <f>SUM(AH2:AH9)</f>
-        <v>111</v>
-      </c>
-      <c r="AI10" s="4">
+        <v>111.0</v>
+      </c>
+      <c r="AI10" s="4" t="n">
         <f>SUM(AI2:AI9)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AJ10" s="3"/>
-      <c r="AK10" s="10">
+      <c r="AK10" s="10" t="n">
         <f>SUM(AK2:AK9)</f>
-        <v>392</v>
-      </c>
-      <c r="AL10" s="4">
+        <v>392.0</v>
+      </c>
+      <c r="AL10" s="4" t="n">
         <f>SUM(AL2:AL9)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -2176,45 +2183,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB0A179-3460-4B7F-B6A0-F84428E1F30B}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.86328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.86328125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.1328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.81640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.08984375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.81640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.08984375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2229,9 +2236,9 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2248,9 +2255,9 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="15">
         <v>1</v>
@@ -2269,9 +2276,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -2288,34 +2295,34 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="7">
+        <v>37</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <f>SUM(B3:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f>SUM(C3:C5)</f>
-        <v>959</v>
+        <v>959.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="n">
         <f>F4</f>
-        <v>9587290</v>
-      </c>
-      <c r="G6" s="14">
+        <v>9587290.0</v>
+      </c>
+      <c r="G6" s="14" t="n">
         <f>F6</f>
-        <v>9587290</v>
+        <v>9587290.0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2326,9 +2333,9 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2339,9 +2346,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2358,9 +2365,9 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
@@ -2377,9 +2384,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
@@ -2396,13 +2403,13 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="15">
+        <v>37</v>
+      </c>
+      <c r="B12" s="15" t="n">
         <f>SUM(B10:B11)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C12" s="1">
         <v>16</v>
@@ -2411,18 +2418,18 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="n">
         <f>F10</f>
-        <v>672000</v>
-      </c>
-      <c r="G12" s="14">
+        <v>672000.0</v>
+      </c>
+      <c r="G12" s="14" t="n">
         <f>F12</f>
-        <v>672000</v>
+        <v>672000.0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2433,7 +2440,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2444,7 +2451,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2455,40 +2462,40 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1">
         <v>9587290</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="n">
         <f>$E17/$E$19</f>
-        <v>0.93449839121420686</v>
+        <v>0.9344983912142069</v>
       </c>
       <c r="G17" s="1">
         <v>10000</v>
@@ -2496,21 +2503,21 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="1">
         <v>672000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="n">
         <f>$E18/$E$19</f>
-        <v>6.5501608785793169E-2</v>
+        <v>0.06550160878579317</v>
       </c>
       <c r="G18" s="1">
         <v>42000</v>
@@ -2518,27 +2525,27 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="n">
         <f>SUM(E17:E18)</f>
-        <v>10259290</v>
+        <v>1.025929E7</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="9">
@@ -2549,30 +2556,30 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="n">
         <f>E19-E20</f>
-        <v>10258270</v>
+        <v>1.025827E7</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2">
+      <c r="E22" s="2" t="n">
         <f>E21/E20</f>
         <v>10057.127450980392</v>
       </c>
@@ -2581,7 +2588,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2592,7 +2599,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2603,7 +2610,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2628,26 +2635,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wire Rows noch einmal angepasst, Exceltabelle angepasst
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\OneDrive\Dokumente\Technikum\WS23\SEPRJ\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AA2C01E-D2B1-47C1-9178-97C5F878A561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5FDD44-6126-4812-88C8-F29F256213C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="675" yWindow="2062" windowWidth="13583" windowHeight="9308" firstSheet="3" activeTab="3" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Basisinformation" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="108">
   <si>
     <t>Kaufpreis</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>Braumüllergasse 21</t>
+  </si>
+  <si>
+    <t>Gesamtinvestitionskosten</t>
+  </si>
+  <si>
+    <t>Mittelverwendung und Mittelherkunft</t>
   </si>
 </sst>
 </file>
@@ -471,7 +477,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -544,12 +550,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -589,10 +604,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -608,9 +624,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -648,7 +664,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -754,7 +770,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -896,7 +912,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -906,19 +922,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B9F7DB-AB41-497D-B306-2E29F3117BD9}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.53125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.53125" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="50.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="27" t="s">
         <v>72</v>
       </c>
@@ -939,7 +955,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -968,7 +984,7 @@
         <v>W II</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -999,7 +1015,7 @@
         <v>gk</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
@@ -1031,7 +1047,7 @@
         <v>W II gk</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1072,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
@@ -1079,7 +1095,7 @@
       <c r="L6" s="19"/>
       <c r="O6" s="19"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
@@ -1102,7 +1118,7 @@
       <c r="L7" s="19"/>
       <c r="O7" s="19"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
@@ -1125,7 +1141,7 @@
       <c r="L8" s="19"/>
       <c r="O8" s="19"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
@@ -1148,7 +1164,7 @@
       <c r="L9" s="19"/>
       <c r="O9" s="19"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -1166,7 +1182,7 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
@@ -1184,7 +1200,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
@@ -1206,148 +1222,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57066AFC-3CC1-4339-B554-0D5829A53635}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.86328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>12</v>
       </c>
-      <c r="C2" s="3">
-        <f>B2*B21</f>
+      <c r="C3" s="3">
+        <f>B3*B22</f>
         <v>1.44</v>
       </c>
-      <c r="D2" s="18">
-        <f>C2/B2</f>
+      <c r="D3" s="18">
+        <f>C3/B3</f>
         <v>0.12</v>
       </c>
-      <c r="E2" s="3">
-        <f t="shared" ref="E2:E10" si="0">B2+C2</f>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E11" si="0">B3+C3</f>
         <v>13.44</v>
       </c>
-      <c r="F2" s="2">
-        <f t="shared" ref="F2:F10" si="1">$E2/$E$14</f>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F11" si="1">$E3/$E$15</f>
         <v>3.6226415094339624E-2</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>34</v>
       </c>
-      <c r="C3" s="3">
-        <f t="shared" ref="C3:C9" si="2">B3*$B$20</f>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C10" si="2">B4*$B$21</f>
         <v>7.82</v>
       </c>
-      <c r="D3" s="6">
-        <f t="shared" ref="D3:D9" si="3">C3/B3</f>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:D10" si="3">C4/B4</f>
         <v>0.23</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>41.82</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F4" s="2">
         <f t="shared" si="1"/>
         <v>0.11272237196765499</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>12</v>
       </c>
-      <c r="C4" s="3">
-        <f>B4*$B$20</f>
+      <c r="C5" s="3">
+        <f>B5*$B$21</f>
         <v>2.7600000000000002</v>
       </c>
-      <c r="D4" s="6">
-        <f>C4/B4</f>
+      <c r="D5" s="6">
+        <f>C5/B5</f>
         <v>0.23</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>14.76</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
         <v>3.9784366576819406E-2</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>34</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <f t="shared" si="2"/>
         <v>7.82</v>
-      </c>
-      <c r="D5" s="6">
-        <f t="shared" si="3"/>
-        <v>0.23</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="0"/>
-        <v>41.82</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.11272237196765499</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3">
-        <f t="shared" si="2"/>
-        <v>2.7600000000000002</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="3"/>
@@ -1355,24 +1357,24 @@
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>14.76</v>
+        <v>41.82</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="1"/>
-        <v>3.9784366576819406E-2</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.11272237196765499</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="2"/>
-        <v>7.82</v>
+        <v>2.7600000000000002</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="3"/>
@@ -1380,24 +1382,24 @@
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>41.82</v>
+        <v>14.76</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>0.11272237196765499</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9784366576819406E-2</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="2"/>
-        <v>28.290000000000003</v>
+        <v>7.82</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="3"/>
@@ -1405,24 +1407,24 @@
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>151.29</v>
+        <v>41.82</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>0.40778975741239892</v>
+        <v>0.11272237196765499</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="2"/>
-        <v>5.29</v>
+        <v>28.290000000000003</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="3"/>
@@ -1430,119 +1432,135 @@
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>28.29</v>
+        <v>151.29</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>7.6253369272237193E-2</v>
+        <v>0.40778975741239892</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="9">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1">
         <v>23</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5.29</v>
       </c>
       <c r="D10" s="6">
-        <v>0.12</v>
+        <f t="shared" si="3"/>
+        <v>0.23</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>28.29</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
+        <v>7.6253369272237193E-2</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="9">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
         <v>6.1994609164420483E-2</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3">
-        <f>SUM(B2:B10)</f>
+      <c r="B13" s="3">
+        <f>SUM(B3:B11)</f>
         <v>307</v>
       </c>
-      <c r="C12" s="3">
-        <f>SUM(C2:C10)</f>
+      <c r="C13" s="3">
+        <f>SUM(C3:C11)</f>
         <v>64.000000000000014</v>
       </c>
-      <c r="D12" s="4">
-        <f>C12/B12</f>
+      <c r="D13" s="4">
+        <f>C13/B13</f>
         <v>0.20846905537459287</v>
       </c>
-      <c r="E12" s="10">
-        <f>B12+C12</f>
+      <c r="E13" s="10">
+        <f>B13+C13</f>
         <v>371</v>
       </c>
-      <c r="F12" s="4">
-        <f>SUM(F2:F10)</f>
+      <c r="F13" s="4">
+        <f>SUM(F3:F11)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3">
-        <f>B12</f>
+      <c r="B15" s="3">
+        <f>B13</f>
         <v>307</v>
       </c>
-      <c r="C14" s="3">
-        <f>C12</f>
+      <c r="C15" s="3">
+        <f>C13</f>
         <v>64.000000000000014</v>
       </c>
-      <c r="D14" s="3">
-        <f>D12</f>
+      <c r="D15" s="3">
+        <f>D13</f>
         <v>0.20846905537459287</v>
       </c>
-      <c r="E14" s="10">
-        <f>E12</f>
+      <c r="E15" s="10">
+        <f>E13</f>
         <v>371</v>
       </c>
-      <c r="F14" s="4">
-        <f>F12</f>
+      <c r="F15" s="4">
+        <f>F13</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1551,7 +1569,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1560,39 +1578,51 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B21" s="11">
         <v>0.23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B22" s="12">
         <v>0.12</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C08536-E6A3-4E31-88A7-DF1DE6751CED}">
-  <dimension ref="A1:AL11"/>
+  <dimension ref="A1:AL12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1:AL1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
@@ -1616,621 +1646,668 @@
     <col min="37" max="38" width="10.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.45">
+      <c r="A1" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="I1" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="Q1" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="Y1" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AG1" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+    </row>
+    <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33"/>
-      <c r="I1" s="30" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="I2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31" t="s">
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
-      <c r="Q1" s="30" t="s">
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
+      <c r="Q2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="31" t="s">
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
-      <c r="Y1" s="30" t="s">
+      <c r="U2" s="32"/>
+      <c r="V2" s="33"/>
+      <c r="Y2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="31" t="s">
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="33"/>
-      <c r="AG1" s="30" t="s">
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="33"/>
+      <c r="AG2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="31" t="s">
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="33"/>
-    </row>
-    <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="33"/>
+    </row>
+    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
-        <f>$B2/$B7</f>
+      <c r="C3" s="2">
+        <f>$B3/$B8</f>
         <v>9.1743119266055051E-2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="1">
         <v>20</v>
       </c>
-      <c r="F2" s="2">
-        <f>$E2/$E7</f>
+      <c r="F3" s="2">
+        <f>$E3/$E8</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J3" s="1">
         <v>123</v>
       </c>
-      <c r="K2" s="2">
-        <f>$J2/$J6</f>
+      <c r="K3" s="2">
+        <f>$J3/$J7</f>
         <v>0.55405405405405406</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M3" s="1">
         <v>234</v>
       </c>
-      <c r="N2" s="2">
-        <f>$M2/$M6</f>
+      <c r="N3" s="2">
+        <f>$M3/$M7</f>
         <v>0.20689655172413793</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R3" s="1">
         <v>2</v>
       </c>
-      <c r="S2" s="2">
-        <f>$R2/$R8</f>
+      <c r="S3" s="2">
+        <f>$R3/$R9</f>
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="1">
+      <c r="U3" s="1">
         <v>1</v>
       </c>
-      <c r="V2" s="2">
-        <f>$U2/$U8</f>
+      <c r="V3" s="2">
+        <f>$U3/$U9</f>
         <v>1.2345679012345678E-2</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="Z3" s="1">
         <v>10</v>
       </c>
-      <c r="AA2" s="2">
-        <f>$Z2/$Z9</f>
+      <c r="AA3" s="2">
+        <f>$Z3/$Z10</f>
         <v>9.1743119266055051E-2</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AC3" s="1">
         <v>20</v>
       </c>
-      <c r="AD2" s="2">
-        <f>$AC2/$AC9</f>
+      <c r="AD3" s="2">
+        <f>$AC3/$AC10</f>
         <v>0.37735849056603776</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AH3" s="1">
         <v>1</v>
       </c>
-      <c r="AI2" s="2">
-        <f>$AH2/$AH10</f>
+      <c r="AI3" s="2">
+        <f>$AH3/$AH11</f>
         <v>0.01</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AK3" s="1">
         <v>2</v>
       </c>
-      <c r="AL2" s="2">
-        <f>$AK2/$AK10</f>
+      <c r="AL3" s="2">
+        <f>$AK3/$AK11</f>
         <v>1.1428571428571429E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B4" s="16">
         <v>99</v>
       </c>
-      <c r="C3" s="2">
-        <f>$B3/$B7</f>
+      <c r="C4" s="2">
+        <f>$B4/$B8</f>
         <v>0.90825688073394495</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
-        <f>$E3/$E7</f>
+      <c r="F4" s="2">
+        <f>$E4/$E8</f>
         <v>2.8571428571428571E-2</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J4" s="16">
         <v>99</v>
       </c>
-      <c r="K3" s="2">
-        <f>$J3/$J6</f>
+      <c r="K4" s="2">
+        <f>$J4/$J7</f>
         <v>0.44594594594594594</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M4" s="1">
         <v>555</v>
       </c>
-      <c r="N3" s="2">
-        <f>$M3/$M6</f>
+      <c r="N4" s="2">
+        <f>$M4/$M7</f>
         <v>0.49071618037135278</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R4" s="16">
         <v>99</v>
       </c>
-      <c r="S3" s="2">
-        <f>$R3/$R8</f>
+      <c r="S4" s="2">
+        <f>$R4/$R9</f>
         <v>0.98019801980198018</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="T4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="U3" s="1">
+      <c r="U4" s="1">
         <v>10</v>
       </c>
-      <c r="V3" s="2">
-        <f>$U3/$U8</f>
+      <c r="V4" s="2">
+        <f>$U4/$U9</f>
         <v>0.12345679012345678</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="16">
+      <c r="Z4" s="16">
         <v>99</v>
       </c>
-      <c r="AA3" s="2">
-        <f>$Z3/$Z9</f>
+      <c r="AA4" s="2">
+        <f>$Z4/$Z10</f>
         <v>0.90825688073394495</v>
       </c>
-      <c r="AB3" s="13" t="s">
+      <c r="AB4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AC4" s="1">
         <v>1</v>
       </c>
-      <c r="AD3" s="2">
-        <f>$AC3/$AC9</f>
+      <c r="AD4" s="2">
+        <f>$AC4/$AC10</f>
         <v>1.8867924528301886E-2</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="16">
+      <c r="AH4" s="16">
         <v>99</v>
       </c>
-      <c r="AI3" s="2">
-        <f>$AH3/$AH10</f>
+      <c r="AI4" s="2">
+        <f>$AH4/$AH11</f>
         <v>0.99</v>
       </c>
-      <c r="AJ3" s="13" t="s">
+      <c r="AJ4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AK3" s="1">
+      <c r="AK4" s="1">
         <v>23</v>
       </c>
-      <c r="AL3" s="2">
-        <f>$AK3/$AK10</f>
+      <c r="AL4" s="2">
+        <f>$AK4/$AK11</f>
         <v>0.13142857142857142</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2">
-        <f>$E4/$E7</f>
-        <v>5.7142857142857141E-2</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="1">
-        <v>342</v>
-      </c>
-      <c r="N4" s="2">
-        <f>$M4/$M6</f>
-        <v>0.30238726790450926</v>
-      </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="U4" s="1">
-        <v>23</v>
-      </c>
-      <c r="V4" s="2">
-        <f>$U4/$U8</f>
-        <v>0.2839506172839506</v>
-      </c>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AD4" s="2">
-        <f>$AC4/$AC9</f>
-        <v>3.7735849056603772E-2</v>
-      </c>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="3"/>
-      <c r="AJ4" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK4" s="1">
-        <v>34</v>
-      </c>
-      <c r="AL4" s="2">
-        <f>$AK4/$AK10</f>
-        <v>0.19428571428571428</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="1" t="s">
-        <v>37</v>
+      <c r="D5" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="E5" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2">
-        <f>$E5/$E7</f>
-        <v>0.34285714285714286</v>
+        <f>$E5/$E8</f>
+        <v>5.7142857142857141E-2</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="2"/>
+      <c r="L5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="1">
+        <v>342</v>
+      </c>
+      <c r="N5" s="2">
+        <f>$M5/$M7</f>
+        <v>0.30238726790450926</v>
+      </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="3"/>
       <c r="T5" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="U5" s="1">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="V5" s="2">
-        <f>$U5/$U8</f>
-        <v>0.55555555555555558</v>
+        <f>$U5/$U9</f>
+        <v>0.2839506172839506</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD5" s="2">
-        <f>$AC5/$AC9</f>
-        <v>5.6603773584905662E-2</v>
+        <f>$AC5/$AC10</f>
+        <v>3.7735849056603772E-2</v>
       </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AK5" s="1">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="AL5" s="2">
-        <f>$AK5/$AK10</f>
-        <v>0.50857142857142856</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <f>$AK5/$AK11</f>
+        <v>0.19428571428571428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="I6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="3">
-        <f>SUM(J2:J5)</f>
-        <v>222</v>
-      </c>
-      <c r="K6" s="4">
-        <f>SUM(K2:K5)</f>
-        <v>1</v>
-      </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="10">
-        <f>SUM(M2:M5)</f>
-        <v>1131</v>
-      </c>
-      <c r="N6" s="4">
-        <f>SUM(N2:N5)</f>
-        <v>1</v>
-      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <f>$E6/$E8</f>
+        <v>0.34285714285714286</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="2"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="3"/>
-      <c r="T6" s="1" t="s">
-        <v>37</v>
+      <c r="T6" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="U6" s="1">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="V6" s="2">
-        <f>$U6/$U8</f>
-        <v>2.4691358024691357E-2</v>
+        <f>$U6/$U9</f>
+        <v>0.55555555555555558</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AC6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD6" s="2">
-        <f>$AC6/$AC9</f>
-        <v>7.5471698113207544E-2</v>
+        <f>$AC6/$AC10</f>
+        <v>5.6603773584905662E-2</v>
       </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AK6" s="1">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="AL6" s="2">
-        <f>$AK6/$AK10</f>
-        <v>6.8571428571428575E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+        <f>$AK6/$AK11</f>
+        <v>0.50857142857142856</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="I7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="3">
-        <f>SUM(B2:B6)</f>
-        <v>109</v>
-      </c>
-      <c r="C7" s="4">
-        <f>SUM(C2:C6)</f>
+      <c r="J7" s="3">
+        <f>SUM(J3:J6)</f>
+        <v>222</v>
+      </c>
+      <c r="K7" s="4">
+        <f>SUM(K3:K6)</f>
         <v>1</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="10">
-        <f>SUM(E2:E6)</f>
-        <v>35</v>
-      </c>
-      <c r="F7" s="4">
-        <f>SUM(F2:F6)</f>
+      <c r="L7" s="3"/>
+      <c r="M7" s="10">
+        <f>SUM(M3:M6)</f>
+        <v>1131</v>
+      </c>
+      <c r="N7" s="4">
+        <f>SUM(N3:N6)</f>
         <v>1</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="2"/>
+      <c r="T7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="1">
+        <v>2</v>
+      </c>
+      <c r="V7" s="2">
+        <f>$U7/$U9</f>
+        <v>2.4691358024691357E-2</v>
+      </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="1" t="s">
-        <v>37</v>
+      <c r="AB7" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="AC7" s="1">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="AD7" s="2">
-        <f>$AC7/$AC9</f>
-        <v>0.43396226415094341</v>
+        <f>$AC7/$AC10</f>
+        <v>7.5471698113207544E-2</v>
       </c>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AK7" s="1">
         <v>12</v>
       </c>
       <c r="AL7" s="2">
-        <f>$AK7/$AK10</f>
+        <f>$AK7/$AK11</f>
         <v>6.8571428571428575E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q8" s="1" t="s">
+    <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R8" s="3">
-        <f>SUM(R2:R7)</f>
-        <v>101</v>
-      </c>
-      <c r="S8" s="4">
-        <f>SUM(S2:S7)</f>
+      <c r="B8" s="3">
+        <f>SUM(B3:B7)</f>
+        <v>109</v>
+      </c>
+      <c r="C8" s="4">
+        <f>SUM(C3:C7)</f>
         <v>1</v>
       </c>
-      <c r="T8" s="3"/>
-      <c r="U8" s="10">
-        <f>SUM(U2:U7)</f>
-        <v>81</v>
-      </c>
-      <c r="V8" s="4">
-        <f>SUM(V2:V7)</f>
+      <c r="D8" s="3"/>
+      <c r="E8" s="10">
+        <f>SUM(E3:E7)</f>
+        <v>35</v>
+      </c>
+      <c r="F8" s="4">
+        <f>SUM(F3:F7)</f>
         <v>1</v>
       </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="2"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="2"/>
+      <c r="AB8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>23</v>
+      </c>
+      <c r="AD8" s="2">
+        <f>$AC8/$AC10</f>
+        <v>0.43396226415094341</v>
+      </c>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="3"/>
-      <c r="AJ8" s="1" t="s">
-        <v>37</v>
+      <c r="AJ8" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="AK8" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="AL8" s="2">
-        <f>$AK8/$AK10</f>
-        <v>1.7142857142857144E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y9" s="1" t="s">
+        <f>$AK8/$AK11</f>
+        <v>6.8571428571428575E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Q9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z9" s="3">
-        <f>SUM(Z2:Z8)</f>
-        <v>109</v>
-      </c>
-      <c r="AA9" s="4">
-        <f>SUM(AA2:AA8)</f>
+      <c r="R9" s="3">
+        <f>SUM(R3:R8)</f>
+        <v>101</v>
+      </c>
+      <c r="S9" s="4">
+        <f>SUM(S3:S8)</f>
         <v>1</v>
       </c>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="10">
-        <f>SUM(AC2:AC8)</f>
-        <v>53</v>
-      </c>
-      <c r="AD9" s="4">
-        <f>SUM(AD2:AD8)</f>
+      <c r="T9" s="3"/>
+      <c r="U9" s="10">
+        <f>SUM(U3:U8)</f>
+        <v>81</v>
+      </c>
+      <c r="V9" s="4">
+        <f>SUM(V3:V8)</f>
         <v>1</v>
       </c>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="2"/>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="3"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="2"/>
-    </row>
-    <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AG10" s="1" t="s">
+      <c r="AJ9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL9" s="2">
+        <f>$AK9/$AK11</f>
+        <v>1.7142857142857144E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Y10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH10" s="3">
-        <f>SUM(AH2:AH9)</f>
+      <c r="Z10" s="3">
+        <f>SUM(Z3:Z9)</f>
+        <v>109</v>
+      </c>
+      <c r="AA10" s="4">
+        <f>SUM(AA3:AA9)</f>
+        <v>1</v>
+      </c>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="10">
+        <f>SUM(AC3:AC9)</f>
+        <v>53</v>
+      </c>
+      <c r="AD10" s="4">
+        <f>SUM(AD3:AD9)</f>
+        <v>1</v>
+      </c>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="2"/>
+    </row>
+    <row r="11" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AG11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH11" s="3">
+        <f>SUM(AH3:AH10)</f>
         <v>100</v>
       </c>
-      <c r="AI10" s="4">
-        <f>SUM(AI2:AI9)</f>
+      <c r="AI11" s="4">
+        <f>SUM(AI3:AI10)</f>
         <v>1</v>
       </c>
-      <c r="AJ10" s="3"/>
-      <c r="AK10" s="10">
-        <f>SUM(AK2:AK9)</f>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="10">
+        <f>SUM(AK3:AK10)</f>
         <v>175</v>
       </c>
-      <c r="AL10" s="4">
-        <f>SUM(AL2:AL9)</f>
+      <c r="AL11" s="4">
+        <f>SUM(AL3:AL10)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="G11" s="1" t="s">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.45">
+      <c r="G12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H12" s="1">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="AB1:AD1"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="AJ1:AL1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="Y1:AA1"/>
+  <mergeCells count="15">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Y1:AD1"/>
+    <mergeCell ref="AG1:AL1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2238,162 +2315,162 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB0A179-3460-4B7F-B6A0-F84428E1F30B}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.86328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.86328125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1">
+      <c r="E3" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
         <v>9091</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F4" s="16">
         <v>125</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="17">
+      <c r="G4" s="1"/>
+      <c r="H4" s="17">
         <v>12</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B5" s="15">
         <v>35</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>959</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
-        <v>9587290</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="15">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>9587290</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="7">
-        <f>SUM(B3:B5)</f>
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="B6" s="15">
+        <v>12</v>
       </c>
       <c r="C6" s="1">
-        <f>SUM(C3:C5)</f>
-        <v>959</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <f>F4</f>
-        <v>9587290</v>
-      </c>
-      <c r="G6" s="14">
-        <f>F6</f>
-        <v>9587290</v>
-      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="7">
+        <f>SUM(B4:B6)</f>
+        <v>47</v>
+      </c>
+      <c r="C7" s="1">
+        <f>SUM(C4:C6)</f>
+        <v>959</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="1">
+        <f>F5</f>
+        <v>9587290</v>
+      </c>
+      <c r="G7" s="14">
+        <f>F7</f>
+        <v>9587290</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>49</v>
-      </c>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2403,101 +2480,103 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>46</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
         <v>38182</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="1">
         <v>34</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="14">
+      <c r="G10" s="1"/>
+      <c r="H10" s="14">
         <v>12</v>
       </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B11" s="15">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>12</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
         <v>672000</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="15">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>34</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B12" s="15">
-        <f>SUM(B10:B11)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
-        <f>F10</f>
-        <v>672000</v>
-      </c>
-      <c r="G12" s="14">
-        <f>F12</f>
-        <v>672000</v>
-      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="15">
+        <f>SUM(B11:B12)</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>16</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <f>F11</f>
+        <v>672000</v>
+      </c>
+      <c r="G13" s="14">
+        <f>F13</f>
+        <v>672000</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2508,7 +2587,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2519,155 +2598,155 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
-      <c r="B16" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="1">
-        <v>9587290</v>
-      </c>
-      <c r="F17" s="2">
-        <f>$E17/$E$19</f>
-        <v>0.93449839121420686</v>
-      </c>
-      <c r="G17" s="1">
-        <v>10000</v>
+      <c r="B17" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="1">
-        <v>672000</v>
+        <v>9587290</v>
       </c>
       <c r="F18" s="2">
-        <f>$E18/$E$19</f>
-        <v>6.5501608785793169E-2</v>
+        <f>$E18/$E$20</f>
+        <v>0.93449839121420686</v>
       </c>
       <c r="G18" s="1">
-        <v>42000</v>
+        <v>10000</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="3">
-        <f>SUM(E17:E18)</f>
-        <v>10259290</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="1">
+        <v>672000</v>
+      </c>
+      <c r="F19" s="2">
+        <f>$E19/$E$20</f>
+        <v>6.5501608785793169E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>42000</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="9">
-        <v>1020</v>
+      <c r="E20" s="3">
+        <f>SUM(E18:E19)</f>
+        <v>10259290</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
-        <f>E19-E20</f>
-        <v>10258270</v>
+      <c r="E21" s="9">
+        <v>1020</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="2">
-        <f>E21/E20</f>
-        <v>10057.127450980392</v>
+      <c r="E22" s="3">
+        <f>E20-E21</f>
+        <v>10258270</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="7"/>
+      <c r="E23" s="2">
+        <f>E22/E21</f>
+        <v>10057.127450980392</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2678,9 +2757,21 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B16:D16"/>
+  <mergeCells count="2">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2694,15 +2785,15 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>95</v>
       </c>
@@ -2716,13 +2807,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
@@ -2736,7 +2827,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>91</v>
       </c>
@@ -2750,7 +2841,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>92</v>
       </c>
@@ -2764,7 +2855,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>93</v>
       </c>
@@ -2778,7 +2869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2786,7 +2877,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="14"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2794,7 +2885,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2802,7 +2893,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -2810,7 +2901,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -2818,7 +2909,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -2837,24 +2928,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2865,6 +2956,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -3028,24 +3136,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3061,28 +3176,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excel to PDF update
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\IdeaProjects\SEPJ\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30E3FCD-ED78-4F9C-A4AF-CC86805EF46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C940C5B8-745F-4844-9642-223D15DA86DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Executive Summary" sheetId="22" r:id="rId1"/>
     <sheet name="Basisinformation" sheetId="7" r:id="rId2"/>
     <sheet name="Standort" sheetId="11" r:id="rId3"/>
-    <sheet name="Widmung" sheetId="23" r:id="rId4"/>
-    <sheet name="Gesamtinvestitionskosten" sheetId="8" r:id="rId5"/>
-    <sheet name="Mittelverwendung - Mittelherkun" sheetId="9" r:id="rId6"/>
-    <sheet name="Wirtschaftlichkeitsrechnung" sheetId="10" r:id="rId7"/>
-    <sheet name="MVMH1" sheetId="12" r:id="rId8"/>
-    <sheet name="MVMH2" sheetId="18" r:id="rId9"/>
-    <sheet name="MVMH3" sheetId="19" r:id="rId10"/>
-    <sheet name="MVMH4" sheetId="20" r:id="rId11"/>
-    <sheet name="MVMH5" sheetId="21" r:id="rId12"/>
-    <sheet name="Restliche Fragen" sheetId="4" r:id="rId13"/>
+    <sheet name="Lage" sheetId="24" r:id="rId4"/>
+    <sheet name="Widmung" sheetId="23" r:id="rId5"/>
+    <sheet name="Gesamtinvestitionskosten" sheetId="8" r:id="rId6"/>
+    <sheet name="Mittelverwendung - Mittelherkun" sheetId="9" r:id="rId7"/>
+    <sheet name="Wirtschaftlichkeitsrechnung" sheetId="10" r:id="rId8"/>
+    <sheet name="MVMH1" sheetId="12" r:id="rId9"/>
+    <sheet name="MVMH2" sheetId="18" r:id="rId10"/>
+    <sheet name="MVMH3" sheetId="19" r:id="rId11"/>
+    <sheet name="MVMH4" sheetId="20" r:id="rId12"/>
+    <sheet name="MVMH5" sheetId="21" r:id="rId13"/>
+    <sheet name="Restliche Fragen" sheetId="4" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="122">
   <si>
     <t>Wohneinheiten</t>
   </si>
@@ -78,9 +79,6 @@
     <t>Garagenstellplätze</t>
   </si>
   <si>
-    <t>ROI</t>
-  </si>
-  <si>
     <t>Ziel-Baubeginn</t>
   </si>
   <si>
@@ -240,18 +238,6 @@
     <t>Ort</t>
   </si>
   <si>
-    <t xml:space="preserve">Entfernung zur Schule </t>
-  </si>
-  <si>
-    <t>Lagebeschreibung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maps - Bild </t>
-  </si>
-  <si>
-    <t>Lage der Öffi Anbindung</t>
-  </si>
-  <si>
     <t>Basisinformationen</t>
   </si>
   <si>
@@ -273,31 +259,10 @@
     <t>Wien</t>
   </si>
   <si>
-    <t>Hallo</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
     <t>Tranche</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>23</t>
   </si>
   <si>
     <t>Schulen</t>
@@ -334,12 +299,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>hierU6</t>
-  </si>
-  <si>
-    <t>u7</t>
-  </si>
-  <si>
     <t>gk = gekuppelte Bauweise</t>
   </si>
   <si>
@@ -370,18 +329,12 @@
     <t>Kaufpreis (in €)</t>
   </si>
   <si>
-    <t>Gewinn (in €)</t>
-  </si>
-  <si>
     <t>Standortlage</t>
   </si>
   <si>
     <t>m²</t>
   </si>
   <si>
-    <t>Prognostizierter Verkaufserlös (in €)</t>
-  </si>
-  <si>
     <t>Executive Summary</t>
   </si>
   <si>
@@ -467,6 +420,24 @@
   </si>
   <si>
     <t>G = Gärtnerische Ausgestaltung</t>
+  </si>
+  <si>
+    <t>Nahversorgung, Restaurants u. Geschäfte des täglichen Bedarfs in unmittelbarer Nähe</t>
+  </si>
+  <si>
+    <t>Bestlage im 17. Bezirk</t>
+  </si>
+  <si>
+    <t>Absolute Ruhelage, mit Fernblick über Wien</t>
+  </si>
+  <si>
+    <t>Zentrum Wien 18 Autominuten, öffentlich 25 Minuten</t>
+  </si>
+  <si>
+    <t>Nahversorgung, Restaurants u. Geschäfte deees täglichen Bedarfs in unmittelbarer Nähe</t>
+  </si>
+  <si>
+    <t>Nahversorgung, Restaurants u. Geschäfte dees täglichen Bedarfs in unmittelbarer Nähe</t>
   </si>
 </sst>
 </file>
@@ -524,14 +495,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +551,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -707,12 +689,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1037,21 +1026,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC82671E-D144-4B50-AABB-443299DFAAD9}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="101.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="101.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
-        <v>103</v>
+      <c r="A1" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="B1" s="26"/>
     </row>
@@ -1079,21 +1068,21 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="str">
         <f>+Basisinformation!Y5</f>
-        <v>Grundstücksgröße: 20 m²</v>
+        <v>Grundstücksgröße: 797 m²</v>
       </c>
       <c r="B5" s="18"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="str">
         <f>+Basisinformation!Y6</f>
-        <v>Erzielbare Wohnnutzfläche laut Architekt: 120 m² WNFL zzgl. gew. Außenflächen von 34 m²</v>
+        <v>Erzielbare Wohnnutzfläche laut Architekt: 800 m² WNFL zzgl. gew. Außenflächen von 160 m²</v>
       </c>
       <c r="B6" s="21"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="str">
         <f>+Basisinformation!Y7</f>
-        <v>Nutzung: 34 Wohneinheiten mit 12 Garagenstellplätzen</v>
+        <v>Nutzung: 8 Wohneinheiten mit 16 Garagenstellplätzen</v>
       </c>
       <c r="B7" s="18"/>
     </row>
@@ -1107,14 +1096,14 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="str">
         <f>+Basisinformation!Y9</f>
-        <v>Prognostizierter Verkaufserlös: EUR 10260000; ø Verkaufspreis EUR 10000</v>
+        <v>Prognostizierter Verkaufserlös: EUR 10270000; ø Verkaufspreis EUR 10000</v>
       </c>
       <c r="B9" s="18"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="str">
         <f>+Basisinformation!Y10</f>
-        <v>Gewinn: EUR 2500000 (gerundet ROI 32,33%)</v>
+        <v>Gewinn: EUR 2500000 (gerundet ROI 32,5%)</v>
       </c>
       <c r="B10" s="18"/>
     </row>
@@ -1158,6 +1147,152 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE9CAD6-D690-4F39-9F95-0EFEA57D740F}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="str" cm="1">
+        <f t="array" ref="A3:C4">+'Mittelverwendung - Mittelherkun'!A3:C4</f>
+        <v>Investitionskosten</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>9.1743119266055051E-2</v>
+      </c>
+      <c r="D3" s="1" t="str" cm="1">
+        <f t="array" ref="D3:F6">+'Mittelverwendung - Mittelherkun'!D3:F6</f>
+        <v>Eigenkapital</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="str">
+        <v>Finanzierungskosten</v>
+      </c>
+      <c r="B4" s="16">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.90825688073394495</v>
+      </c>
+      <c r="D4" s="13" t="str">
+        <v>Fremdkapital Tranche 1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="13" t="str">
+        <v>Fremdkapital Tranche 2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1" t="str">
+        <v>BTVG Erlöse</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.34285714285714286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="str" cm="1">
+        <f t="array" ref="A8:C8">+'Mittelverwendung - Mittelherkun'!A8:C8</f>
+        <v>Summe</v>
+      </c>
+      <c r="B8" s="3">
+        <v>109</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="10" cm="1">
+        <f t="array" ref="E8:F8">+'Mittelverwendung - Mittelherkun'!E8:F8</f>
+        <v>35</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CC4E7A-DD07-46E4-800C-29AAAD817904}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -1174,26 +1309,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="A1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str" cm="1">
@@ -1325,7 +1460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED108C8A-0089-49D9-A899-5A80F96B0F9A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -1342,26 +1477,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="A1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str" cm="1">
@@ -1499,7 +1634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B850460-7005-44F1-8B1C-A579BD0AD684}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1516,26 +1651,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="A1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str" cm="1">
@@ -1687,7 +1822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0F1FA0-C1BF-4C59-8CFC-4ADA78F070EE}">
   <dimension ref="A3:A7"/>
   <sheetViews>
@@ -1697,22 +1832,22 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1725,7 +1860,7 @@
   <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1734,39 +1869,39 @@
     <col min="8" max="8" width="25.33203125" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="24.5546875" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="50.6640625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
+      <c r="A1" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
-      <c r="H1" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="36"/>
+      <c r="H1" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="43"/>
       <c r="O1" s="24" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="T1" s="24" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -1774,30 +1909,30 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
       <c r="O2" s="18" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="P2" t="str">
         <f>LEFT(O2,SEARCH("=",O2)-2)</f>
         <v>W II</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="U2" s="18" t="str">
         <f>+Basisinformation!I3</f>
         <v>Braumüllergasse 21</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="W2" s="18"/>
       <c r="X2" s="18"/>
@@ -1808,10 +1943,10 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>72</v>
+        <v>80</v>
+      </c>
+      <c r="B3" s="18">
+        <v>797</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -1819,23 +1954,23 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="18" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="O3" s="18" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="P3" t="str">
         <f>LEFT(O3,SEARCH("=",O3)-2)</f>
         <v>gk</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="U3" s="18" t="str">
         <f>+Basisinformation!B2</f>
@@ -1851,10 +1986,10 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>73</v>
+        <v>81</v>
+      </c>
+      <c r="B4" s="18">
+        <v>800</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -1862,33 +1997,33 @@
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="H4" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="O4" s="27" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="P4" s="25" t="str">
         <f>CONCATENATE(P2," ",P3)</f>
         <v>W II gk</v>
       </c>
       <c r="Q4" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="U4" s="18" t="str">
         <f>+Basisinformation!P7</f>
         <v>G</v>
       </c>
       <c r="V4" s="18" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="W4" s="18" t="str">
         <f>+Basisinformation!P4</f>
@@ -1904,8 +2039,8 @@
       <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>74</v>
+      <c r="B5" s="18">
+        <v>8</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
@@ -1913,10 +2048,10 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
@@ -1927,40 +2062,36 @@
         <v>G</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="U5" s="18" t="str">
+        <v>96</v>
+      </c>
+      <c r="U5" s="18">
         <f>+Basisinformation!B3</f>
-        <v>20</v>
+        <v>797</v>
       </c>
       <c r="V5" s="18" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="W5" s="18"/>
       <c r="X5" s="18"/>
       <c r="Y5" t="str">
         <f t="shared" si="0"/>
-        <v>Grundstücksgröße: 20 m²</v>
+        <v>Grundstücksgröße: 797 m²</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>69</v>
+      <c r="B6" s="18">
+        <v>16</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
-      <c r="H6" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>87</v>
-      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
@@ -1970,45 +2101,41 @@
         <v>angefordert</v>
       </c>
       <c r="T6" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="U6" s="18" t="str">
+        <v>98</v>
+      </c>
+      <c r="U6" s="18">
         <f>+Basisinformation!B4</f>
-        <v>120</v>
+        <v>800</v>
       </c>
       <c r="V6" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="W6" s="18" t="str">
+        <v>99</v>
+      </c>
+      <c r="W6" s="18">
         <f>+Basisinformation!B7</f>
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="X6" s="18" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="Y6" t="str">
         <f t="shared" si="0"/>
-        <v>Erzielbare Wohnnutzfläche laut Architekt: 120 m² WNFL zzgl. gew. Außenflächen von 34 m²</v>
+        <v>Erzielbare Wohnnutzfläche laut Architekt: 800 m² WNFL zzgl. gew. Außenflächen von 160 m²</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>74</v>
+        <v>82</v>
+      </c>
+      <c r="B7" s="18">
+        <v>160</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>67</v>
-      </c>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
@@ -2018,61 +2145,57 @@
         <v>G</v>
       </c>
       <c r="Q7" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="T7" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="U7" s="18" t="str">
+        <v>100</v>
+      </c>
+      <c r="U7" s="18">
         <f>+Basisinformation!B5</f>
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="V7" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="W7" s="18" t="str">
+        <v>101</v>
+      </c>
+      <c r="W7" s="18">
         <f>+Basisinformation!B6</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X7" s="18" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="0"/>
-        <v>Nutzung: 34 Wohneinheiten mit 12 Garagenstellplätzen</v>
+        <v>Nutzung: 8 Wohneinheiten mit 16 Garagenstellplätzen</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>75</v>
+      <c r="A8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>88</v>
-      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
       <c r="O8" s="18"/>
       <c r="T8" s="18" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="U8" s="18">
         <f>+ROUND(Gesamtinvestitionskosten!E15,-4)</f>
         <v>7750000</v>
       </c>
       <c r="V8" s="18" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="W8" s="18"/>
       <c r="X8" s="18"/>
@@ -2082,54 +2205,46 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>69</v>
+      <c r="A9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>110</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="20"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>68</v>
-      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
       <c r="O9" s="18"/>
       <c r="T9" s="18" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="U9" s="18">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!E20,-4)</f>
-        <v>10260000</v>
+        <v>10270000</v>
       </c>
       <c r="V9" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="W9" s="30">
+        <v>106</v>
+      </c>
+      <c r="W9" s="29">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!F4,0)</f>
         <v>10000</v>
       </c>
       <c r="X9" s="18"/>
       <c r="Y9" t="str">
         <f t="shared" si="0"/>
-        <v>Prognostizierter Verkaufserlös: EUR 10260000; ø Verkaufspreis EUR 10000</v>
+        <v>Prognostizierter Verkaufserlös: EUR 10270000; ø Verkaufspreis EUR 10000</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -2141,34 +2256,30 @@
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
       <c r="T10" s="18" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="U10" s="18">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!E22,-5)</f>
         <v>2500000</v>
       </c>
       <c r="V10" s="18" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="W10" s="20">
         <f>+Wirtschaftlichkeitsrechnung!E23</f>
-        <v>0.32334413683406937</v>
+        <v>0.32498359765242629</v>
       </c>
       <c r="X10" s="18" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="Y10" t="str">
         <f>+CONCATENATE(T10,U10,V10,ROUND(W10*100,2),X10)</f>
-        <v>Gewinn: EUR 2500000 (gerundet ROI 32,33%)</v>
+        <v>Gewinn: EUR 2500000 (gerundet ROI 32,5%)</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>126</v>
-      </c>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -2180,10 +2291,10 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
       <c r="T11" s="18" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="U11" s="18" t="str">
-        <f>+Basisinformation!B10</f>
+        <f>+B8</f>
         <v>Q4/2025</v>
       </c>
       <c r="V11" s="18"/>
@@ -2195,20 +2306,16 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="A12" s="30"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="T12" s="18" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="U12" s="18" t="str">
-        <f>+Basisinformation!B11</f>
+        <f>+B9</f>
         <v>Q2/2026</v>
       </c>
       <c r="V12" s="18"/>
@@ -2233,7 +2340,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2246,34 +2353,40 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1">
         <v>8</v>
@@ -2281,13 +2394,13 @@
       <c r="C4" s="1">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1">
         <v>8</v>
@@ -2295,13 +2408,13 @@
       <c r="C5" s="1">
         <v>8</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1">
         <v>8</v>
@@ -2309,38 +2422,32 @@
       <c r="C6" s="1">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="1">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="F7" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>85</v>
+      <c r="F9" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2348,7 +2455,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2356,7 +2463,7 @@
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="F11" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2364,7 +2471,7 @@
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="F12" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2372,7 +2479,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="F13" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2381,74 +2488,189 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F1B394-FC16-4981-9813-BB2630F00164}">
-  <dimension ref="A1:A10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECEC122-E6AD-46FD-8341-64D0B93B9E90}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="str">
-        <f>+CONCATENATE(Basisinformation!I3,", ",Basisinformation!I4," ",Basisinformation!I5)</f>
-        <v>Braumüllergasse 21, 1170 Wien</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="str" cm="1">
-        <f t="array" ref="A3:A4">+Basisinformation!O2:O3</f>
-        <v>W II = Bauklasse 2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="str">
-        <v>gk = gekuppelte Bauweise</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="str">
-        <f>+IF(ISBLANK(Basisinformation!O4),"",Basisinformation!O4)</f>
-        <v>G = Gärtnerische Ausgestaltung</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="str">
-        <f>+IF(ISBLANK(Basisinformation!O5),"",Basisinformation!O5)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="str">
-        <f>+IF(ISBLANK(Basisinformation!O6),"",Basisinformation!O6)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="str">
-        <f>+IF(ISBLANK(Basisinformation!O7),"",Basisinformation!O7)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="str">
-        <f>+IF(ISBLANK(Basisinformation!O8),"",Basisinformation!O8)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="str">
-        <f>+IF(ISBLANK(Basisinformation!O9),"",Basisinformation!O9)</f>
-        <v/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="str">
+        <f>+IF(ISBLANK(Standort!F3),"",Standort!F3)</f>
+        <v>Bestlage im 17. Bezirk</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="str">
+        <f>+IF(ISBLANK(Standort!F4),"",Standort!F4)</f>
+        <v>Absolute Ruhelage, mit Fernblick über Wien</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="str">
+        <f>+IF(ISBLANK(Standort!F5),"",Standort!F5)</f>
+        <v>Zentrum Wien 18 Autominuten, öffentlich 25 Minuten</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="str">
+        <f>+IF(ISBLANK(Standort!F6),"",Standort!F6)</f>
+        <v>Nahversorgung, Restaurants u. Geschäfte des täglichen Bedarfs in unmittelbarer Nähe</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="str">
+        <f>+IF(ISBLANK(Standort!F7),"",Standort!F7)</f>
+        <v>Nahversorgung, Restaurants u. Geschäfte dees täglichen Bedarfs in unmittelbarer Nähe</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="str">
+        <f>+IF(ISBLANK(Standort!F8),"",Standort!F8)</f>
+        <v>Nahversorgung, Restaurants u. Geschäfte deees täglichen Bedarfs in unmittelbarer Nähe</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="1">
+        <f>+Standort!B3</f>
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <f>+Standort!B3</f>
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
+        <f>+Standort!B5</f>
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
+        <f>+Standort!B6</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="1">
+        <f>+Standort!C3</f>
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <f>+Standort!C4</f>
+        <v>8</v>
+      </c>
+      <c r="D12" s="1">
+        <f>+Standort!C5</f>
+        <v>8</v>
+      </c>
+      <c r="E12" s="1">
+        <f>+Standort!C6</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="F19" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="F20" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="F21" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2457,11 +2679,87 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F1B394-FC16-4981-9813-BB2630F00164}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.21875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="str">
+        <f>+CONCATENATE(Basisinformation!I3,", ",Basisinformation!I4," ",Basisinformation!I5)</f>
+        <v>Braumüllergasse 21, 1170 Wien</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="str" cm="1">
+        <f t="array" ref="A3:A4">+Basisinformation!O2:O3</f>
+        <v>W II = Bauklasse 2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="str">
+        <v>gk = gekuppelte Bauweise</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="str">
+        <f>+IF(ISBLANK(Basisinformation!O4),"",Basisinformation!O4)</f>
+        <v>G = Gärtnerische Ausgestaltung</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="str">
+        <f>+IF(ISBLANK(Basisinformation!O5),"",Basisinformation!O5)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="str">
+        <f>+IF(ISBLANK(Basisinformation!O6),"",Basisinformation!O6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="str">
+        <f>+IF(ISBLANK(Basisinformation!O7),"",Basisinformation!O7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="str">
+        <f>+IF(ISBLANK(Basisinformation!O8),"",Basisinformation!O8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="str">
+        <f>+IF(ISBLANK(Basisinformation!O9),"",Basisinformation!O9)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57066AFC-3CC1-4339-B554-0D5829A53635}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2472,38 +2770,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="A1" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>2530800</v>
@@ -2528,7 +2826,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>85892</v>
@@ -2553,7 +2851,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>2475206</v>
@@ -2578,7 +2876,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>212558</v>
@@ -2603,7 +2901,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>612366</v>
@@ -2628,7 +2926,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>39881</v>
@@ -2653,7 +2951,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>101581</v>
@@ -2678,7 +2976,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>52000</v>
@@ -2703,7 +3001,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="9">
         <v>901060</v>
@@ -2735,7 +3033,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3">
         <f>SUM(B3:B11)</f>
@@ -2761,7 +3059,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2772,7 +3070,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3">
         <f>B13</f>
@@ -2825,7 +3123,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="11">
         <v>0.2</v>
@@ -2833,13 +3131,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="12">
         <v>0.01</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2850,7 +3148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C08536-E6A3-4E31-88A7-DF1DE6751CED}">
   <dimension ref="A1:AL12"/>
   <sheetViews>
@@ -2883,102 +3181,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="I1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="Q1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="Y1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AG1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
+      <c r="A1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="I1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="Q1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="Y1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AG1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
     </row>
     <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="I2" s="38" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+      <c r="I2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="40"/>
-      <c r="N2" s="41"/>
-      <c r="Q2" s="38" t="s">
+      <c r="M2" s="47"/>
+      <c r="N2" s="48"/>
+      <c r="Q2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" s="40"/>
-      <c r="V2" s="41"/>
-      <c r="Y2" s="38" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="48"/>
+      <c r="Y2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="41"/>
-      <c r="AG2" s="38" t="s">
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="48"/>
+      <c r="AG2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="AH2" s="38"/>
-      <c r="AI2" s="38"/>
-      <c r="AJ2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK2" s="40"/>
-      <c r="AL2" s="41"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="48"/>
     </row>
     <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
         <v>10</v>
@@ -2988,7 +3286,7 @@
         <v>9.1743119266055051E-2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1">
         <v>20</v>
@@ -2998,7 +3296,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" s="1">
         <v>123</v>
@@ -3008,7 +3306,7 @@
         <v>0.55405405405405406</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M3" s="1">
         <v>234</v>
@@ -3018,7 +3316,7 @@
         <v>0.20689655172413793</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R3" s="1">
         <v>2</v>
@@ -3028,7 +3326,7 @@
         <v>1.9801980198019802E-2</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U3" s="1">
         <v>1</v>
@@ -3038,7 +3336,7 @@
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Z3" s="1">
         <v>10</v>
@@ -3048,7 +3346,7 @@
         <v>9.1743119266055051E-2</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC3" s="1">
         <v>20</v>
@@ -3058,7 +3356,7 @@
         <v>0.37735849056603776</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AH3" s="1">
         <v>1</v>
@@ -3068,7 +3366,7 @@
         <v>0.01</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AK3" s="1">
         <v>2</v>
@@ -3080,7 +3378,7 @@
     </row>
     <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="16">
         <v>99</v>
@@ -3090,7 +3388,7 @@
         <v>0.90825688073394495</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -3100,7 +3398,7 @@
         <v>2.8571428571428571E-2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="16">
         <v>99</v>
@@ -3110,7 +3408,7 @@
         <v>0.44594594594594594</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M4" s="1">
         <v>555</v>
@@ -3120,7 +3418,7 @@
         <v>0.49071618037135278</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R4" s="16">
         <v>99</v>
@@ -3130,7 +3428,7 @@
         <v>0.98019801980198018</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="U4" s="1">
         <v>10</v>
@@ -3140,7 +3438,7 @@
         <v>0.12345679012345678</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z4" s="16">
         <v>99</v>
@@ -3150,7 +3448,7 @@
         <v>0.90825688073394495</v>
       </c>
       <c r="AB4" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AC4" s="1">
         <v>1</v>
@@ -3160,7 +3458,7 @@
         <v>1.8867924528301886E-2</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AH4" s="16">
         <v>99</v>
@@ -3170,7 +3468,7 @@
         <v>0.99</v>
       </c>
       <c r="AJ4" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AK4" s="1">
         <v>23</v>
@@ -3185,7 +3483,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -3198,7 +3496,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M5" s="1">
         <v>342</v>
@@ -3211,7 +3509,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="3"/>
       <c r="T5" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="U5" s="1">
         <v>23</v>
@@ -3224,7 +3522,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="AC5" s="1">
         <v>2</v>
@@ -3237,7 +3535,7 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="AK5" s="1">
         <v>34</v>
@@ -3252,7 +3550,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1">
         <v>12</v>
@@ -3271,7 +3569,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="3"/>
       <c r="T6" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="U6" s="1">
         <v>45</v>
@@ -3284,7 +3582,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="AC6" s="1">
         <v>3</v>
@@ -3297,7 +3595,7 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="AK6" s="1">
         <v>89</v>
@@ -3315,7 +3613,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" s="3">
         <f>SUM(J3:J6)</f>
@@ -3338,7 +3636,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="3"/>
       <c r="T7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U7" s="1">
         <v>2</v>
@@ -3351,7 +3649,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AC7" s="1">
         <v>4</v>
@@ -3364,7 +3662,7 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AK7" s="1">
         <v>12</v>
@@ -3376,7 +3674,7 @@
     </row>
     <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3">
         <f>SUM(B3:B7)</f>
@@ -3405,7 +3703,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC8" s="1">
         <v>23</v>
@@ -3418,7 +3716,7 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="AK8" s="1">
         <v>12</v>
@@ -3430,7 +3728,7 @@
     </row>
     <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R9" s="3">
         <f>SUM(R3:R8)</f>
@@ -3459,7 +3757,7 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AK9" s="1">
         <v>3</v>
@@ -3471,7 +3769,7 @@
     </row>
     <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Y10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Z10" s="3">
         <f>SUM(Z3:Z9)</f>
@@ -3499,7 +3797,7 @@
     </row>
     <row r="11" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AG11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AH11" s="3">
         <f>SUM(AH3:AH10)</f>
@@ -3521,7 +3819,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="G12" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H12" s="1">
         <v>5</v>
@@ -3529,6 +3827,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Y1:AD1"/>
+    <mergeCell ref="AG1:AL1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="AB2:AD2"/>
@@ -3539,22 +3842,17 @@
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="Y1:AD1"/>
-    <mergeCell ref="AG1:AL1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB0A179-3460-4B7F-B6A0-F84428E1F30B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3562,54 +3860,56 @@
     <col min="1" max="1" width="42.88671875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="12.109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="A1" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="F3" s="15">
+      <c r="E3" s="15">
         <v>0.1</v>
       </c>
       <c r="G3" s="1"/>
@@ -3620,41 +3920,43 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="16">
-        <v>9091</v>
-      </c>
-      <c r="F4" s="29">
-        <f>+E4*1.1</f>
-        <v>10000.1</v>
+      <c r="E4" s="34">
+        <f>+F4/1.1</f>
+        <v>9090.9090909090901</v>
+      </c>
+      <c r="F4" s="33">
+        <v>10000</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="28">
+      <c r="H4" s="34">
         <f>+E4*1.2</f>
-        <v>10909.199999999999</v>
+        <v>10909.090909090908</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="16">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1">
-        <v>959</v>
+        <v>36</v>
+      </c>
+      <c r="B5" s="37">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <f>+B5*C7</f>
+        <v>960</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <v>9587290</v>
+      <c r="F5" s="3">
+        <f>+F4*C5</f>
+        <v>9600000</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -3662,48 +3964,60 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="16">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
+        <v>37</v>
+      </c>
+      <c r="B6" s="36">
+        <f>1-B5</f>
         <v>0</v>
       </c>
+      <c r="C6" s="3">
+        <f>+B6*C7</f>
+        <v>0</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="E6" s="40">
+        <v>0</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="3">
+        <f>+H4*C6</f>
+        <v>0</v>
+      </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="7">
-        <f>SUM(B4:B6)</f>
-        <v>47</v>
-      </c>
-      <c r="C7" s="1">
-        <f>SUM(C4:C6)</f>
-        <v>959</v>
+        <v>29</v>
+      </c>
+      <c r="B7" s="36">
+        <f>B5+B6</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="35">
+        <f>+Basisinformation!B4+Basisinformation!B7</f>
+        <v>960</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
-        <f>F5</f>
-        <v>9587290</v>
-      </c>
-      <c r="G7" s="14">
-        <f>F7</f>
-        <v>9587290</v>
-      </c>
-      <c r="H7" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="E7" s="40">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <f>+F5</f>
+        <v>9600000</v>
+      </c>
+      <c r="G7" s="38">
+        <f>+H7+F7</f>
+        <v>9600000</v>
+      </c>
+      <c r="H7" s="3">
+        <f>+H6</f>
+        <v>0</v>
+      </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -3719,7 +4033,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3732,36 +4046,40 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="16">
-        <v>38182</v>
-      </c>
-      <c r="F10" s="1">
-        <v>34</v>
+      <c r="E10" s="28">
+        <f>+F10/1.1</f>
+        <v>38181.818181818177</v>
+      </c>
+      <c r="F10" s="16">
+        <v>42000</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="14">
-        <v>12</v>
+      <c r="H10" s="39">
+        <f>+E10*1.2</f>
+        <v>45818.181818181809</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="15">
+        <f>+C11/C13</f>
         <v>1</v>
       </c>
       <c r="C11" s="16">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
+        <f>+F10*C11</f>
         <v>672000</v>
       </c>
       <c r="G11" s="1"/>
@@ -3770,47 +4088,55 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="15">
+        <f>+C12/C13</f>
         <v>0</v>
       </c>
       <c r="C12" s="16">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1">
+      <c r="E12" s="40">
         <v>0</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="3">
+        <f>+H10*C12</f>
+        <v>0</v>
+      </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="15">
-        <f>SUM(B11:B12)</f>
+        <f>+B11+B12</f>
         <v>1</v>
       </c>
       <c r="C13" s="1">
+        <f>+C11+C12</f>
         <v>16</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1">
+      <c r="E13" s="40">
         <v>0</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <f>F11</f>
         <v>672000</v>
       </c>
-      <c r="G13" s="14">
-        <f>F13</f>
+      <c r="G13" s="38">
+        <f>+F13+H13</f>
         <v>672000</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="3">
+        <f>+H12</f>
+        <v>0</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -3848,19 +4174,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -3869,19 +4195,21 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="1">
-        <v>9587290</v>
+        <v>43</v>
+      </c>
+      <c r="E18" s="3">
+        <f>+G7</f>
+        <v>9600000</v>
       </c>
       <c r="F18" s="2">
         <f>$E18/$E$20</f>
-        <v>0.93449839121420686</v>
-      </c>
-      <c r="G18" s="1">
+        <v>0.93457943925233644</v>
+      </c>
+      <c r="G18" s="3">
+        <f>+G7/C7</f>
         <v>10000</v>
       </c>
       <c r="H18" s="1"/>
@@ -3891,19 +4219,21 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="1">
+        <v>43</v>
+      </c>
+      <c r="E19" s="3">
+        <f>+G13</f>
         <v>672000</v>
       </c>
       <c r="F19" s="2">
         <f>$E19/$E$20</f>
-        <v>6.5501608785793169E-2</v>
-      </c>
-      <c r="G19" s="1">
+        <v>6.5420560747663545E-2</v>
+      </c>
+      <c r="G19" s="3">
+        <f>+G13/C13</f>
         <v>42000</v>
       </c>
       <c r="H19" s="1"/>
@@ -3913,12 +4243,12 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="3">
         <f>SUM(E18:E19)</f>
-        <v>10259290</v>
+        <v>10272000</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -3930,7 +4260,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="9">
         <f>+Gesamtinvestitionskosten!E15</f>
@@ -3946,11 +4276,11 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="3">
         <f>E20-E21</f>
-        <v>2506741.2000000002</v>
+        <v>2519451.2000000002</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -3962,11 +4292,11 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2">
         <f>E22/E21</f>
-        <v>0.32334413683406937</v>
+        <v>0.32498359765242629</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -4015,7 +4345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4EA2CB-3137-483B-BB0D-B03B8C368056}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -4032,26 +4362,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="A1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
@@ -4148,152 +4478,6 @@
       </c>
       <c r="F7" s="4">
         <f>+'Mittelverwendung - Mittelherkun'!N7</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE9CAD6-D690-4F39-9F95-0EFEA57D740F}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="str" cm="1">
-        <f t="array" ref="A3:C4">+'Mittelverwendung - Mittelherkun'!A3:C4</f>
-        <v>Investitionskosten</v>
-      </c>
-      <c r="B3" s="1">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9.1743119266055051E-2</v>
-      </c>
-      <c r="D3" s="1" t="str" cm="1">
-        <f t="array" ref="D3:F6">+'Mittelverwendung - Mittelherkun'!D3:F6</f>
-        <v>Eigenkapital</v>
-      </c>
-      <c r="E3" s="1">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.5714285714285714</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="str">
-        <v>Finanzierungskosten</v>
-      </c>
-      <c r="B4" s="16">
-        <v>99</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.90825688073394495</v>
-      </c>
-      <c r="D4" s="13" t="str">
-        <v>Fremdkapital Tranche 1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2.8571428571428571E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="13" t="str">
-        <v>Fremdkapital Tranche 2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>5.7142857142857141E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="1" t="str">
-        <v>BTVG Erlöse</v>
-      </c>
-      <c r="E6" s="1">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.34285714285714286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="str" cm="1">
-        <f t="array" ref="A8:C8">+'Mittelverwendung - Mittelherkun'!A8:C8</f>
-        <v>Summe</v>
-      </c>
-      <c r="B8" s="3">
-        <v>109</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="10" cm="1">
-        <f t="array" ref="E8:F8">+'Mittelverwendung - Mittelherkun'!E8:F8</f>
-        <v>35</v>
-      </c>
-      <c r="F8" s="4">
         <v>1</v>
       </c>
     </row>
@@ -4308,14 +4492,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -4479,6 +4655,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4489,22 +4673,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4522,6 +4690,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
combine pdf last step
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\IdeaProjects\SEPJ\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43677\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C940C5B8-745F-4844-9642-223D15DA86DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646AB3D-577E-4F4C-9685-7B8E95F225D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="7" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Executive Summary" sheetId="22" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="116">
   <si>
     <t>Wohneinheiten</t>
   </si>
@@ -420,24 +420,6 @@
   </si>
   <si>
     <t>G = Gärtnerische Ausgestaltung</t>
-  </si>
-  <si>
-    <t>Nahversorgung, Restaurants u. Geschäfte des täglichen Bedarfs in unmittelbarer Nähe</t>
-  </si>
-  <si>
-    <t>Bestlage im 17. Bezirk</t>
-  </si>
-  <si>
-    <t>Absolute Ruhelage, mit Fernblick über Wien</t>
-  </si>
-  <si>
-    <t>Zentrum Wien 18 Autominuten, öffentlich 25 Minuten</t>
-  </si>
-  <si>
-    <t>Nahversorgung, Restaurants u. Geschäfte deees täglichen Bedarfs in unmittelbarer Nähe</t>
-  </si>
-  <si>
-    <t>Nahversorgung, Restaurants u. Geschäfte dees täglichen Bedarfs in unmittelbarer Nähe</t>
   </si>
 </sst>
 </file>
@@ -1026,118 +1008,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC82671E-D144-4B50-AABB-443299DFAAD9}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="101.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="101.36328125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="32" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="str">
         <f>+Basisinformation!Y2</f>
         <v>Ankauf der Liegenschaft “Braumüllergasse 21” in Form eines Asset Deals mit einer eigens gegründeten Projektgesellschaft</v>
       </c>
       <c r="B2" s="18"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="str">
         <f>+Basisinformation!Y3</f>
         <v>Kaufpreis: EUR 10</v>
       </c>
       <c r="B3" s="18"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="str">
         <f>+Basisinformation!Y4</f>
         <v>Bebauungsbestimmungen: G; Widmung: W II gk</v>
       </c>
       <c r="B4" s="22"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="str">
         <f>+Basisinformation!Y5</f>
         <v>Grundstücksgröße: 797 m²</v>
       </c>
       <c r="B5" s="18"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="str">
         <f>+Basisinformation!Y6</f>
         <v>Erzielbare Wohnnutzfläche laut Architekt: 800 m² WNFL zzgl. gew. Außenflächen von 160 m²</v>
       </c>
       <c r="B6" s="21"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="str">
         <f>+Basisinformation!Y7</f>
         <v>Nutzung: 8 Wohneinheiten mit 16 Garagenstellplätzen</v>
       </c>
       <c r="B7" s="18"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="str">
         <f>+Basisinformation!Y8</f>
-        <v>Gesamtinvestitionskosten: EUR 7750000 (gerundet)</v>
+        <v>Gesamtinvestitionskosten: EUR 0 (gerundet)</v>
       </c>
       <c r="B8" s="18"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="str">
         <f>+Basisinformation!Y9</f>
         <v>Prognostizierter Verkaufserlös: EUR 10270000; ø Verkaufspreis EUR 10000</v>
       </c>
       <c r="B9" s="18"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="str">
         <f>+Basisinformation!Y10</f>
-        <v>Gewinn: EUR 2500000 (gerundet ROI 32,5%)</v>
+        <v>Gewinn: EUR 10300000 (gerundet ROI 12051994.33%)</v>
       </c>
       <c r="B10" s="18"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="str">
         <f>+Basisinformation!Y11</f>
         <v>Ziel-Baubeginn: Q4/2025</v>
       </c>
       <c r="B11" s="18"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="str">
         <f>+Basisinformation!Y12</f>
         <v>Ziel-Fertigstellung: Q2/2026</v>
       </c>
       <c r="B12" s="18"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
     </row>
@@ -1154,15 +1136,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="10.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>78</v>
       </c>
@@ -1172,7 +1154,7 @@
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="45" t="s">
         <v>23</v>
       </c>
@@ -1184,77 +1166,77 @@
       <c r="E2" s="47"/>
       <c r="F2" s="48"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str" cm="1">
         <f t="array" ref="A3:C4">+'Mittelverwendung - Mittelherkun'!A3:C4</f>
         <v>Investitionskosten</v>
       </c>
-      <c r="B3" s="1">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9.1743119266055051E-2</v>
+      <c r="B3" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.09174311926605505</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F6">+'Mittelverwendung - Mittelherkun'!D3:F6</f>
         <v>Eigenkapital</v>
       </c>
-      <c r="E3" s="1">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="1" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <v>Finanzierungskosten</v>
       </c>
-      <c r="B4" s="16">
-        <v>99</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.90825688073394495</v>
+      <c r="B4" s="16" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0.908256880733945</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 1</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2.8571428571428571E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.02857142857142857</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="str">
         <v>Fremdkapital Tranche 2</v>
       </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>5.7142857142857141E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0.05714285714285714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="str">
         <v>BTVG Erlöse</v>
       </c>
-      <c r="E6" s="1">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>0.34285714285714286</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
@@ -1262,24 +1244,24 @@
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str" cm="1">
         <f t="array" ref="A8:C8">+'Mittelverwendung - Mittelherkun'!A8:C8</f>
         <v>Summe</v>
       </c>
-      <c r="B8" s="3">
-        <v>109</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
+      <c r="B8" s="3" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>1.0</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="10" cm="1">
+      <c r="E8" s="10" cm="1" t="n">
         <f t="array" ref="E8:F8">+'Mittelverwendung - Mittelherkun'!E8:F8</f>
-        <v>35</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
+        <v>35.0</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1300,15 +1282,15 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="10.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>78</v>
       </c>
@@ -1318,7 +1300,7 @@
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="46" t="s">
         <v>23</v>
       </c>
@@ -1330,91 +1312,91 @@
       <c r="E2" s="47"/>
       <c r="F2" s="48"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str" cm="1">
         <f t="array" ref="A3:C4">+'Mittelverwendung - Mittelherkun'!Q3:S4</f>
         <v>Investitionskosten</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.9801980198019802E-2</v>
+      <c r="B3" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.019801980198019802</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F7">+'Mittelverwendung - Mittelherkun'!T3:V7</f>
         <v>Eigenkapital</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.2345679012345678E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.012345679012345678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <v>Finanzierungskosten</v>
       </c>
-      <c r="B4" s="16">
-        <v>99</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.98019801980198018</v>
+      <c r="B4" s="16" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0.9801980198019802</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 1</v>
       </c>
-      <c r="E4" s="1">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>0.12345679012345678</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="str">
         <v>Fremdkapital Tranche 2</v>
       </c>
-      <c r="E5" s="1">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="1" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <v>0.2839506172839506</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="13" t="str">
         <v>Fremdkapital Tranche 3</v>
       </c>
-      <c r="E6" s="1">
-        <v>45</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.55555555555555558</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
       <c r="D7" s="13" t="str">
         <v>BTVG Erlöse</v>
       </c>
-      <c r="E7" s="1">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2.4691358024691357E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.024691358024691357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
@@ -1422,7 +1404,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
@@ -1430,24 +1412,24 @@
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str" cm="1">
         <f t="array" ref="A10:C10">+'Mittelverwendung - Mittelherkun'!Q9:S9</f>
         <v>Summe</v>
       </c>
-      <c r="B10" s="3">
-        <v>101</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
+      <c r="B10" s="3" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>1.0</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="10" cm="1">
+      <c r="E10" s="10" cm="1" t="n">
         <f t="array" ref="E10:F10">+'Mittelverwendung - Mittelherkun'!U9:V9</f>
-        <v>81</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
+        <v>81.0</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1468,15 +1450,15 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="10.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>78</v>
       </c>
@@ -1486,7 +1468,7 @@
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="45" t="s">
         <v>23</v>
       </c>
@@ -1498,105 +1480,105 @@
       <c r="E2" s="47"/>
       <c r="F2" s="48"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str" cm="1">
         <f t="array" ref="A3:C4">+'Mittelverwendung - Mittelherkun'!Y3:AA4</f>
         <v>Investitionskosten</v>
       </c>
-      <c r="B3" s="1">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9.1743119266055051E-2</v>
+      <c r="B3" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.09174311926605505</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F8">+'Mittelverwendung - Mittelherkun'!AB3:AD8</f>
         <v>Eigenkapital</v>
       </c>
-      <c r="E3" s="1">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="1" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>0.37735849056603776</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <v>Finanzierungskosten</v>
       </c>
-      <c r="B4" s="16">
-        <v>99</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.90825688073394495</v>
+      <c r="B4" s="16" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0.908256880733945</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 1</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.8867924528301886E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.018867924528301886</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="str">
         <v>Fremdkapital Tranche 2</v>
       </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>3.7735849056603772E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0.03773584905660377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="13" t="str">
         <v>Fremdkapital Tranche 3</v>
       </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5.6603773584905662E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.05660377358490566</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
       <c r="D7" s="13" t="str">
         <v>Fremdkapital Tranche 4</v>
       </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2">
-        <v>7.5471698113207544E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.07547169811320754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1" t="str">
         <v>BTVG Erlöse</v>
       </c>
-      <c r="E8" s="1">
-        <v>23</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.43396226415094341</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.4339622641509434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
@@ -1604,24 +1586,24 @@
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str" cm="1">
         <f t="array" ref="A10:C10">+'Mittelverwendung - Mittelherkun'!Y10:AA10</f>
         <v>Summe</v>
       </c>
-      <c r="B10" s="3">
-        <v>109</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
+      <c r="B10" s="3" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>1.0</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="10" cm="1">
+      <c r="E10" s="10" cm="1" t="n">
         <f t="array" ref="E10:F10">+'Mittelverwendung - Mittelherkun'!AC10:AD10</f>
-        <v>53</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
+        <v>53.0</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1642,15 +1624,15 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="10.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>78</v>
       </c>
@@ -1660,7 +1642,7 @@
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="45" t="s">
         <v>23</v>
       </c>
@@ -1672,119 +1654,119 @@
       <c r="E2" s="47"/>
       <c r="F2" s="48"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str" cm="1">
         <f t="array" ref="A3:C4">+'Mittelverwendung - Mittelherkun'!AG3:AI4</f>
         <v>Investitionskosten</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>0.01</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F9">+'Mittelverwendung - Mittelherkun'!AJ3:AL9</f>
         <v>Eigenkapital</v>
       </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.1428571428571429E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.011428571428571429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <v>Finanzierungskosten</v>
       </c>
-      <c r="B4" s="16">
-        <v>99</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="16" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>0.99</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 1</v>
       </c>
-      <c r="E4" s="1">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="1" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>0.13142857142857142</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="str">
         <v>Fremdkapital Tranche 2</v>
       </c>
-      <c r="E5" s="1">
-        <v>34</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="1" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <v>0.19428571428571428</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="13" t="str">
         <v>Fremdkapital Tranche 3</v>
       </c>
-      <c r="E6" s="1">
-        <v>89</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.50857142857142856</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.5085714285714286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
       <c r="D7" s="13" t="str">
         <v>Fremdkapital Tranche 4</v>
       </c>
-      <c r="E7" s="1">
-        <v>12</v>
-      </c>
-      <c r="F7" s="2">
-        <v>6.8571428571428575E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.06857142857142857</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="13" t="str">
         <v>Fremdkapital Tranche 5</v>
       </c>
-      <c r="E8" s="1">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2">
-        <v>6.8571428571428575E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.06857142857142857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="str">
         <v>BTVG Erlöse</v>
       </c>
-      <c r="E9" s="1">
-        <v>3</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.7142857142857144E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0.017142857142857144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
@@ -1792,24 +1774,24 @@
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str" cm="1">
         <f t="array" ref="A11:C11">+'Mittelverwendung - Mittelherkun'!AG11:AI11</f>
         <v>Summe</v>
       </c>
-      <c r="B11" s="3">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
+      <c r="B11" s="3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>1.0</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="10" cm="1">
+      <c r="E11" s="10" cm="1" t="n">
         <f t="array" ref="E11:F11">+'Mittelverwendung - Mittelherkun'!AK11:AL11</f>
-        <v>175</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
+        <v>175.0</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1828,24 +1810,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1863,16 +1845,16 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.5546875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="50.6640625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="35.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.54296875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.36328125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.54296875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="50.6328125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="35.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="41" t="s">
         <v>55</v>
       </c>
@@ -1896,7 +1878,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>84</v>
       </c>
@@ -1941,7 +1923,7 @@
         <v>Ankauf der Liegenschaft “Braumüllergasse 21” in Form eines Asset Deals mit einer eigens gegründeten Projektgesellschaft</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>80</v>
       </c>
@@ -1984,7 +1966,7 @@
         <v>Kaufpreis: EUR 10</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>81</v>
       </c>
@@ -2035,7 +2017,7 @@
         <v>Bebauungsbestimmungen: G; Widmung: W II gk</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
@@ -2064,9 +2046,9 @@
       <c r="T5" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U5" s="18" t="n">
         <f>+Basisinformation!B3</f>
-        <v>797</v>
+        <v>797.0</v>
       </c>
       <c r="V5" s="18" t="s">
         <v>97</v>
@@ -2078,7 +2060,7 @@
         <v>Grundstücksgröße: 797 m²</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>1</v>
       </c>
@@ -2103,16 +2085,16 @@
       <c r="T6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="18" t="n">
         <f>+Basisinformation!B4</f>
-        <v>800</v>
+        <v>800.0</v>
       </c>
       <c r="V6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="W6" s="18">
+      <c r="W6" s="18" t="n">
         <f>+Basisinformation!B7</f>
-        <v>160</v>
+        <v>160.0</v>
       </c>
       <c r="X6" s="18" t="s">
         <v>97</v>
@@ -2122,7 +2104,7 @@
         <v>Erzielbare Wohnnutzfläche laut Architekt: 800 m² WNFL zzgl. gew. Außenflächen von 160 m²</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>82</v>
       </c>
@@ -2150,16 +2132,16 @@
       <c r="T7" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="18" t="n">
         <f>+Basisinformation!B5</f>
-        <v>8</v>
+        <v>8.0</v>
       </c>
       <c r="V7" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="W7" s="18">
+      <c r="W7" s="18" t="n">
         <f>+Basisinformation!B6</f>
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="X7" s="18" t="s">
         <v>102</v>
@@ -2169,7 +2151,7 @@
         <v>Nutzung: 8 Wohneinheiten mit 16 Garagenstellplätzen</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>2</v>
       </c>
@@ -2190,9 +2172,9 @@
       <c r="T8" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="18" t="n">
         <f>+ROUND(Gesamtinvestitionskosten!E15,-4)</f>
-        <v>7750000</v>
+        <v>0.0</v>
       </c>
       <c r="V8" s="18" t="s">
         <v>104</v>
@@ -2201,10 +2183,10 @@
       <c r="X8" s="18"/>
       <c r="Y8" t="str">
         <f t="shared" si="0"/>
-        <v>Gesamtinvestitionskosten: EUR 7750000 (gerundet)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+        <v>Gesamtinvestitionskosten: EUR 0 (gerundet)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -2225,16 +2207,16 @@
       <c r="T9" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="U9" s="18">
+      <c r="U9" s="18" t="n">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!E20,-4)</f>
-        <v>10270000</v>
+        <v>1.027E7</v>
       </c>
       <c r="V9" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="W9" s="29">
+      <c r="W9" s="29" t="n">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!F4,0)</f>
-        <v>10000</v>
+        <v>10000.0</v>
       </c>
       <c r="X9" s="18"/>
       <c r="Y9" t="str">
@@ -2242,7 +2224,7 @@
         <v>Prognostizierter Verkaufserlös: EUR 10270000; ø Verkaufspreis EUR 10000</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="30"/>
       <c r="B10" s="30"/>
       <c r="C10" s="18"/>
@@ -2258,26 +2240,26 @@
       <c r="T10" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="U10" s="18">
+      <c r="U10" s="18" t="n">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!E22,-5)</f>
-        <v>2500000</v>
+        <v>1.03E7</v>
       </c>
       <c r="V10" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="W10" s="20">
+      <c r="W10" s="20" t="n">
         <f>+Wirtschaftlichkeitsrechnung!E23</f>
-        <v>0.32498359765242629</v>
+        <v>120519.94332981344</v>
       </c>
       <c r="X10" s="18" t="s">
         <v>112</v>
       </c>
       <c r="Y10" t="str">
         <f>+CONCATENATE(T10,U10,V10,ROUND(W10*100,2),X10)</f>
-        <v>Gewinn: EUR 2500000 (gerundet ROI 32,5%)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+        <v>Gewinn: EUR 10300000 (gerundet ROI 12051994.33%)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="30"/>
       <c r="B11" s="30"/>
       <c r="C11" s="23"/>
@@ -2305,7 +2287,7 @@
         <v>Ziel-Baubeginn: Q4/2025</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="30"/>
       <c r="B12" s="4"/>
       <c r="C12" s="1"/>
@@ -2343,20 +2325,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.90625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.90625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.90625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.08984375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>113</v>
       </c>
@@ -2370,7 +2352,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -2381,10 +2363,10 @@
         <v>8</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
@@ -2395,10 +2377,10 @@
         <v>8</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>66</v>
       </c>
@@ -2409,10 +2391,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -2423,34 +2405,34 @@
         <v>8</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="F7" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="F8" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="14"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="F9" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2458,7 +2440,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -2466,7 +2448,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -2474,7 +2456,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -2495,64 +2477,70 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.6328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="30.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.08984375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F3),"",Standort!F3)</f>
-        <v>Bestlage im 17. Bezirk</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>
+</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F4),"",Standort!F4)</f>
-        <v>Absolute Ruhelage, mit Fernblick über Wien</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>
+</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F5),"",Standort!F5)</f>
-        <v>Zentrum Wien 18 Autominuten, öffentlich 25 Minuten</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>
+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F6),"",Standort!F6)</f>
-        <v>Nahversorgung, Restaurants u. Geschäfte des täglichen Bedarfs in unmittelbarer Nähe</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>
+</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F7),"",Standort!F7)</f>
-        <v>Nahversorgung, Restaurants u. Geschäfte dees täglichen Bedarfs in unmittelbarer Nähe</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>
+</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F8),"",Standort!F8)</f>
-        <v>Nahversorgung, Restaurants u. Geschäfte deees täglichen Bedarfs in unmittelbarer Nähe</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>
+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>113</v>
       </c>
@@ -2569,63 +2557,63 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="n">
         <f>+Standort!B3</f>
-        <v>8</v>
-      </c>
-      <c r="C11" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <f>+Standort!B3</f>
-        <v>8</v>
-      </c>
-      <c r="D11" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <f>+Standort!B5</f>
-        <v>8</v>
-      </c>
-      <c r="E11" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="E11" s="1" t="n">
         <f>+Standort!B6</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <f>+Standort!C3</f>
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="C12" s="1" t="n">
         <f>+Standort!C4</f>
-        <v>8</v>
-      </c>
-      <c r="D12" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="D12" s="1" t="n">
         <f>+Standort!C5</f>
-        <v>8</v>
-      </c>
-      <c r="E12" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="E12" s="1" t="n">
         <f>+Standort!C6</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2633,7 +2621,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2641,7 +2629,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2649,7 +2637,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -2657,7 +2645,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -2665,7 +2653,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -2686,64 +2674,64 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="32.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="24" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="str">
         <f>+CONCATENATE(Basisinformation!I3,", ",Basisinformation!I4," ",Basisinformation!I5)</f>
         <v>Braumüllergasse 21, 1170 Wien</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="str" cm="1">
         <f t="array" ref="A3:A4">+Basisinformation!O2:O3</f>
         <v>W II = Bauklasse 2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="str">
         <v>gk = gekuppelte Bauweise</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="27" t="str">
         <f>+IF(ISBLANK(Basisinformation!O4),"",Basisinformation!O4)</f>
         <v>G = Gärtnerische Ausgestaltung</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="str">
         <f>+IF(ISBLANK(Basisinformation!O5),"",Basisinformation!O5)</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="str">
         <f>+IF(ISBLANK(Basisinformation!O6),"",Basisinformation!O6)</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="str">
         <f>+IF(ISBLANK(Basisinformation!O7),"",Basisinformation!O7)</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="str">
         <f>+IF(ISBLANK(Basisinformation!O8),"",Basisinformation!O8)</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="str">
         <f>+IF(ISBLANK(Basisinformation!O9),"",Basisinformation!O9)</f>
         <v/>
@@ -2759,17 +2747,17 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.08984375" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.90625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -2780,7 +2768,7 @@
       <c r="F1" s="44"/>
       <c r="G1" s="44"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="8"/>
       <c r="B2" s="8" t="s">
         <v>4</v>
@@ -2799,230 +2787,231 @@
       </c>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>2530800</v>
-      </c>
-      <c r="C3" s="3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <f>B3*B22</f>
-        <v>25308</v>
-      </c>
-      <c r="D3" s="17">
+        <v>2.2</v>
+      </c>
+      <c r="D3" s="17" t="n">
         <f>+B22</f>
-        <v>0.01</v>
-      </c>
-      <c r="E3" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="E3" s="3" t="n">
         <f t="shared" ref="E3:E11" si="0">B3+C3</f>
-        <v>2556108</v>
-      </c>
-      <c r="F3" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <f t="shared" ref="F3:F11" si="1">$E3/$E$15</f>
-        <v>0.32971195228077765</v>
+        <v>0.1431420861199108</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1">
-        <v>85892</v>
-      </c>
-      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <f t="shared" ref="C4:C10" si="2">B4*$B$21</f>
-        <v>17178.400000000001</v>
-      </c>
-      <c r="D4" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="D4" s="6" t="n">
         <f t="shared" ref="D4:D10" si="3">C4/B4</f>
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>103070.39999999999</v>
-      </c>
-      <c r="F4" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.329503401513577E-2</v>
+        <v>0.015604833978646017</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>2475206</v>
-      </c>
-      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <f>B5*$B$21</f>
-        <v>495041.2</v>
-      </c>
-      <c r="D5" s="6">
+        <v>0.66</v>
+      </c>
+      <c r="D5" s="6" t="n">
         <f>C5/B5</f>
-        <v>0.2</v>
-      </c>
-      <c r="E5" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>2970247.2</v>
-      </c>
-      <c r="F5" s="2">
+        <v>2.66</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.38313169986108314</v>
+        <v>0.031209667957292034</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>212558</v>
-      </c>
-      <c r="C6" s="3">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>42511.600000000006</v>
-      </c>
-      <c r="D6" s="6">
+        <v>1.98</v>
+      </c>
+      <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.20000000000000004</v>
-      </c>
-      <c r="E6" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>255069.6</v>
-      </c>
-      <c r="F6" s="2">
+        <v>7.98</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>3.2901385928715471E-2</v>
+        <v>0.0936290038718761</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>612366</v>
-      </c>
-      <c r="C7" s="3">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>122473.20000000001</v>
-      </c>
-      <c r="D7" s="6">
+        <v>2.31</v>
+      </c>
+      <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="E7" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>734839.2</v>
-      </c>
-      <c r="F7" s="2">
+        <v>9.31</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>9.4786788056077764E-2</v>
+        <v>0.10923383785052211</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>39881</v>
-      </c>
-      <c r="C8" s="3">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>7976.2000000000007</v>
-      </c>
-      <c r="D8" s="6">
+        <v>2.64</v>
+      </c>
+      <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>47857.2</v>
-      </c>
-      <c r="F8" s="2">
+        <v>10.64</v>
+      </c>
+      <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>6.1730923899505153E-3</v>
+        <v>0.12483867182916814</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>101581</v>
-      </c>
-      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>20316.2</v>
-      </c>
-      <c r="D9" s="6">
+        <v>2.97</v>
+      </c>
+      <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>121897.2</v>
-      </c>
-      <c r="F9" s="2">
+        <v>11.97</v>
+      </c>
+      <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>1.572349986368354E-2</v>
+        <v>0.14044350580781415</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>52000</v>
-      </c>
-      <c r="C10" s="3">
-        <f t="shared" si="2"/>
-        <v>10400</v>
-      </c>
-      <c r="D10" s="6">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <f>B10*$B$21</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="D10" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="E10" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>62400</v>
-      </c>
-      <c r="F10" s="2">
+        <v>13.3</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>8.0489657801315617E-3</v>
+        <v>0.15604833978646016</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="9">
-        <v>901060</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <f>+B11*D11</f>
+        <v>4.84</v>
       </c>
       <c r="D11" s="6">
-        <v>0.12</v>
-      </c>
-      <c r="E11" s="3">
+        <v>0.44</v>
+      </c>
+      <c r="E11" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>901060</v>
-      </c>
-      <c r="F11" s="2">
+        <v>15.84</v>
+      </c>
+      <c r="F11" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.11622758182444463</v>
+        <v>0.18585005279831043</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -3031,33 +3020,33 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="3" t="n">
         <f>SUM(B3:B11)</f>
-        <v>7011344</v>
-      </c>
-      <c r="C13" s="3">
+        <v>64.0</v>
+      </c>
+      <c r="C13" s="3" t="n">
         <f>SUM(C3:C11)</f>
-        <v>741204.79999999981</v>
-      </c>
-      <c r="D13" s="4">
+        <v>21.23</v>
+      </c>
+      <c r="D13" s="4" t="n">
         <f>C13/B13</f>
-        <v>0.10571508115990312</v>
-      </c>
-      <c r="E13" s="10">
+        <v>0.33171875</v>
+      </c>
+      <c r="E13" s="10" t="n">
         <f>B13+C13</f>
-        <v>7752548.7999999998</v>
-      </c>
-      <c r="F13" s="4">
+        <v>85.23</v>
+      </c>
+      <c r="F13" s="4" t="n">
         <f>SUM(F3:F11)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -3068,33 +3057,33 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="3" t="n">
         <f>B13</f>
-        <v>7011344</v>
-      </c>
-      <c r="C15" s="3">
+        <v>64.0</v>
+      </c>
+      <c r="C15" s="3" t="n">
         <f>C13</f>
-        <v>741204.79999999981</v>
-      </c>
-      <c r="D15" s="3">
+        <v>21.23</v>
+      </c>
+      <c r="D15" s="3" t="n">
         <f>D13</f>
-        <v>0.10571508115990312</v>
-      </c>
-      <c r="E15" s="10">
+        <v>0.33171875</v>
+      </c>
+      <c r="E15" s="10" t="n">
         <f>E13</f>
-        <v>7752548.7999999998</v>
-      </c>
-      <c r="F15" s="4">
+        <v>85.23</v>
+      </c>
+      <c r="F15" s="4" t="n">
         <f>F13</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -3103,7 +3092,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -3112,7 +3101,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -3121,20 +3110,20 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="12">
-        <v>0.01</v>
+        <v>0.22</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -3156,31 +3145,31 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="37" max="38" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="26" max="27" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="29" max="30" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="34" max="35" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="37" max="38" customWidth="true" width="10.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>78</v>
       </c>
@@ -3222,7 +3211,7 @@
       <c r="AK1" s="44"/>
       <c r="AL1" s="44"/>
     </row>
-    <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="45" t="s">
         <v>23</v>
       </c>
@@ -3274,16 +3263,16 @@
       <c r="AK2" s="47"/>
       <c r="AL2" s="48"/>
     </row>
-    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <f>$B3/$B8</f>
-        <v>9.1743119266055051E-2</v>
+        <v>0.09174311926605505</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
@@ -3291,7 +3280,7 @@
       <c r="E3" s="1">
         <v>20</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <f>$E3/$E8</f>
         <v>0.5714285714285714</v>
       </c>
@@ -3301,9 +3290,9 @@
       <c r="J3" s="1">
         <v>123</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="2" t="n">
         <f>$J3/$J7</f>
-        <v>0.55405405405405406</v>
+        <v>0.5540540540540541</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>26</v>
@@ -3311,7 +3300,7 @@
       <c r="M3" s="1">
         <v>234</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="2" t="n">
         <f>$M3/$M7</f>
         <v>0.20689655172413793</v>
       </c>
@@ -3321,9 +3310,9 @@
       <c r="R3" s="1">
         <v>2</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="2" t="n">
         <f>$R3/$R9</f>
-        <v>1.9801980198019802E-2</v>
+        <v>0.019801980198019802</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>26</v>
@@ -3331,9 +3320,9 @@
       <c r="U3" s="1">
         <v>1</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3" s="2" t="n">
         <f>$U3/$U9</f>
-        <v>1.2345679012345678E-2</v>
+        <v>0.012345679012345678</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>25</v>
@@ -3341,9 +3330,9 @@
       <c r="Z3" s="1">
         <v>10</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3" s="2" t="n">
         <f>$Z3/$Z10</f>
-        <v>9.1743119266055051E-2</v>
+        <v>0.09174311926605505</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>26</v>
@@ -3351,7 +3340,7 @@
       <c r="AC3" s="1">
         <v>20</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AD3" s="2" t="n">
         <f>$AC3/$AC10</f>
         <v>0.37735849056603776</v>
       </c>
@@ -3361,7 +3350,7 @@
       <c r="AH3" s="1">
         <v>1</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AI3" s="2" t="n">
         <f>$AH3/$AH11</f>
         <v>0.01</v>
       </c>
@@ -3371,21 +3360,21 @@
       <c r="AK3" s="1">
         <v>2</v>
       </c>
-      <c r="AL3" s="2">
+      <c r="AL3" s="2" t="n">
         <f>$AK3/$AK11</f>
-        <v>1.1428571428571429E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.011428571428571429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="16">
         <v>99</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <f>$B4/$B8</f>
-        <v>0.90825688073394495</v>
+        <v>0.908256880733945</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>58</v>
@@ -3393,9 +3382,9 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <f>$E4/$E8</f>
-        <v>2.8571428571428571E-2</v>
+        <v>0.02857142857142857</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>27</v>
@@ -3403,7 +3392,7 @@
       <c r="J4" s="16">
         <v>99</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="2" t="n">
         <f>$J4/$J7</f>
         <v>0.44594594594594594</v>
       </c>
@@ -3413,9 +3402,9 @@
       <c r="M4" s="1">
         <v>555</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="2" t="n">
         <f>$M4/$M7</f>
-        <v>0.49071618037135278</v>
+        <v>0.4907161803713528</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>27</v>
@@ -3423,9 +3412,9 @@
       <c r="R4" s="16">
         <v>99</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="2" t="n">
         <f>$R4/$R9</f>
-        <v>0.98019801980198018</v>
+        <v>0.9801980198019802</v>
       </c>
       <c r="T4" s="13" t="s">
         <v>58</v>
@@ -3433,7 +3422,7 @@
       <c r="U4" s="1">
         <v>10</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="2" t="n">
         <f>$U4/$U9</f>
         <v>0.12345679012345678</v>
       </c>
@@ -3443,9 +3432,9 @@
       <c r="Z4" s="16">
         <v>99</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4" s="2" t="n">
         <f>$Z4/$Z10</f>
-        <v>0.90825688073394495</v>
+        <v>0.908256880733945</v>
       </c>
       <c r="AB4" s="13" t="s">
         <v>58</v>
@@ -3453,9 +3442,9 @@
       <c r="AC4" s="1">
         <v>1</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD4" s="2" t="n">
         <f>$AC4/$AC10</f>
-        <v>1.8867924528301886E-2</v>
+        <v>0.018867924528301886</v>
       </c>
       <c r="AG4" s="1" t="s">
         <v>27</v>
@@ -3463,7 +3452,7 @@
       <c r="AH4" s="16">
         <v>99</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AI4" s="2" t="n">
         <f>$AH4/$AH11</f>
         <v>0.99</v>
       </c>
@@ -3473,12 +3462,12 @@
       <c r="AK4" s="1">
         <v>23</v>
       </c>
-      <c r="AL4" s="2">
+      <c r="AL4" s="2" t="n">
         <f>$AK4/$AK11</f>
         <v>0.13142857142857142</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
@@ -3488,9 +3477,9 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <f>$E5/$E8</f>
-        <v>5.7142857142857141E-2</v>
+        <v>0.05714285714285714</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -3501,7 +3490,7 @@
       <c r="M5" s="1">
         <v>342</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="2" t="n">
         <f>$M5/$M7</f>
         <v>0.30238726790450926</v>
       </c>
@@ -3514,7 +3503,7 @@
       <c r="U5" s="1">
         <v>23</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="2" t="n">
         <f>$U5/$U9</f>
         <v>0.2839506172839506</v>
       </c>
@@ -3527,9 +3516,9 @@
       <c r="AC5" s="1">
         <v>2</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5" s="2" t="n">
         <f>$AC5/$AC10</f>
-        <v>3.7735849056603772E-2</v>
+        <v>0.03773584905660377</v>
       </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
@@ -3540,12 +3529,12 @@
       <c r="AK5" s="1">
         <v>34</v>
       </c>
-      <c r="AL5" s="2">
+      <c r="AL5" s="2" t="n">
         <f>$AK5/$AK11</f>
         <v>0.19428571428571428</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
@@ -3555,7 +3544,7 @@
       <c r="E6" s="1">
         <v>12</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <f>$E6/$E8</f>
         <v>0.34285714285714286</v>
       </c>
@@ -3574,9 +3563,9 @@
       <c r="U6" s="1">
         <v>45</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6" s="2" t="n">
         <f>$U6/$U9</f>
-        <v>0.55555555555555558</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
@@ -3587,9 +3576,9 @@
       <c r="AC6" s="1">
         <v>3</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD6" s="2" t="n">
         <f>$AC6/$AC10</f>
-        <v>5.6603773584905662E-2</v>
+        <v>0.05660377358490566</v>
       </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
@@ -3600,12 +3589,12 @@
       <c r="AK6" s="1">
         <v>89</v>
       </c>
-      <c r="AL6" s="2">
+      <c r="AL6" s="2" t="n">
         <f>$AK6/$AK11</f>
-        <v>0.50857142857142856</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.5085714285714286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
@@ -3615,22 +3604,22 @@
       <c r="I7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="3" t="n">
         <f>SUM(J3:J6)</f>
-        <v>222</v>
-      </c>
-      <c r="K7" s="4">
+        <v>222.0</v>
+      </c>
+      <c r="K7" s="4" t="n">
         <f>SUM(K3:K6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="L7" s="3"/>
-      <c r="M7" s="10">
+      <c r="M7" s="10" t="n">
         <f>SUM(M3:M6)</f>
-        <v>1131</v>
-      </c>
-      <c r="N7" s="4">
+        <v>1131.0</v>
+      </c>
+      <c r="N7" s="4" t="n">
         <f>SUM(N3:N6)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -3641,9 +3630,9 @@
       <c r="U7" s="1">
         <v>2</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7" s="2" t="n">
         <f>$U7/$U9</f>
-        <v>2.4691358024691357E-2</v>
+        <v>0.024691358024691357</v>
       </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
@@ -3654,9 +3643,9 @@
       <c r="AC7" s="1">
         <v>4</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AD7" s="2" t="n">
         <f>$AC7/$AC10</f>
-        <v>7.5471698113207544E-2</v>
+        <v>0.07547169811320754</v>
       </c>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
@@ -3667,31 +3656,31 @@
       <c r="AK7" s="1">
         <v>12</v>
       </c>
-      <c r="AL7" s="2">
+      <c r="AL7" s="2" t="n">
         <f>$AK7/$AK11</f>
-        <v>6.8571428571428575E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.06857142857142857</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="3" t="n">
         <f>SUM(B3:B7)</f>
-        <v>109</v>
-      </c>
-      <c r="C8" s="4">
+        <v>109.0</v>
+      </c>
+      <c r="C8" s="4" t="n">
         <f>SUM(C3:C7)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="10">
+      <c r="E8" s="10" t="n">
         <f>SUM(E3:E7)</f>
-        <v>35</v>
-      </c>
-      <c r="F8" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="F8" s="4" t="n">
         <f>SUM(F3:F7)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -3708,9 +3697,9 @@
       <c r="AC8" s="1">
         <v>23</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AD8" s="2" t="n">
         <f>$AC8/$AC10</f>
-        <v>0.43396226415094341</v>
+        <v>0.4339622641509434</v>
       </c>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
@@ -3721,31 +3710,31 @@
       <c r="AK8" s="1">
         <v>12</v>
       </c>
-      <c r="AL8" s="2">
+      <c r="AL8" s="2" t="n">
         <f>$AK8/$AK11</f>
-        <v>6.8571428571428575E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.06857142857142857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Q9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="3" t="n">
         <f>SUM(R3:R8)</f>
-        <v>101</v>
-      </c>
-      <c r="S9" s="4">
+        <v>101.0</v>
+      </c>
+      <c r="S9" s="4" t="n">
         <f>SUM(S3:S8)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="T9" s="3"/>
-      <c r="U9" s="10">
+      <c r="U9" s="10" t="n">
         <f>SUM(U3:U8)</f>
-        <v>81</v>
-      </c>
-      <c r="V9" s="4">
+        <v>81.0</v>
+      </c>
+      <c r="V9" s="4" t="n">
         <f>SUM(V3:V8)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -3762,31 +3751,31 @@
       <c r="AK9" s="1">
         <v>3</v>
       </c>
-      <c r="AL9" s="2">
+      <c r="AL9" s="2" t="n">
         <f>$AK9/$AK11</f>
-        <v>1.7142857142857144E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.017142857142857144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Y10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Z10" s="3">
+      <c r="Z10" s="3" t="n">
         <f>SUM(Z3:Z9)</f>
-        <v>109</v>
-      </c>
-      <c r="AA10" s="4">
+        <v>109.0</v>
+      </c>
+      <c r="AA10" s="4" t="n">
         <f>SUM(AA3:AA9)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="10">
+      <c r="AC10" s="10" t="n">
         <f>SUM(AC3:AC9)</f>
-        <v>53</v>
-      </c>
-      <c r="AD10" s="4">
+        <v>53.0</v>
+      </c>
+      <c r="AD10" s="4" t="n">
         <f>SUM(AD3:AD9)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
@@ -3795,29 +3784,29 @@
       <c r="AK10" s="1"/>
       <c r="AL10" s="2"/>
     </row>
-    <row r="11" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AG11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AH11" s="3">
+      <c r="AH11" s="3" t="n">
         <f>SUM(AH3:AH10)</f>
-        <v>100</v>
-      </c>
-      <c r="AI11" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="AI11" s="4" t="n">
         <f>SUM(AI3:AI10)</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AJ11" s="3"/>
-      <c r="AK11" s="10">
+      <c r="AK11" s="10" t="n">
         <f>SUM(AK3:AK10)</f>
-        <v>175</v>
-      </c>
-      <c r="AL11" s="4">
+        <v>175.0</v>
+      </c>
+      <c r="AL11" s="4" t="n">
         <f>SUM(AL3:AL10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="G12" s="1" t="s">
         <v>63</v>
       </c>
@@ -3827,11 +3816,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="Y1:AD1"/>
-    <mergeCell ref="AG1:AL1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="AB2:AD2"/>
@@ -3842,6 +3826,11 @@
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Y1:AD1"/>
+    <mergeCell ref="AG1:AL1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3851,22 +3840,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB0A179-3460-4B7F-B6A0-F84428E1F30B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="42.90625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.08984375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.6328125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>79</v>
       </c>
@@ -3879,7 +3868,7 @@
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
     </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
@@ -3902,7 +3891,7 @@
       </c>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -3918,61 +3907,61 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="34">
+      <c r="E4" s="34" t="n">
         <f>+F4/1.1</f>
-        <v>9090.9090909090901</v>
+        <v>9090.90909090909</v>
       </c>
       <c r="F4" s="33">
         <v>10000</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="34">
+      <c r="H4" s="34" t="n">
         <f>+E4*1.2</f>
         <v>10909.090909090908</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="37">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <f>+B5*C7</f>
-        <v>960</v>
+        <v>960.0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>86</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="3">
+      <c r="F5" s="3" t="n">
         <f>+F4*C5</f>
-        <v>9600000</v>
+        <v>9600000.0</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="36" t="n">
         <f>1-B5</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <f>+B6*C7</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>86</v>
@@ -3982,23 +3971,23 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="3">
+      <c r="H6" s="3" t="n">
         <f>+H4*C6</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="36" t="n">
         <f>B5+B6</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="35" t="n">
         <f>+Basisinformation!B4+Basisinformation!B7</f>
-        <v>960</v>
+        <v>960.0</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>86</v>
@@ -4006,21 +3995,21 @@
       <c r="E7" s="40">
         <v>0</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="3" t="n">
         <f>+F5</f>
-        <v>9600000</v>
-      </c>
-      <c r="G7" s="38">
+        <v>9600000.0</v>
+      </c>
+      <c r="G7" s="38" t="n">
         <f>+H7+F7</f>
-        <v>9600000</v>
-      </c>
-      <c r="H7" s="3">
+        <v>9600000.0</v>
+      </c>
+      <c r="H7" s="3" t="n">
         <f>+H6</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4031,7 +4020,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>38</v>
       </c>
@@ -4044,55 +4033,55 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="28">
+      <c r="E10" s="28" t="n">
         <f>+F10/1.1</f>
-        <v>38181.818181818177</v>
+        <v>38181.81818181818</v>
       </c>
       <c r="F10" s="16">
         <v>42000</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="39">
+      <c r="H10" s="39" t="n">
         <f>+E10*1.2</f>
-        <v>45818.181818181809</v>
+        <v>45818.18181818181</v>
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="15" t="n">
         <f>+C11/C13</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C11" s="16">
         <v>16</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="3">
+      <c r="F11" s="3" t="n">
         <f>+F10*C11</f>
-        <v>672000</v>
+        <v>672000.0</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="15" t="n">
         <f>+C12/C13</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="C12" s="16">
         <v>0</v>
@@ -4103,43 +4092,43 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="3">
+      <c r="H12" s="3" t="n">
         <f>+H10*C12</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="15" t="n">
         <f>+B11+B12</f>
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <f>+C11+C12</f>
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="40">
         <v>0</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="3" t="n">
         <f>F11</f>
-        <v>672000</v>
-      </c>
-      <c r="G13" s="38">
+        <v>672000.0</v>
+      </c>
+      <c r="G13" s="38" t="n">
         <f>+F13+H13</f>
-        <v>672000</v>
-      </c>
-      <c r="H13" s="3">
+        <v>672000.0</v>
+      </c>
+      <c r="H13" s="3" t="n">
         <f>+H12</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -4150,7 +4139,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4161,7 +4150,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -4172,7 +4161,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="49" t="s">
         <v>39</v>
@@ -4191,7 +4180,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -4200,22 +4189,22 @@
       <c r="D18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="3" t="n">
         <f>+G7</f>
-        <v>9600000</v>
-      </c>
-      <c r="F18" s="2">
+        <v>9600000.0</v>
+      </c>
+      <c r="F18" s="2" t="n">
         <f>$E18/$E$20</f>
-        <v>0.93457943925233644</v>
-      </c>
-      <c r="G18" s="3">
+        <v>0.9345794392523364</v>
+      </c>
+      <c r="G18" s="3" t="n">
         <f>+G7/C7</f>
-        <v>10000</v>
+        <v>10000.0</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -4224,86 +4213,86 @@
       <c r="D19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="3" t="n">
         <f>+G13</f>
-        <v>672000</v>
-      </c>
-      <c r="F19" s="2">
+        <v>672000.0</v>
+      </c>
+      <c r="F19" s="2" t="n">
         <f>$E19/$E$20</f>
-        <v>6.5420560747663545E-2</v>
-      </c>
-      <c r="G19" s="3">
+        <v>0.06542056074766354</v>
+      </c>
+      <c r="G19" s="3" t="n">
         <f>+G13/C13</f>
-        <v>42000</v>
+        <v>42000.0</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="3">
+      <c r="E20" s="3" t="n">
         <f>SUM(E18:E19)</f>
-        <v>10272000</v>
+        <v>1.0272E7</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="9" t="n">
         <f>+Gesamtinvestitionskosten!E15</f>
-        <v>7752548.7999999998</v>
+        <v>85.23</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="3" t="n">
         <f>E20-E21</f>
-        <v>2519451.2000000002</v>
+        <v>1.027191477E7</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="2" t="n">
         <f>E22/E21</f>
-        <v>0.32498359765242629</v>
+        <v>120519.94332981344</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -4314,7 +4303,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4325,7 +4314,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -4353,15 +4342,15 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="10.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.6328125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="10.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>78</v>
       </c>
@@ -4371,7 +4360,7 @@
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="45" t="s">
         <v>23</v>
       </c>
@@ -4383,42 +4372,42 @@
       <c r="E2" s="47"/>
       <c r="F2" s="48"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
         <f>+'Mittelverwendung - Mittelherkun'!I3</f>
         <v>Investitionskosten</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!J3</f>
-        <v>123</v>
-      </c>
-      <c r="C3" s="2">
+        <v>123.0</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K3</f>
-        <v>0.55405405405405406</v>
+        <v>0.5540540540540541</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>+'Mittelverwendung - Mittelherkun'!L3</f>
         <v>Eigenkapital</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="1" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!M3</f>
-        <v>234</v>
-      </c>
-      <c r="F3" s="2" cm="1">
+        <v>234.0</v>
+      </c>
+      <c r="F3" s="2" cm="1" t="n">
         <f t="array" ref="F3:F5">+'Mittelverwendung - Mittelherkun'!N3:N5</f>
         <v>0.20689655172413793</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <f>+'Mittelverwendung - Mittelherkun'!I4</f>
         <v>Finanzierungskosten</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="16" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!J4</f>
-        <v>99</v>
-      </c>
-      <c r="C4" s="2">
+        <v>99.0</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K4</f>
         <v>0.44594594594594594</v>
       </c>
@@ -4426,15 +4415,15 @@
         <f>+'Mittelverwendung - Mittelherkun'!L4</f>
         <v>Fremdkapital Tranche 1</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="1" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!M4</f>
-        <v>555</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.49071618037135278</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>555.0</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.4907161803713528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
@@ -4442,15 +4431,15 @@
         <f>+'Mittelverwendung - Mittelherkun'!L5</f>
         <v>BTVG Erlöse</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="1" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!M5</f>
-        <v>342</v>
-      </c>
-      <c r="F5" s="2">
+        <v>342.0</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <v>0.30238726790450926</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
@@ -4458,27 +4447,27 @@
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <f>+'Mittelverwendung - Mittelherkun'!I7</f>
         <v>Summe</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!J7</f>
-        <v>222</v>
-      </c>
-      <c r="C7" s="4">
+        <v>222.0</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K7</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10">
+      <c r="E7" s="10" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!M7</f>
-        <v>1131</v>
-      </c>
-      <c r="F7" s="4">
+        <v>1131.0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!N7</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -4492,6 +4481,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -4655,37 +4661,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4707,9 +4686,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
test pdf: Finanzierungskosten Fehler behoben im Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43677\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646AB3D-577E-4F4C-9685-7B8E95F225D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89F1170-C67A-4F4C-B19C-67B2AC4E1054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="7" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="11" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
   <sheets>
     <sheet name="Executive Summary" sheetId="22" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="128">
   <si>
     <t>Wohneinheiten</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Wien</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Tranche</t>
   </si>
   <si>
@@ -287,21 +284,12 @@
   </si>
   <si>
     <t>1170</t>
-  </si>
-  <si>
-    <t>W II = Bauklasse 2</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>gk = gekuppelte Bauweise</t>
-  </si>
-  <si>
     <t>Braumüllergasse 21</t>
   </si>
   <si>
@@ -401,12 +389,6 @@
     <t xml:space="preserve">Ziel-Fertigstellung: </t>
   </si>
   <si>
-    <t>Q4/2025</t>
-  </si>
-  <si>
-    <t>Q2/2026</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (gerundet ROI </t>
   </si>
   <si>
@@ -447,6 +429,33 @@
   </si>
   <si>
     <t>Bank Book</t>
+  </si>
+  <si>
+    <t>Absolute Ruhelage, mit Fernblick über Wien</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 1 bis Baubeginn</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 2 ab Baubeginn</t>
+  </si>
+  <si>
+    <t>W I = Bauklasse 1 beschränkt auf 6,5 Meter</t>
+  </si>
+  <si>
+    <t>o = offene Bauweise</t>
+  </si>
+  <si>
+    <t>Bestlage 17.Bezirk</t>
+  </si>
+  <si>
+    <t>Zentru, Wien 18 Autominuten, öffentlich 25 Minuten</t>
+  </si>
+  <si>
+    <t>Nahversorgung, Restaurants u. Geschäfte des täglichen Bedarfs in unmittelbarere Nähe</t>
+  </si>
+  <si>
+    <t>Perfekte öffentliche Anbindung, 7 Gehminuten über Rebenweg</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1058,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B1" s="26"/>
     </row>
@@ -1068,9 +1077,9 @@
       <c r="B3" s="18"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="str">
+      <c r="A4" s="18" t="e">
         <f>+Basisinformation!Y4</f>
-        <v>Bebauungsbestimmungen: G; Widmung: W II gk</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B4" s="22"/>
     </row>
@@ -1098,7 +1107,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="str">
         <f>+Basisinformation!Y8</f>
-        <v>Gesamtinvestitionskosten: EUR 0 (gerundet)</v>
+        <v>Gesamtinvestitionskosten: EUR 7750000 (gerundet)</v>
       </c>
       <c r="B8" s="18"/>
     </row>
@@ -1112,7 +1121,7 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="str">
         <f>+Basisinformation!Y10</f>
-        <v>Gewinn: EUR 10300000 (gerundet ROI 12051994.33%)</v>
+        <v>Gewinn: EUR 2500000 (gerundet ROI 32.5%)</v>
       </c>
       <c r="B10" s="18"/>
     </row>
@@ -1173,7 +1182,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1199,20 +1208,20 @@
         <v>Investitionskosten</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>10.0</v>
+        <v>6851180.0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.09174311926605505</v>
+        <v>0.8837677884069637</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F6">+'Mittelverwendung - Mittelherkun'!D3:F6</f>
         <v>Eigenkapital</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>20.0</v>
+        <v>900000.0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.1160954918959542</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1220,19 +1229,19 @@
         <v>Finanzierungskosten</v>
       </c>
       <c r="B4" s="16" t="n">
-        <v>99.0</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.908256880733945</v>
+        <v>0.11623221159303633</v>
       </c>
       <c r="D4" s="13" t="str">
-        <v>Fremdkapital Tranche 1</v>
+        <v>Fremdkapital Tranche 1 bis Baubeginn</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>1.0</v>
+        <v>2450000.0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.02857142857142857</v>
+        <v>0.3160377279389864</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1240,13 +1249,13 @@
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="str">
-        <v>Fremdkapital Tranche 2</v>
+        <v>Fremdkapital Tranche 2 ab Baubeginn</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>2.0</v>
+        <v>2250000.0</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.05714285714285714</v>
+        <v>0.29023872973988546</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1257,10 +1266,10 @@
         <v>BTVG Erlöse</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>12.0</v>
+        <v>2152239.0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.34285714285714286</v>
+        <v>0.27762805042517397</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1277,7 +1286,7 @@
         <v>Summe</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>109.0</v>
+        <v>7752240.0</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>1.0</v>
@@ -1285,7 +1294,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="10" cm="1" t="n">
         <f t="array" ref="E8:F8">+'Mittelverwendung - Mittelherkun'!E8:F8</f>
-        <v>35.0</v>
+        <v>7752239.0</v>
       </c>
       <c r="F8" s="4" t="n">
         <v>1.0</v>
@@ -1319,7 +1328,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1348,7 +1357,7 @@
         <v>2.0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.019801980198019802</v>
+        <v>2.219603090575343E-6</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F7">+'Mittelverwendung - Mittelherkun'!T3:V7</f>
@@ -1366,10 +1375,10 @@
         <v>Finanzierungskosten</v>
       </c>
       <c r="B4" s="16" t="n">
-        <v>99.0</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.9801980198019802</v>
+        <v>0.9999977803969095</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 1</v>
@@ -1445,7 +1454,7 @@
         <v>Summe</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>101.0</v>
+        <v>901062.0</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>1.0</v>
@@ -1473,7 +1482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED108C8A-0089-49D9-A899-5A80F96B0F9A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1487,7 +1496,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1516,7 +1525,7 @@
         <v>10.0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.09174311926605505</v>
+        <v>1.109791692099393E-5</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F8">+'Mittelverwendung - Mittelherkun'!AB3:AD8</f>
@@ -1534,10 +1543,10 @@
         <v>Finanzierungskosten</v>
       </c>
       <c r="B4" s="16" t="n">
-        <v>99.0</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.908256880733945</v>
+        <v>0.999988902083079</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 1</v>
@@ -1619,7 +1628,7 @@
         <v>Summe</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>109.0</v>
+        <v>901070.0</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>1.0</v>
@@ -1661,7 +1670,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1690,7 +1699,7 @@
         <v>1.0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.01</v>
+        <v>1.1098027769485084E-6</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F9">+'Mittelverwendung - Mittelherkun'!AJ3:AL9</f>
@@ -1708,10 +1717,10 @@
         <v>Finanzierungskosten</v>
       </c>
       <c r="B4" s="16" t="n">
-        <v>99.0</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.99</v>
+        <v>0.9999988901972231</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 1</v>
@@ -1807,7 +1816,7 @@
         <v>Summe</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>100.0</v>
+        <v>901061.0</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>1.0</v>
@@ -1899,18 +1908,18 @@
       <c r="K1" s="42"/>
       <c r="L1" s="43"/>
       <c r="O1" s="24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="T1" s="24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -1921,27 +1930,27 @@
         <v>52</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
       <c r="O2" s="18" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="P2" t="str">
         <f>LEFT(O2,SEARCH("=",O2)-2)</f>
-        <v>W II</v>
+        <v>W I</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="U2" s="18" t="str">
         <f>+Basisinformation!I3</f>
         <v>Braumüllergasse 21</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="W2" s="18"/>
       <c r="X2" s="18"/>
@@ -1952,10 +1961,10 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -1963,23 +1972,23 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="O3" s="18" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="P3" t="str">
         <f>LEFT(O3,SEARCH("=",O3)-2)</f>
-        <v>gk</v>
+        <v>o</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="U3" s="18" t="str">
         <f>+Basisinformation!B2</f>
@@ -1995,10 +2004,10 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -2009,47 +2018,47 @@
         <v>53</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="O4" s="27" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="P4" s="25" t="str">
         <f>CONCATENATE(P2," ",P3)</f>
-        <v>W II gk</v>
+        <v>W I o</v>
       </c>
       <c r="Q4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="U4" s="18" t="str">
+        <v>90</v>
+      </c>
+      <c r="U4" s="18" t="e">
         <f>+Basisinformation!P7</f>
-        <v>G</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V4" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="W4" s="18" t="str">
         <f>+Basisinformation!P4</f>
-        <v>W II gk</v>
+        <v>W I o</v>
       </c>
       <c r="X4" s="18"/>
-      <c r="Y4" t="str">
+      <c r="Y4" t="e">
         <f t="shared" si="0"/>
-        <v>Bebauungsbestimmungen: G; Widmung: W II gk</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
@@ -2065,20 +2074,22 @@
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
-      <c r="O5" s="27"/>
+      <c r="O5" s="27" t="s">
+        <v>71</v>
+      </c>
       <c r="P5" t="str">
         <f>+IF(ISBLANK(O4),"angefordert",LEFT(O4,SEARCH("=",O4)-2))</f>
         <v>G</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="U5" s="18" t="str">
         <f>+Basisinformation!B3</f>
         <v>797</v>
       </c>
       <c r="V5" s="18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="W5" s="18"/>
       <c r="X5" s="18"/>
@@ -2092,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -2105,26 +2116,26 @@
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
       <c r="O6" s="18"/>
-      <c r="P6" t="str">
+      <c r="P6" t="e">
         <f>+IF(ISBLANK(O5),"angefordert",LEFT(O5,SEARCH("=",O5)-2))</f>
-        <v>angefordert</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T6" s="18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="U6" s="18" t="str">
         <f>+Basisinformation!B4</f>
         <v>800</v>
       </c>
       <c r="V6" s="18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="W6" s="18" t="str">
         <f>+Basisinformation!B7</f>
         <v>160</v>
       </c>
       <c r="X6" s="18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Y6" t="str">
         <f t="shared" si="0"/>
@@ -2133,10 +2144,10 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -2149,29 +2160,29 @@
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="O7" s="18"/>
-      <c r="P7" s="25" t="str">
+      <c r="P7" s="25" t="e">
         <f>+IF(AND(P5="angefordert",P6="angefordert"),"angefordert",CONCATENATE(IF(ISBLANK(O4),,P5),IF(ISBLANK(O5),,P6)))</f>
-        <v>G</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Q7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="T7" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="U7" s="18" t="str">
         <f>+Basisinformation!B5</f>
         <v>8</v>
       </c>
       <c r="V7" s="18" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="W7" s="18" t="str">
         <f>+Basisinformation!B6</f>
         <v>16</v>
       </c>
       <c r="X7" s="18" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="0"/>
@@ -2183,7 +2194,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
@@ -2197,20 +2208,20 @@
       <c r="L8" s="18"/>
       <c r="O8" s="18"/>
       <c r="T8" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="U8" s="18" t="n">
         <f>+ROUND(Gesamtinvestitionskosten!E15,-4)</f>
-        <v>0.0</v>
+        <v>7750000.0</v>
       </c>
       <c r="V8" s="18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="W8" s="18"/>
       <c r="X8" s="18"/>
       <c r="Y8" t="str">
         <f t="shared" si="0"/>
-        <v>Gesamtinvestitionskosten: EUR 0 (gerundet)</v>
+        <v>Gesamtinvestitionskosten: EUR 7750000 (gerundet)</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.35">
@@ -2218,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -2232,14 +2243,14 @@
       <c r="L9" s="18"/>
       <c r="O9" s="18"/>
       <c r="T9" s="18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="U9" s="18" t="n">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!E20,-4)</f>
         <v>1.027E7</v>
       </c>
       <c r="V9" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="W9" s="29" t="n">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!F4,0)</f>
@@ -2265,25 +2276,25 @@
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
       <c r="T10" s="18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="U10" s="18" t="n">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!E22,-5)</f>
-        <v>1.03E7</v>
+        <v>2500000.0</v>
       </c>
       <c r="V10" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="W10" s="20" t="n">
         <f>+Wirtschaftlichkeitsrechnung!E23</f>
-        <v>120519.94332981344</v>
+        <v>0.3249835976524263</v>
       </c>
       <c r="X10" s="18" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="Y10" t="str">
         <f>+CONCATENATE(T10,U10,V10,ROUND(W10*100,2),X10)</f>
-        <v>Gewinn: EUR 10300000 (gerundet ROI 12051994.33%)</v>
+        <v>Gewinn: EUR 2500000 (gerundet ROI 32.5%)</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.35">
@@ -2300,7 +2311,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
       <c r="T11" s="18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="U11" s="18" t="str">
         <f>+B8</f>
@@ -2321,7 +2332,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="T12" s="18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="U12" s="18" t="str">
         <f>+B9</f>
@@ -2362,77 +2373,77 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="F2" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="1">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>8.0</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="1">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8</v>
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>5.0</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="1">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
-        <v>8</v>
+        <v>65</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>2.0</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="1">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1.0</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -2440,7 +2451,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="F7" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -2448,7 +2459,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="F8" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -2456,7 +2467,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="F9" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -2464,7 +2475,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -2472,7 +2483,7 @@
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="F11" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2480,7 +2491,7 @@
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2488,7 +2499,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="F13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2516,7 +2527,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2569,45 +2580,45 @@
     </row>
     <row r="10" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="n">
         <f>+Standort!B3</f>
-        <v>8.0</v>
+        <v>15.0</v>
       </c>
       <c r="C11" s="1" t="n">
         <f>+Standort!B3</f>
-        <v>8.0</v>
+        <v>15.0</v>
       </c>
       <c r="D11" s="1" t="n">
         <f>+Standort!B5</f>
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="E11" s="1" t="n">
         <f>+Standort!B6</f>
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="n">
         <f>+Standort!C3</f>
@@ -2615,15 +2626,15 @@
       </c>
       <c r="C12" s="1" t="n">
         <f>+Standort!C4</f>
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="D12" s="1" t="n">
         <f>+Standort!C5</f>
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="E12" s="1" t="n">
         <f>+Standort!C6</f>
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2645,7 +2656,7 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -2653,7 +2664,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -2661,7 +2672,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -2669,7 +2680,7 @@
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="F19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -2677,7 +2688,7 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="F20" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -2685,7 +2696,7 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="F21" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2708,7 +2719,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -2720,12 +2731,12 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="str" cm="1">
         <f t="array" ref="A3:A4">+Basisinformation!O2:O3</f>
-        <v>W II = Bauklasse 2</v>
+        <v>W I = Bauklasse 1 beschränkt auf 6,5 Meter</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="str">
-        <v>gk = gekuppelte Bauweise</v>
+        <v>o = offene Bauweise</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
@@ -2737,7 +2748,8 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="str">
         <f>+IF(ISBLANK(Basisinformation!O5),"",Basisinformation!O5)</f>
-        <v/>
+        <v>
+</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
@@ -2786,7 +2798,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -2819,23 +2831,23 @@
         <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>2530800</v>
       </c>
       <c r="C3" s="3" t="n">
         <f>B3*B22</f>
-        <v>2.2</v>
+        <v>25308.0</v>
       </c>
       <c r="D3" s="17" t="n">
         <f>+B22</f>
-        <v>0.22</v>
+        <v>0.01</v>
       </c>
       <c r="E3" s="3" t="n">
         <f t="shared" ref="E3:E11" si="0">B3+C3</f>
-        <v>12.2</v>
+        <v>2556108.0</v>
       </c>
       <c r="F3" s="2" t="n">
         <f t="shared" ref="F3:F11" si="1">$E3/$E$15</f>
-        <v>0.1431420861199108</v>
+        <v>0.32971195228077765</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -2844,23 +2856,23 @@
         <v>9</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>85892</v>
       </c>
       <c r="C4" s="3" t="n">
-        <f t="shared" ref="C4:C10" si="2">B4*$B$21</f>
-        <v>0.33</v>
+        <f t="shared" ref="C4:C9" si="2">B4*$B$21</f>
+        <v>17178.4</v>
       </c>
       <c r="D4" s="6" t="n">
         <f t="shared" ref="D4:D10" si="3">C4/B4</f>
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>1.33</v>
+        <v>103070.4</v>
       </c>
       <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.015604833978646017</v>
+        <v>0.01329503401513577</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -2869,23 +2881,23 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>2475206</v>
       </c>
       <c r="C5" s="3" t="n">
         <f>B5*$B$21</f>
-        <v>0.66</v>
+        <v>495041.2</v>
       </c>
       <c r="D5" s="6" t="n">
         <f>C5/B5</f>
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>2.66</v>
+        <v>2970247.2</v>
       </c>
       <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.031209667957292034</v>
+        <v>0.38313169986108314</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -2894,23 +2906,23 @@
         <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>6</v>
+        <v>212558</v>
       </c>
       <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>1.98</v>
+        <v>42511.600000000006</v>
       </c>
       <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.33</v>
+        <v>0.20000000000000004</v>
       </c>
       <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>7.98</v>
+        <v>255069.6</v>
       </c>
       <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.0936290038718761</v>
+        <v>0.03290138592871547</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -2919,23 +2931,23 @@
         <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>7</v>
+        <v>612366</v>
       </c>
       <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>2.31</v>
+        <v>122473.20000000001</v>
       </c>
       <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>9.31</v>
+        <v>734839.2</v>
       </c>
       <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.10923383785052211</v>
+        <v>0.09478678805607776</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -2944,23 +2956,23 @@
         <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>8</v>
+        <v>39881</v>
       </c>
       <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>2.64</v>
+        <v>7976.200000000001</v>
       </c>
       <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>10.64</v>
+        <v>47857.2</v>
       </c>
       <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.12483867182916814</v>
+        <v>0.006173092389950515</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -2969,23 +2981,23 @@
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>9</v>
+        <v>101581</v>
       </c>
       <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>2.97</v>
+        <v>20316.2</v>
       </c>
       <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>11.97</v>
+        <v>121897.2</v>
       </c>
       <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.14044350580781415</v>
+        <v>0.01572349986368354</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -2994,23 +3006,23 @@
         <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>10</v>
+        <v>52000</v>
       </c>
       <c r="C10" s="3" t="n">
         <f>B10*$B$21</f>
-        <v>3.3000000000000003</v>
+        <v>10400.0</v>
       </c>
       <c r="D10" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>13.3</v>
+        <v>62400.0</v>
       </c>
       <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.15604833978646016</v>
+        <v>0.008048965780131562</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -3019,22 +3031,22 @@
         <v>16</v>
       </c>
       <c r="B11" s="9">
-        <v>11</v>
+        <v>901060</v>
       </c>
       <c r="C11" s="3" t="n">
         <f>+B11*D11</f>
-        <v>4.84</v>
+        <v>0.0</v>
       </c>
       <c r="D11" s="6">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="E11" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>15.84</v>
+        <v>901060.0</v>
       </c>
       <c r="F11" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.18585005279831043</v>
+        <v>0.11622758182444463</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -3053,19 +3065,19 @@
       </c>
       <c r="B13" s="3" t="n">
         <f>SUM(B3:B11)</f>
-        <v>64.0</v>
+        <v>7011344.0</v>
       </c>
       <c r="C13" s="3" t="n">
         <f>SUM(C3:C11)</f>
-        <v>21.23</v>
+        <v>741204.7999999998</v>
       </c>
       <c r="D13" s="4" t="n">
         <f>C13/B13</f>
-        <v>0.33171875</v>
+        <v>0.10571508115990312</v>
       </c>
       <c r="E13" s="10" t="n">
         <f>B13+C13</f>
-        <v>85.23</v>
+        <v>7752548.8</v>
       </c>
       <c r="F13" s="4" t="n">
         <f>SUM(F3:F11)</f>
@@ -3090,19 +3102,19 @@
       </c>
       <c r="B15" s="3" t="n">
         <f>B13</f>
-        <v>64.0</v>
+        <v>7011344.0</v>
       </c>
       <c r="C15" s="3" t="n">
         <f>C13</f>
-        <v>21.23</v>
+        <v>741204.7999999998</v>
       </c>
       <c r="D15" s="3" t="n">
         <f>D13</f>
-        <v>0.33171875</v>
+        <v>0.10571508115990312</v>
       </c>
       <c r="E15" s="10" t="n">
         <f>E13</f>
-        <v>85.23</v>
+        <v>7752548.8</v>
       </c>
       <c r="F15" s="4" t="n">
         <f>F13</f>
@@ -3142,7 +3154,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="11">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -3150,7 +3162,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="12">
-        <v>0.22</v>
+        <v>0.01</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -3168,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C08536-E6A3-4E31-88A7-DF1DE6751CED}">
   <dimension ref="A1:AL12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <selection activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3198,7 +3210,7 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -3206,7 +3218,7 @@
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
       <c r="I1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
@@ -3214,7 +3226,7 @@
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
       <c r="Q1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R1" s="44"/>
       <c r="S1" s="44"/>
@@ -3222,7 +3234,7 @@
       <c r="U1" s="44"/>
       <c r="V1" s="44"/>
       <c r="Y1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Z1" s="44"/>
       <c r="AA1" s="44"/>
@@ -3230,7 +3242,7 @@
       <c r="AC1" s="44"/>
       <c r="AD1" s="44"/>
       <c r="AG1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AH1" s="44"/>
       <c r="AI1" s="44"/>
@@ -3295,21 +3307,21 @@
         <v>25</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>6851180</v>
       </c>
       <c r="C3" s="2" t="n">
         <f>$B3/$B8</f>
-        <v>0.09174311926605505</v>
+        <v>0.8837677884069637</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="1">
-        <v>20</v>
+        <v>900000</v>
       </c>
       <c r="F3" s="2" t="n">
         <f>$E3/$E8</f>
-        <v>0.5714285714285714</v>
+        <v>0.1160954918959542</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>25</v>
@@ -3319,7 +3331,7 @@
       </c>
       <c r="K3" s="2" t="n">
         <f>$J3/$J7</f>
-        <v>0.5540540540540541</v>
+        <v>1.3648726174373017E-4</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>26</v>
@@ -3339,7 +3351,7 @@
       </c>
       <c r="S3" s="2" t="n">
         <f>$R3/$R9</f>
-        <v>0.019801980198019802</v>
+        <v>2.219603090575343E-6</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>26</v>
@@ -3359,7 +3371,7 @@
       </c>
       <c r="AA3" s="2" t="n">
         <f>$Z3/$Z10</f>
-        <v>0.09174311926605505</v>
+        <v>1.109791692099393E-5</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>26</v>
@@ -3379,7 +3391,7 @@
       </c>
       <c r="AI3" s="2" t="n">
         <f>$AH3/$AH11</f>
-        <v>0.01</v>
+        <v>1.1098027769485084E-6</v>
       </c>
       <c r="AJ3" s="1" t="s">
         <v>26</v>
@@ -3396,32 +3408,34 @@
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="16">
-        <v>99</v>
+      <c r="B4" s="16" t="n">
+        <f>+Gesamtinvestitionskosten!E11</f>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
         <f>$B4/$B8</f>
-        <v>0.908256880733945</v>
+        <v>0.11623221159303633</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
+        <v>2450000</v>
       </c>
       <c r="F4" s="2" t="n">
         <f>$E4/$E8</f>
-        <v>0.02857142857142857</v>
+        <v>0.3160377279389864</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="16">
-        <v>99</v>
+      <c r="J4" s="16" t="n">
+        <f>+Gesamtinvestitionskosten!E11</f>
+        <v>901060.0</v>
       </c>
       <c r="K4" s="2" t="n">
         <f>$J4/$J7</f>
-        <v>0.44594594594594594</v>
+        <v>0.9998635127382562</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>58</v>
@@ -3436,12 +3450,13 @@
       <c r="Q4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="16">
-        <v>99</v>
+      <c r="R4" s="16" t="n">
+        <f>+Gesamtinvestitionskosten!E11</f>
+        <v>901060.0</v>
       </c>
       <c r="S4" s="2" t="n">
         <f>$R4/$R9</f>
-        <v>0.9801980198019802</v>
+        <v>0.9999977803969095</v>
       </c>
       <c r="T4" s="13" t="s">
         <v>58</v>
@@ -3456,12 +3471,13 @@
       <c r="Y4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="16">
-        <v>99</v>
+      <c r="Z4" s="16" t="n">
+        <f>+Gesamtinvestitionskosten!E11</f>
+        <v>901060.0</v>
       </c>
       <c r="AA4" s="2" t="n">
         <f>$Z4/$Z10</f>
-        <v>0.908256880733945</v>
+        <v>0.999988902083079</v>
       </c>
       <c r="AB4" s="13" t="s">
         <v>58</v>
@@ -3476,12 +3492,13 @@
       <c r="AG4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AH4" s="16">
-        <v>99</v>
+      <c r="AH4" s="16" t="n">
+        <f>+Gesamtinvestitionskosten!E11</f>
+        <v>901060.0</v>
       </c>
       <c r="AI4" s="2" t="n">
         <f>$AH4/$AH11</f>
-        <v>0.99</v>
+        <v>0.9999988901972231</v>
       </c>
       <c r="AJ4" s="13" t="s">
         <v>58</v>
@@ -3499,14 +3516,14 @@
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="E5" s="1">
-        <v>2</v>
+        <v>2250000</v>
       </c>
       <c r="F5" s="2" t="n">
         <f>$E5/$E8</f>
-        <v>0.05714285714285714</v>
+        <v>0.29023872973988546</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -3569,11 +3586,11 @@
         <v>28</v>
       </c>
       <c r="E6" s="1">
-        <v>12</v>
+        <v>2152239</v>
       </c>
       <c r="F6" s="2" t="n">
         <f>$E6/$E8</f>
-        <v>0.34285714285714286</v>
+        <v>0.27762805042517397</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -3633,7 +3650,7 @@
       </c>
       <c r="J7" s="3" t="n">
         <f>SUM(J3:J6)</f>
-        <v>222.0</v>
+        <v>901183.0</v>
       </c>
       <c r="K7" s="4" t="n">
         <f>SUM(K3:K6)</f>
@@ -3694,7 +3711,7 @@
       </c>
       <c r="B8" s="3" t="n">
         <f>SUM(B3:B7)</f>
-        <v>109.0</v>
+        <v>7752240.0</v>
       </c>
       <c r="C8" s="4" t="n">
         <f>SUM(C3:C7)</f>
@@ -3703,7 +3720,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="10" t="n">
         <f>SUM(E3:E7)</f>
-        <v>35.0</v>
+        <v>7752239.0</v>
       </c>
       <c r="F8" s="4" t="n">
         <f>SUM(F3:F7)</f>
@@ -3748,7 +3765,7 @@
       </c>
       <c r="R9" s="3" t="n">
         <f>SUM(R3:R8)</f>
-        <v>101.0</v>
+        <v>901062.0</v>
       </c>
       <c r="S9" s="4" t="n">
         <f>SUM(S3:S8)</f>
@@ -3789,7 +3806,7 @@
       </c>
       <c r="Z10" s="3" t="n">
         <f>SUM(Z3:Z9)</f>
-        <v>109.0</v>
+        <v>901070.0</v>
       </c>
       <c r="AA10" s="4" t="n">
         <f>SUM(AA3:AA9)</f>
@@ -3817,7 +3834,7 @@
       </c>
       <c r="AH11" s="3" t="n">
         <f>SUM(AH3:AH10)</f>
-        <v>100.0</v>
+        <v>901061.0</v>
       </c>
       <c r="AI11" s="4" t="n">
         <f>SUM(AI3:AI10)</f>
@@ -3835,14 +3852,19 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="G12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H12" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Y1:AD1"/>
+    <mergeCell ref="AG1:AL1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="AB2:AD2"/>
@@ -3853,11 +3875,6 @@
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="Y1:AD1"/>
-    <mergeCell ref="AG1:AL1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3867,7 +3884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB0A179-3460-4B7F-B6A0-F84428E1F30B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3884,7 +3901,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -3967,7 +3984,7 @@
         <v>960.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="3" t="n">
@@ -3991,7 +4008,7 @@
         <v>0.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E6" s="40">
         <v>0</v>
@@ -4017,7 +4034,7 @@
         <v>960.0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E7" s="40">
         <v>0</v>
@@ -4280,7 +4297,7 @@
       </c>
       <c r="E21" s="9" t="n">
         <f>+Gesamtinvestitionskosten!E15</f>
-        <v>85.23</v>
+        <v>7752548.8</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -4296,7 +4313,7 @@
       </c>
       <c r="E22" s="3" t="n">
         <f>E20-E21</f>
-        <v>1.027191477E7</v>
+        <v>2519451.2</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -4312,7 +4329,7 @@
       </c>
       <c r="E23" s="2" t="n">
         <f>E22/E21</f>
-        <v>120519.94332981344</v>
+        <v>0.3249835976524263</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -4366,7 +4383,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4379,7 +4396,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -4410,7 +4427,7 @@
       </c>
       <c r="C3" s="2" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K3</f>
-        <v>0.5540540540540541</v>
+        <v>1.3648726174373017E-4</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>+'Mittelverwendung - Mittelherkun'!L3</f>
@@ -4432,11 +4449,11 @@
       </c>
       <c r="B4" s="16" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!J4</f>
-        <v>99.0</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K4</f>
-        <v>0.44594594594594594</v>
+        <v>0.9998635127382562</v>
       </c>
       <c r="D4" s="13" t="str">
         <f>+'Mittelverwendung - Mittelherkun'!L4</f>
@@ -4481,7 +4498,7 @@
       </c>
       <c r="B7" s="3" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!J7</f>
-        <v>222.0</v>
+        <v>901183.0</v>
       </c>
       <c r="C7" s="4" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K7</f>
@@ -4508,23 +4525,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -4688,10 +4688,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4713,19 +4740,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
nicht mehr benötigte Klassen und Dokumente entfernt
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
+++ b/src/main/resources/com/example/financingtool/SEPJ-Rechnungen.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="186">
   <si>
     <t>Wohneinheiten</t>
   </si>
@@ -482,6 +482,156 @@
   </si>
   <si>
     <t>USt</t>
+  </si>
+  <si>
+    <t>898</t>
+  </si>
+  <si>
+    <t>fghjkl</t>
+  </si>
+  <si>
+    <t>hahahahah</t>
+  </si>
+  <si>
+    <t>ahsososos</t>
+  </si>
+  <si>
+    <t>120000</t>
+  </si>
+  <si>
+    <t>djsfkdsh</t>
+  </si>
+  <si>
+    <t>hiiiiiiiiiiiiiiiiiiiiiiiiiiiiiii</t>
+  </si>
+  <si>
+    <t>jduhsfiushidfuhsdkjncskdjcsdjkc</t>
+  </si>
+  <si>
+    <t>sdjcksdcnjdnclkjdscnks</t>
+  </si>
+  <si>
+    <t>sdcnkjsdcnsdjnksdj</t>
+  </si>
+  <si>
+    <t>skdcnksdjncjhdsbckjsdbcjs</t>
+  </si>
+  <si>
+    <t>sdnckjsdcnksdjncjhbsdjc</t>
+  </si>
+  <si>
+    <t>IG VI = Bauklasse 6 beschränkt auf vdjkjfkldnvkjd</t>
+  </si>
+  <si>
+    <t>gk = gekuppelte Bauweise</t>
+  </si>
+  <si>
+    <t>ÖZ = Grundflächen für öffentliche Zwecke (Enteignung möglich)</t>
+  </si>
+  <si>
+    <t>ahsososos 5</t>
+  </si>
+  <si>
+    <t>Höchstädtplatz 6</t>
+  </si>
+  <si>
+    <t>Fremdkapital 1</t>
+  </si>
+  <si>
+    <t>Tranche 2</t>
+  </si>
+  <si>
+    <t>Batzen 3</t>
+  </si>
+  <si>
+    <t>Bestlage im 17. Bezirk</t>
+  </si>
+  <si>
+    <t>Absolute Ruhelage, mit Fernblick über Wien</t>
+  </si>
+  <si>
+    <t>Zentrum Wien 18 Autominuten, öffentlich 25 Minuten</t>
+  </si>
+  <si>
+    <t>Nahversorgung, Restaurants u. Geschäfte des täglichen Bedarfs in unmittelbarer Nähe</t>
+  </si>
+  <si>
+    <t>Perfekte öffentliche Anbindung, 7 Gehminuten über Rebenweg</t>
+  </si>
+  <si>
+    <t>Genießen Sie die Aussichten Hernals</t>
+  </si>
+  <si>
+    <t>Genießen Sie die Aussichten Hernals und ruhigem Verkehr</t>
+  </si>
+  <si>
+    <t>Wagramer Straße 315</t>
+  </si>
+  <si>
+    <t>1220</t>
+  </si>
+  <si>
+    <t>Ostsee</t>
+  </si>
+  <si>
+    <t>Höchststädtplatz 6</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>Teststraße 6</t>
+  </si>
+  <si>
+    <t>Piaristenhalle 15</t>
+  </si>
+  <si>
+    <t>5620</t>
+  </si>
+  <si>
+    <t>Trab</t>
+  </si>
+  <si>
+    <t>Juwel</t>
+  </si>
+  <si>
+    <t>Hoiooo</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Kolmin</t>
+  </si>
+  <si>
+    <t>Beste Aussicht aus Hernals bei ruhigem Verkehr</t>
+  </si>
+  <si>
+    <t>W I = Bauklasse 1 beschränkt auf 6,5 Meter</t>
+  </si>
+  <si>
+    <t>G = Gärtnerische Ausgestaltung</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 1 (bis Baubeginn)</t>
+  </si>
+  <si>
+    <t>Fremdkapital Tranche 2 (ab Baubeginn)</t>
+  </si>
+  <si>
+    <t>hallo</t>
+  </si>
+  <si>
+    <t>sahdkaskdb</t>
+  </si>
+  <si>
+    <t>shdkas#</t>
+  </si>
+  <si>
+    <t>asda</t>
+  </si>
+  <si>
+    <t>Gute Aussicht über Hernals mit ruhigem Verkehr</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1257,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="str">
         <f>+Basisinformation!Y4</f>
-        <v>Bebauungsbestimmungen: angefordert; Widmung: W II o</v>
+        <v>Bebauungsbestimmungen: angefordert; Widmung: W I o</v>
       </c>
       <c r="B4" s="22"/>
     </row>
@@ -1135,7 +1285,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="str">
         <f>+Basisinformation!Y8</f>
-        <v>Gesamtinvestitionskosten: EUR 7430000 (gerundet)</v>
+        <v>Gesamtinvestitionskosten: EUR 7750000 (gerundet)</v>
       </c>
       <c r="B8" s="18"/>
     </row>
@@ -1149,7 +1299,7 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="str">
         <f>+Basisinformation!Y10</f>
-        <v>Gewinn: EUR 2800000 (gerundet ROI 38.21%)</v>
+        <v>Gewinn: EUR 2500000 (gerundet ROI 32.51%)</v>
       </c>
       <c r="B10" s="18"/>
     </row>
@@ -1654,7 +1804,7 @@
         <v>44</v>
       </c>
       <c r="B25" s="9" t="n">
-        <v>7432024.64</v>
+        <v>7751740.8</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1669,7 +1819,7 @@
         <v>45</v>
       </c>
       <c r="B26" s="3" t="n">
-        <v>2839975.3600000003</v>
+        <v>2520259.2</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1684,7 +1834,7 @@
         <v>132</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0.3821267417111255</v>
+        <v>0.32512170685583297</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1784,7 +1934,7 @@
       </c>
       <c r="C3" s="2" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K3</f>
-        <v>1.2876256246292843E-4</v>
+        <v>1.3648726174373017E-4</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>+'Mittelverwendung - Mittelherkun'!L3</f>
@@ -1806,11 +1956,11 @@
       </c>
       <c r="B4" s="16" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!J4</f>
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K4</f>
-        <v>0.999871237437537</v>
+        <v>0.9998635127382562</v>
       </c>
       <c r="D4" s="13" t="str">
         <f>+'Mittelverwendung - Mittelherkun'!L4</f>
@@ -1855,7 +2005,7 @@
       </c>
       <c r="B7" s="3" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!J7</f>
-        <v>955246.6</v>
+        <v>901183.0</v>
       </c>
       <c r="C7" s="4" t="n">
         <f>+'Mittelverwendung - Mittelherkun'!K7</f>
@@ -1928,7 +2078,7 @@
         <v>6851180.0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.877647136347605</v>
+        <v>0.8837677884069637</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F6">+'Mittelverwendung - Mittelherkun'!D3:F6</f>
@@ -1938,7 +2088,7 @@
         <v>900000.0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.1160954918959542</v>
+        <v>0.1547657534340801</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1946,19 +2096,19 @@
         <v>Finanzierungskosten</v>
       </c>
       <c r="B4" s="16" t="n">
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.12235286365239498</v>
+        <v>0.11623221159303633</v>
       </c>
       <c r="D4" s="13" t="str">
-        <v>Fremdkapital Tranche 1 - bis Baubeginn</v>
+        <v>Fremdkapital Tranche 1 (bis Baubeginn)</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>2450000.0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.3160377279389864</v>
+        <v>0.42130677323721805</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1966,13 +2116,13 @@
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="str">
-        <v>Fremdkapital Tranche 2 - ab Baubeginn</v>
+        <v>Fremdkapital Tranche 2 (ab Baubeginn)</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>2250000.0</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.29023872973988546</v>
+        <v>0.38691438358520025</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1983,10 +2133,10 @@
         <v>BTVG Erlöse</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>2152239.0</v>
+        <v>215240.0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.27762805042517397</v>
+        <v>0.03701308974350156</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2003,7 +2153,7 @@
         <v>Summe</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>7806303.6</v>
+        <v>7752240.0</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>1.0</v>
@@ -2011,7 +2161,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="10" cm="1" t="n">
         <f t="array" ref="E8:F8">+'Mittelverwendung - Mittelherkun'!E8:F8</f>
-        <v>7752239.0</v>
+        <v>5815240.0</v>
       </c>
       <c r="F8" s="4" t="n">
         <v>1.0</v>
@@ -2071,20 +2221,20 @@
         <v>Investitionskosten</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2.0</v>
+        <v>456123.0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>2.0939654428695034E-6</v>
+        <v>0.33608069066588664</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F7">+'Mittelverwendung - Mittelherkun'!T3:V7</f>
         <v>Eigenkapital</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>1.0</v>
+        <v>456123.0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.012345679012345678</v>
+        <v>1.7143948655649988E-5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2092,19 +2242,19 @@
         <v>Finanzierungskosten</v>
       </c>
       <c r="B4" s="16" t="n">
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.9999979060345572</v>
+        <v>0.6639193093341134</v>
       </c>
       <c r="D4" s="13" t="str">
-        <v>Fremdkapital Tranche 1</v>
+        <v>Fremdkapital 1</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>10.0</v>
+        <v>2.4896321456E10</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.12345679012345678</v>
+        <v>0.9357591192643677</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2112,13 +2262,13 @@
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="str">
-        <v>Fremdkapital Tranche 2</v>
+        <v>Tranche 2</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>23.0</v>
+        <v>1.45641235E8</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.2839506172839506</v>
+        <v>0.005474106447132581</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2126,13 +2276,13 @@
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="13" t="str">
-        <v>Fremdkapital Tranche 3</v>
+        <v>Batzen 3</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>45.0</v>
+        <v>16541.0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.5555555555555556</v>
+        <v>6.217139997612628E-7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2143,10 +2293,10 @@
         <v>BTVG Erlöse</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>2.0</v>
+        <v>1.563045632E9</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.024691358024691357</v>
+        <v>0.05874900862584432</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2171,7 +2321,7 @@
         <v>Summe</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>955125.6</v>
+        <v>1357183.0</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>1.0</v>
@@ -2179,10 +2329,10 @@
       <c r="D10" s="3"/>
       <c r="E10" s="10" cm="1" t="n">
         <f t="array" ref="E10:F10">+'Mittelverwendung - Mittelherkun'!U9:V9</f>
-        <v>81.0</v>
+        <v>2.6605480987E10</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2242,7 +2392,7 @@
         <v>10.0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>1.0469739521256502E-5</v>
+        <v>1.109791692099393E-5</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F8">+'Mittelverwendung - Mittelherkun'!AB3:AD8</f>
@@ -2260,10 +2410,10 @@
         <v>Finanzierungskosten</v>
       </c>
       <c r="B4" s="16" t="n">
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.9999895302604788</v>
+        <v>0.999988902083079</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 1</v>
@@ -2345,7 +2495,7 @@
         <v>Summe</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>955133.6</v>
+        <v>901070.0</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>1.0</v>
@@ -2416,7 +2566,7 @@
         <v>4567984.0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.8270677181809748</v>
+        <v>0.8352436001611981</v>
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3:F9">+'Mittelverwendung - Mittelherkun'!AJ3:AL9</f>
@@ -2434,10 +2584,10 @@
         <v>Finanzierungskosten</v>
       </c>
       <c r="B4" s="16" t="n">
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.17293228181902523</v>
+        <v>0.1647563998388018</v>
       </c>
       <c r="D4" s="13" t="str">
         <v>Fremdkapital Tranche 6</v>
@@ -2533,7 +2683,7 @@
         <v>Summe</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>5523107.6</v>
+        <v>5469044.0</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>1.0</v>
@@ -2653,11 +2803,11 @@
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
       <c r="O2" s="18" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="P2" t="str">
         <f>LEFT(O2,SEARCH("=",O2)-2)</f>
-        <v>W II</v>
+        <v>W I</v>
       </c>
       <c r="T2" s="18" t="s">
         <v>80</v>
@@ -2741,11 +2891,11 @@
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="O4" s="27" t="s">
-        <v>105</v>
+        <v>178</v>
       </c>
       <c r="P4" s="25" t="str">
         <f>CONCATENATE(P2," ",P3)</f>
-        <v>W II o</v>
+        <v>W I o</v>
       </c>
       <c r="Q4" t="s">
         <v>84</v>
@@ -2762,12 +2912,12 @@
       </c>
       <c r="W4" s="18" t="str">
         <f>+Basisinformation!P4</f>
-        <v>W II o</v>
+        <v>W I o</v>
       </c>
       <c r="X4" s="18"/>
       <c r="Y4" t="str">
         <f t="shared" si="0"/>
-        <v>Bebauungsbestimmungen: angefordert; Widmung: W II o</v>
+        <v>Bebauungsbestimmungen: angefordert; Widmung: W I o</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
@@ -2929,7 +3079,7 @@
       </c>
       <c r="U8" s="18" t="n">
         <f>+ROUND(Gesamtinvestitionskosten!E15,-4)</f>
-        <v>7430000.0</v>
+        <v>7750000.0</v>
       </c>
       <c r="V8" s="18" t="s">
         <v>96</v>
@@ -2938,7 +3088,7 @@
       <c r="X8" s="18"/>
       <c r="Y8" t="str">
         <f t="shared" si="0"/>
-        <v>Gesamtinvestitionskosten: EUR 7430000 (gerundet)</v>
+        <v>Gesamtinvestitionskosten: EUR 7750000 (gerundet)</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
@@ -2997,21 +3147,21 @@
       </c>
       <c r="U10" s="18" t="n">
         <f>+ROUND(Wirtschaftlichkeitsrechnung!B26,-5)</f>
-        <v>2800000.0</v>
+        <v>2500000.0</v>
       </c>
       <c r="V10" s="18" t="s">
         <v>101</v>
       </c>
       <c r="W10" s="20" t="n">
         <f>+Wirtschaftlichkeitsrechnung!B27</f>
-        <v>0.3821267417111255</v>
+        <v>0.32512170685583297</v>
       </c>
       <c r="X10" s="18" t="s">
         <v>102</v>
       </c>
       <c r="Y10" t="str">
         <f>+CONCATENATE(T10,U10,V10,ROUND(W10*100,2),X10)</f>
-        <v>Gewinn: EUR 2800000 (gerundet ROI 38.21%)</v>
+        <v>Gewinn: EUR 2500000 (gerundet ROI 32.51%)</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
@@ -3111,56 +3261,56 @@
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="1">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1">
-        <v>8</v>
+      <c r="B3" s="1" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>8.0</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>68</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="1">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5</v>
+      <c r="B4" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>2.0</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="1">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
+      <c r="B5" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>5.0</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
+      <c r="B6" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2.0</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>68</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3168,7 +3318,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="F7" s="13" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3176,7 +3326,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="F8" s="13" t="s">
-        <v>68</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,43 +3390,37 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F3),"",Standort!F3)</f>
-        <v>
-</v>
+        <v>Bestlage im 17. Bezirk</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F4),"",Standort!F4)</f>
-        <v>
-</v>
+        <v>Absolute Ruhelage, mit Fernblick über Wien</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F5),"",Standort!F5)</f>
-        <v>
-</v>
+        <v>Zentrum Wien 18 Autominuten, öffentlich 25 Minuten</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F6),"",Standort!F6)</f>
-        <v>
-</v>
+        <v>Nahversorgung, Restaurants u. Geschäfte des täglichen Bedarfs in unmittelbarer Nähe</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F7),"",Standort!F7)</f>
-        <v>
-</v>
+        <v>Perfekte öffentliche Anbindung, 7 Gehminuten über Rebenweg</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f>+IF(ISBLANK(Standort!F8),"",Standort!F8)</f>
-        <v xml:space="preserve">
-</v>
+        <v xml:space="preserve">Gute Aussicht über Hernals mit ruhigem Verkehr</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -3316,7 +3460,7 @@
       </c>
       <c r="D11" s="1" t="n">
         <f>+Standort!B5</f>
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="E11" s="1" t="n">
         <f>+Standort!B6</f>
@@ -3333,11 +3477,11 @@
       </c>
       <c r="C12" s="1" t="n">
         <f>+Standort!C4</f>
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="D12" s="1" t="n">
         <f>+Standort!C5</f>
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="E12" s="1" t="n">
         <f>+Standort!C6</f>
@@ -3438,7 +3582,7 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="str" cm="1">
         <f t="array" ref="A3:A4">+Basisinformation!O2:O3</f>
-        <v>W II = Bauklasse 2</v>
+        <v>W I = Bauklasse 1 beschränkt auf 6,5 Meter</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
@@ -3449,7 +3593,7 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="str">
         <f>+IF(ISBLANK(Basisinformation!O4),"",Basisinformation!O4)</f>
-        <v xml:space="preserve"> </v>
+        <v xml:space="preserve">G = Gärtnerische Ausgestaltung</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -3536,24 +3680,24 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>2530800</v>
+      <c r="B3" s="1" t="n">
+        <v>2530000.0</v>
       </c>
       <c r="C3" s="3" t="n">
         <f>B3*B22</f>
-        <v>151848.0</v>
+        <v>25300.0</v>
       </c>
       <c r="D3" s="17" t="n">
         <f>+B22</f>
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="E3" s="3" t="n">
         <f t="shared" ref="E3:E11" si="0">B3+C3</f>
-        <v>2682648.0</v>
+        <v>2555300.0</v>
       </c>
       <c r="F3" s="2" t="n">
         <f t="shared" ref="F3:F11" si="1">$E3/$E$15</f>
-        <v>0.36095789908468334</v>
+        <v>0.32964208503978876</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -3561,24 +3705,24 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
-        <v>85892</v>
+      <c r="B4" s="1" t="n">
+        <v>85892.0</v>
       </c>
       <c r="C4" s="3" t="n">
         <f t="shared" ref="C4:C9" si="2">B4*$B$21</f>
-        <v>5153.5199999999995</v>
+        <v>17178.4</v>
       </c>
       <c r="D4" s="6" t="n">
         <f t="shared" ref="D4:D10" si="3">C4/B4</f>
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>91045.52</v>
+        <v>103070.4</v>
       </c>
       <c r="F4" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.012250433012557935</v>
+        <v>0.013296419818371636</v>
       </c>
       <c r="G4" s="1"/>
       <c r="I4" s="41" t="s">
@@ -3589,24 +3733,24 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
-        <v>2475206</v>
+      <c r="B5" s="1" t="n">
+        <v>2475206.0</v>
       </c>
       <c r="C5" s="3" t="n">
         <f>B5*$B$21</f>
-        <v>148512.36</v>
+        <v>495041.2</v>
       </c>
       <c r="D5" s="6" t="n">
         <f>C5/B5</f>
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>2623718.36</v>
+        <v>2970247.2</v>
       </c>
       <c r="F5" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.3530287488390243</v>
+        <v>0.3831716354602569</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -3614,24 +3758,24 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
-        <v>212558</v>
+      <c r="B6" s="1" t="n">
+        <v>212558.0</v>
       </c>
       <c r="C6" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>12753.48</v>
+        <v>42511.600000000006</v>
       </c>
       <c r="D6" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.06</v>
+        <v>0.20000000000000004</v>
       </c>
       <c r="E6" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>225311.48</v>
+        <v>255069.6</v>
       </c>
       <c r="F6" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.030316298843702436</v>
+        <v>0.03290481539320819</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -3639,24 +3783,24 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1">
-        <v>612366</v>
+      <c r="B7" s="1" t="n">
+        <v>612366.0</v>
       </c>
       <c r="C7" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>36741.96</v>
+        <v>122473.20000000001</v>
       </c>
       <c r="D7" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E7" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>649107.96</v>
+        <v>734839.2</v>
       </c>
       <c r="F7" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.08733931754026047</v>
+        <v>0.09479666812388773</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -3664,24 +3808,24 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1">
-        <v>39881</v>
+      <c r="B8" s="1" t="n">
+        <v>39881.0</v>
       </c>
       <c r="C8" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>2392.86</v>
+        <v>7976.200000000001</v>
       </c>
       <c r="D8" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.060000000000000005</v>
+        <v>0.2</v>
       </c>
       <c r="E8" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>42273.86</v>
+        <v>47857.2</v>
       </c>
       <c r="F8" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.005688067794134763</v>
+        <v>0.006173735840083816</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -3689,24 +3833,24 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1">
-        <v>101581</v>
+      <c r="B9" s="1" t="n">
+        <v>101581.0</v>
       </c>
       <c r="C9" s="3" t="n">
         <f t="shared" si="2"/>
-        <v>6094.86</v>
+        <v>20316.2</v>
       </c>
       <c r="D9" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>107675.86</v>
+        <v>121897.2</v>
       </c>
       <c r="F9" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.014488092439908812</v>
+        <v>0.015725138797210558</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -3714,24 +3858,24 @@
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1">
-        <v>52000</v>
+      <c r="B10" s="1" t="n">
+        <v>52000.0</v>
       </c>
       <c r="C10" s="3" t="n">
         <f>B10*$B$21</f>
-        <v>3120.0</v>
+        <v>10400.0</v>
       </c>
       <c r="D10" s="6" t="n">
         <f t="shared" si="3"/>
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>55120.0</v>
+        <v>62400.0</v>
       </c>
       <c r="F10" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.007416552375692878</v>
+        <v>0.008049804761273751</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -3739,23 +3883,23 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9">
-        <v>901060</v>
+      <c r="B11" s="9" t="n">
+        <v>901060.0</v>
       </c>
       <c r="C11" s="3" t="n">
         <f>+B11*D11</f>
-        <v>54063.6</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0.06</v>
+        <v>0.0</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>0.0</v>
       </c>
       <c r="E11" s="3" t="n">
         <f t="shared" si="0"/>
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="F11" s="2" t="n">
         <f t="shared" si="1"/>
-        <v>0.12851459007003507</v>
+        <v>0.11623969676591869</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -3774,23 +3918,23 @@
       </c>
       <c r="B13" s="3" t="n">
         <f>SUM(B3:B11)</f>
-        <v>7011344.0</v>
+        <v>7010544.0</v>
       </c>
       <c r="C13" s="3" t="n">
         <f>SUM(C3:C11)</f>
-        <v>420680.63999999996</v>
+        <v>741196.7999999998</v>
       </c>
       <c r="D13" s="4" t="n">
         <f>C13/B13</f>
-        <v>0.05999999999999999</v>
+        <v>0.10572600357404502</v>
       </c>
       <c r="E13" s="10" t="n">
         <f>B13+C13</f>
-        <v>7432024.64</v>
+        <v>7751740.8</v>
       </c>
       <c r="F13" s="4" t="n">
         <f>SUM(F3:F11)</f>
-        <v>1.0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -3811,23 +3955,23 @@
       </c>
       <c r="B15" s="3" t="n">
         <f>B13</f>
-        <v>7011344.0</v>
+        <v>7010544.0</v>
       </c>
       <c r="C15" s="3" t="n">
         <f>C13</f>
-        <v>420680.63999999996</v>
+        <v>741196.7999999998</v>
       </c>
       <c r="D15" s="3" t="n">
         <f>D13</f>
-        <v>0.05999999999999999</v>
+        <v>0.10572600357404502</v>
       </c>
       <c r="E15" s="10" t="n">
         <f>E13</f>
-        <v>7432024.64</v>
+        <v>7751740.8</v>
       </c>
       <c r="F15" s="4" t="n">
         <f>F13</f>
-        <v>1.0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -3862,16 +4006,16 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="11">
-        <v>0.06</v>
+      <c r="B21" s="11" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="12">
-        <v>0.06</v>
+      <c r="B22" s="12" t="n">
+        <v>0.01</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -3936,19 +4080,19 @@
       </c>
       <c r="B3" s="1" cm="1" t="n">
         <f t="array" ref="B3:F11">+GIK_Kalkulation!B3:F11</f>
-        <v>2530800.0</v>
+        <v>2530000.0</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>151848.0</v>
+        <v>25300.0</v>
       </c>
       <c r="D3" s="17" t="n">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>2682648.0</v>
+        <v>2555300.0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.36095789908468334</v>
+        <v>0.32964208503978876</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -3960,16 +4104,16 @@
         <v>85892.0</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>5153.5199999999995</v>
+        <v>17178.4</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>91045.52</v>
+        <v>103070.4</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.012250433012557935</v>
+        <v>0.013296419818371636</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -3981,16 +4125,16 @@
         <v>2475206.0</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>148512.36</v>
+        <v>495041.2</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>2623718.36</v>
+        <v>2970247.2</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.3530287488390243</v>
+        <v>0.3831716354602569</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -4002,16 +4146,16 @@
         <v>212558.0</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>12753.48</v>
+        <v>42511.600000000006</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>0.06</v>
+        <v>0.20000000000000004</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>225311.48</v>
+        <v>255069.6</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.030316298843702436</v>
+        <v>0.03290481539320819</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -4023,16 +4167,16 @@
         <v>612366.0</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>36741.96</v>
+        <v>122473.20000000001</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>649107.96</v>
+        <v>734839.2</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.08733931754026047</v>
+        <v>0.09479666812388773</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -4044,16 +4188,16 @@
         <v>39881.0</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>2392.86</v>
+        <v>7976.200000000001</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>0.060000000000000005</v>
+        <v>0.2</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>42273.86</v>
+        <v>47857.2</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.005688067794134763</v>
+        <v>0.006173735840083816</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -4065,16 +4209,16 @@
         <v>101581.0</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>6094.86</v>
+        <v>20316.2</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>107675.86</v>
+        <v>121897.2</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.014488092439908812</v>
+        <v>0.015725138797210558</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -4086,16 +4230,16 @@
         <v>52000.0</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>3120.0</v>
+        <v>10400.0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>55120.0</v>
+        <v>62400.0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.007416552375692878</v>
+        <v>0.008049804761273751</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -4107,16 +4251,16 @@
         <v>901060.0</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>54063.6</v>
+        <v>0.0</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>0.06</v>
+        <v>0.0</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.12851459007003507</v>
+        <v>0.11623969676591869</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -4135,19 +4279,19 @@
       </c>
       <c r="B13" s="3" cm="1" t="n">
         <f t="array" ref="B13:F13">+GIK_Kalkulation!B13:F13</f>
-        <v>7011344.0</v>
+        <v>7010544.0</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>420680.63999999996</v>
+        <v>741196.7999999998</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>0.05999999999999999</v>
+        <v>0.10572600357404502</v>
       </c>
       <c r="E13" s="10" t="n">
-        <v>7432024.64</v>
+        <v>7751740.8</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>1.0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -4168,19 +4312,19 @@
       </c>
       <c r="B15" s="3" cm="1" t="n">
         <f t="array" ref="B15:F15">+GIK_Kalkulation!B15:F15</f>
-        <v>7011344.0</v>
+        <v>7010544.0</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>420680.63999999996</v>
+        <v>741196.7999999998</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>0.05999999999999999</v>
+        <v>0.10572600357404502</v>
       </c>
       <c r="E15" s="10" t="n">
-        <v>7432024.64</v>
+        <v>7751740.8</v>
       </c>
       <c r="F15" s="4" t="n">
-        <v>1.0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -4217,7 +4361,7 @@
       </c>
       <c r="B21" s="11" cm="1" t="n">
         <f t="array" ref="B21:B22">+GIK_Kalkulation!B21:B22</f>
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -4225,7 +4369,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="n">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
@@ -4366,22 +4510,22 @@
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1">
-        <v>6851180</v>
+      <c r="B3" s="1" t="n">
+        <v>6851180.0</v>
       </c>
       <c r="C3" s="2" t="n">
         <f>$B3/$B8</f>
-        <v>0.877647136347605</v>
+        <v>0.8837677884069637</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="1">
-        <v>900000</v>
+      <c r="E3" s="1" t="n">
+        <v>900000.0</v>
       </c>
       <c r="F3" s="2" t="n">
         <f>$E3/$E8</f>
-        <v>0.1160954918959542</v>
+        <v>0.1547657534340801</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>25</v>
@@ -4391,7 +4535,7 @@
       </c>
       <c r="K3" s="2" t="n">
         <f>$J3/$J7</f>
-        <v>1.2876256246292843E-4</v>
+        <v>1.3648726174373017E-4</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>26</v>
@@ -4406,22 +4550,22 @@
       <c r="Q3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="1">
-        <v>2</v>
+      <c r="R3" s="1" t="n">
+        <v>456123.0</v>
       </c>
       <c r="S3" s="2" t="n">
         <f>$R3/$R9</f>
-        <v>2.0939654428695034E-6</v>
+        <v>0.33608069066588664</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="1">
-        <v>1</v>
+      <c r="U3" s="1" t="n">
+        <v>456123.0</v>
       </c>
       <c r="V3" s="2" t="n">
         <f>$U3/$U9</f>
-        <v>0.012345679012345678</v>
+        <v>1.7143948655649988E-5</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>25</v>
@@ -4431,7 +4575,7 @@
       </c>
       <c r="AA3" s="2" t="n">
         <f>$Z3/$Z10</f>
-        <v>1.0469739521256502E-5</v>
+        <v>1.109791692099393E-5</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>26</v>
@@ -4451,7 +4595,7 @@
       </c>
       <c r="AI3" s="2" t="n">
         <f>$AH3/$AH11</f>
-        <v>0.8270677181809748</v>
+        <v>0.8352436001611981</v>
       </c>
       <c r="AJ3" s="1" t="s">
         <v>26</v>
@@ -4470,32 +4614,32 @@
       </c>
       <c r="B4" s="16" t="n">
         <f>+Gesamtinvestitionskosten!E11</f>
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="C4" s="2" t="n">
         <f>$B4/$B8</f>
-        <v>0.12235286365239498</v>
+        <v>0.11623221159303633</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2450000</v>
+        <v>179</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>2450000.0</v>
       </c>
       <c r="F4" s="2" t="n">
         <f>$E4/$E8</f>
-        <v>0.3160377279389864</v>
+        <v>0.42130677323721805</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J4" s="16" t="n">
         <f>+Gesamtinvestitionskosten!E11</f>
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="K4" s="2" t="n">
         <f>$J4/$J7</f>
-        <v>0.999871237437537</v>
+        <v>0.9998635127382562</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>58</v>
@@ -4512,32 +4656,32 @@
       </c>
       <c r="R4" s="16" t="n">
         <f>+Gesamtinvestitionskosten!E11</f>
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="S4" s="2" t="n">
         <f>$R4/$R9</f>
-        <v>0.9999979060345572</v>
+        <v>0.6639193093341134</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="U4" s="1">
-        <v>10</v>
+        <v>153</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>2.4896321456E10</v>
       </c>
       <c r="V4" s="2" t="n">
         <f>$U4/$U9</f>
-        <v>0.12345679012345678</v>
+        <v>0.9357591192643677</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="Z4" s="16" t="n">
         <f>+Gesamtinvestitionskosten!E11</f>
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="AA4" s="2" t="n">
         <f>$Z4/$Z10</f>
-        <v>0.9999895302604788</v>
+        <v>0.999988902083079</v>
       </c>
       <c r="AB4" s="13" t="s">
         <v>58</v>
@@ -4554,11 +4698,11 @@
       </c>
       <c r="AH4" s="16" t="n">
         <f>+Gesamtinvestitionskosten!E11</f>
-        <v>955123.6</v>
+        <v>901060.0</v>
       </c>
       <c r="AI4" s="2" t="n">
         <f>$AH4/$AH11</f>
-        <v>0.17293228181902523</v>
+        <v>0.1647563998388018</v>
       </c>
       <c r="AJ4" s="13" t="s">
         <v>112</v>
@@ -4576,14 +4720,14 @@
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2250000</v>
+        <v>180</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>2250000.0</v>
       </c>
       <c r="F5" s="2" t="n">
         <f>$E5/$E8</f>
-        <v>0.29023872973988546</v>
+        <v>0.38691438358520025</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -4602,14 +4746,14 @@
       <c r="R5" s="1"/>
       <c r="S5" s="3"/>
       <c r="T5" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="U5" s="1">
-        <v>23</v>
+        <v>154</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>1.45641235E8</v>
       </c>
       <c r="V5" s="2" t="n">
         <f>$U5/$U9</f>
-        <v>0.2839506172839506</v>
+        <v>0.005474106447132581</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -4645,12 +4789,12 @@
       <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1">
-        <v>2152239</v>
+      <c r="E6" s="1" t="n">
+        <v>215240.0</v>
       </c>
       <c r="F6" s="2" t="n">
         <f>$E6/$E8</f>
-        <v>0.27762805042517397</v>
+        <v>0.03701308974350156</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -4662,14 +4806,14 @@
       <c r="R6" s="1"/>
       <c r="S6" s="3"/>
       <c r="T6" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="U6" s="1">
-        <v>45</v>
+        <v>155</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>16541.0</v>
       </c>
       <c r="V6" s="2" t="n">
         <f>$U6/$U9</f>
-        <v>0.5555555555555556</v>
+        <v>6.217139997612628E-7</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
@@ -4710,7 +4854,7 @@
       </c>
       <c r="J7" s="3" t="n">
         <f>SUM(J3:J6)</f>
-        <v>955246.6</v>
+        <v>901183.0</v>
       </c>
       <c r="K7" s="4" t="n">
         <f>SUM(K3:K6)</f>
@@ -4731,12 +4875,12 @@
       <c r="T7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="1">
-        <v>2</v>
+      <c r="U7" s="1" t="n">
+        <v>1.563045632E9</v>
       </c>
       <c r="V7" s="2" t="n">
         <f>$U7/$U9</f>
-        <v>0.024691358024691357</v>
+        <v>0.05874900862584432</v>
       </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
@@ -4771,7 +4915,7 @@
       </c>
       <c r="B8" s="3" t="n">
         <f>SUM(B3:B7)</f>
-        <v>7806303.6</v>
+        <v>7752240.0</v>
       </c>
       <c r="C8" s="4" t="n">
         <f>SUM(C3:C7)</f>
@@ -4780,7 +4924,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="10" t="n">
         <f>SUM(E3:E7)</f>
-        <v>7752239.0</v>
+        <v>5815240.0</v>
       </c>
       <c r="F8" s="4" t="n">
         <f>SUM(F3:F7)</f>
@@ -4825,7 +4969,7 @@
       </c>
       <c r="R9" s="3" t="n">
         <f>SUM(R3:R8)</f>
-        <v>955125.6</v>
+        <v>1357183.0</v>
       </c>
       <c r="S9" s="4" t="n">
         <f>SUM(S3:S8)</f>
@@ -4834,11 +4978,11 @@
       <c r="T9" s="3"/>
       <c r="U9" s="10" t="n">
         <f>SUM(U3:U8)</f>
-        <v>81.0</v>
+        <v>2.6605480987E10</v>
       </c>
       <c r="V9" s="4" t="n">
         <f>SUM(V3:V8)</f>
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -4866,7 +5010,7 @@
       </c>
       <c r="Z10" s="3" t="n">
         <f>SUM(Z3:Z9)</f>
-        <v>955133.6</v>
+        <v>901070.0</v>
       </c>
       <c r="AA10" s="4" t="n">
         <f>SUM(AA3:AA9)</f>
@@ -4894,7 +5038,7 @@
       </c>
       <c r="AH11" s="3" t="n">
         <f>SUM(AH3:AH10)</f>
-        <v>5523107.6</v>
+        <v>5469044.0</v>
       </c>
       <c r="AI11" s="4" t="n">
         <f>SUM(AI3:AI10)</f>
@@ -4914,8 +5058,8 @@
       <c r="G12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="1">
-        <v>2</v>
+      <c r="H12" s="1" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -5022,8 +5166,8 @@
         <f>+F4/1.1</f>
         <v>9090.90909090909</v>
       </c>
-      <c r="F4" s="33">
-        <v>10000</v>
+      <c r="F4" s="33" t="n">
+        <v>10000.0</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="34" t="n">
@@ -5036,8 +5180,8 @@
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="37">
-        <v>1</v>
+      <c r="B5" s="37" t="n">
+        <v>1.0</v>
       </c>
       <c r="C5" s="3" t="n">
         <f>+B5*C7</f>
@@ -5148,8 +5292,8 @@
         <f>+F10/1.1</f>
         <v>38181.81818181818</v>
       </c>
-      <c r="F10" s="16">
-        <v>42000</v>
+      <c r="F10" s="16" t="n">
+        <v>42000.0</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="39" t="n">
@@ -5166,8 +5310,8 @@
         <f>+C11/C13</f>
         <v>1.0</v>
       </c>
-      <c r="C11" s="16">
-        <v>16</v>
+      <c r="C11" s="16" t="n">
+        <v>16.0</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -5187,8 +5331,8 @@
         <f>+C12/C13</f>
         <v>0.0</v>
       </c>
-      <c r="C12" s="16">
-        <v>0</v>
+      <c r="C12" s="16" t="n">
+        <v>0.0</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="40">
@@ -5357,7 +5501,7 @@
       </c>
       <c r="E21" s="9" t="n">
         <f>+Gesamtinvestitionskosten!E15</f>
-        <v>7432024.64</v>
+        <v>7751740.8</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -5373,7 +5517,7 @@
       </c>
       <c r="E22" s="3" t="n">
         <f>E20-E21</f>
-        <v>2839975.3600000003</v>
+        <v>2520259.2</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -5389,7 +5533,7 @@
       </c>
       <c r="E23" s="2" t="n">
         <f>E22/E21</f>
-        <v>0.3821267417111255</v>
+        <v>0.32512170685583297</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>

</xml_diff>